<commit_message>
flangesegments.PolynomialLFlangeSemenge: tmplemented flange tilt
</commit_message>
<xml_diff>
--- a/tests/validation/BnB_ReferenceFlange-Results-ShapeFactor-1.2.xlsx
+++ b/tests/validation/BnB_ReferenceFlange-Results-ShapeFactor-1.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelloB\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\tests\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC4E49B-181F-47B3-B68F-59C0341B1121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CEBE36-FF1C-4E65-B0A4-5DD4F2343FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Gap30deg" sheetId="2" r:id="rId1"/>
@@ -4580,7 +4580,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5043,14 +5043,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="171" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5079,40 +5076,17 @@
     <xf numFmtId="0" fontId="22" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="9" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -19244,7 +19218,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -19658,32 +19632,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="166" t="s">
+      <c r="A3" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="167"/>
-      <c r="C3" s="167"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="167"/>
-      <c r="F3" s="167"/>
-      <c r="G3" s="167"/>
-      <c r="H3" s="167"/>
-      <c r="I3" s="167"/>
-      <c r="J3" s="167"/>
-      <c r="K3" s="167"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="168" t="s">
+      <c r="B4" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="168"/>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
-      <c r="F4" s="168"/>
-      <c r="G4" s="168"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -19699,12 +19673,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="169"/>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="171"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="170"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -19712,12 +19686,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="169"/>
-      <c r="C6" s="170"/>
-      <c r="D6" s="170"/>
-      <c r="E6" s="170"/>
-      <c r="F6" s="170"/>
-      <c r="G6" s="171"/>
+      <c r="B6" s="168"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="169"/>
+      <c r="F6" s="169"/>
+      <c r="G6" s="170"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -19725,12 +19699,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="169"/>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="171"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="169"/>
+      <c r="G7" s="170"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -19738,12 +19712,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="169"/>
-      <c r="C8" s="170"/>
-      <c r="D8" s="170"/>
-      <c r="E8" s="170"/>
-      <c r="F8" s="170"/>
-      <c r="G8" s="171"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="169"/>
+      <c r="D8" s="169"/>
+      <c r="E8" s="169"/>
+      <c r="F8" s="169"/>
+      <c r="G8" s="170"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -19751,12 +19725,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="169"/>
-      <c r="C9" s="170"/>
-      <c r="D9" s="170"/>
-      <c r="E9" s="170"/>
-      <c r="F9" s="170"/>
-      <c r="G9" s="171"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="169"/>
+      <c r="D9" s="169"/>
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="170"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -19804,102 +19778,102 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="162" t="s">
+      <c r="B13" s="171" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="162"/>
-      <c r="D13" s="161" t="s">
+      <c r="C13" s="171"/>
+      <c r="D13" s="173" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="161"/>
-      <c r="F13" s="161"/>
-      <c r="G13" s="161"/>
-      <c r="H13" s="161"/>
-      <c r="I13" s="161"/>
-      <c r="J13" s="161"/>
-      <c r="K13" s="161"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="173"/>
+      <c r="G13" s="173"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
+      <c r="K13" s="173"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="162" t="s">
+      <c r="B14" s="171" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="162"/>
-      <c r="D14" s="161" t="s">
+      <c r="C14" s="171"/>
+      <c r="D14" s="173" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="161"/>
-      <c r="F14" s="161"/>
-      <c r="G14" s="161"/>
-      <c r="H14" s="161"/>
-      <c r="I14" s="161"/>
-      <c r="J14" s="161"/>
-      <c r="K14" s="161"/>
+      <c r="E14" s="173"/>
+      <c r="F14" s="173"/>
+      <c r="G14" s="173"/>
+      <c r="H14" s="173"/>
+      <c r="I14" s="173"/>
+      <c r="J14" s="173"/>
+      <c r="K14" s="173"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="162" t="s">
+      <c r="B15" s="171" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="162"/>
-      <c r="D15" s="161" t="s">
+      <c r="C15" s="171"/>
+      <c r="D15" s="173" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="161"/>
-      <c r="F15" s="161"/>
-      <c r="G15" s="161"/>
-      <c r="H15" s="161"/>
-      <c r="I15" s="161"/>
-      <c r="J15" s="161"/>
-      <c r="K15" s="161"/>
+      <c r="E15" s="173"/>
+      <c r="F15" s="173"/>
+      <c r="G15" s="173"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="173"/>
+      <c r="J15" s="173"/>
+      <c r="K15" s="173"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="162" t="s">
+      <c r="B16" s="171" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="162"/>
-      <c r="D16" s="161" t="str">
+      <c r="C16" s="171"/>
+      <c r="D16" s="173" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 30° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="161"/>
-      <c r="F16" s="161"/>
-      <c r="G16" s="161"/>
-      <c r="H16" s="161"/>
-      <c r="I16" s="161"/>
-      <c r="J16" s="161"/>
-      <c r="K16" s="161"/>
+      <c r="E16" s="173"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="173"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="173"/>
+      <c r="J16" s="173"/>
+      <c r="K16" s="173"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="162" t="s">
+      <c r="B17" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="162"/>
-      <c r="D17" s="160">
+      <c r="C17" s="171"/>
+      <c r="D17" s="174">
         <v>0.1</v>
       </c>
-      <c r="E17" s="161"/>
-      <c r="F17" s="161"/>
-      <c r="G17" s="161"/>
-      <c r="H17" s="161"/>
-      <c r="I17" s="161"/>
-      <c r="J17" s="161"/>
-      <c r="K17" s="161"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="173"/>
+      <c r="J17" s="173"/>
+      <c r="K17" s="173"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="162" t="s">
+      <c r="B18" s="171" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="162"/>
+      <c r="C18" s="171"/>
       <c r="D18" s="172">
         <v>45432</v>
       </c>
@@ -20097,16 +20071,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="163"/>
-      <c r="C28" s="164"/>
-      <c r="D28" s="164"/>
-      <c r="E28" s="164"/>
-      <c r="F28" s="164"/>
-      <c r="G28" s="164"/>
-      <c r="H28" s="164"/>
-      <c r="I28" s="164"/>
-      <c r="J28" s="164"/>
-      <c r="K28" s="165"/>
+      <c r="B28" s="162"/>
+      <c r="C28" s="163"/>
+      <c r="D28" s="163"/>
+      <c r="E28" s="163"/>
+      <c r="F28" s="163"/>
+      <c r="G28" s="163"/>
+      <c r="H28" s="163"/>
+      <c r="I28" s="163"/>
+      <c r="J28" s="163"/>
+      <c r="K28" s="164"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -24021,6 +23995,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B18:C18"/>
@@ -24031,16 +24015,6 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B28:K28"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="26" priority="5" stopIfTrue="1" operator="between">
@@ -24126,32 +24100,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="166" t="s">
+      <c r="A3" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="167"/>
-      <c r="C3" s="167"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="167"/>
-      <c r="F3" s="167"/>
-      <c r="G3" s="167"/>
-      <c r="H3" s="167"/>
-      <c r="I3" s="167"/>
-      <c r="J3" s="167"/>
-      <c r="K3" s="167"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="168" t="s">
+      <c r="B4" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="168"/>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
-      <c r="F4" s="168"/>
-      <c r="G4" s="168"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -24167,12 +24141,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="169"/>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="171"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="170"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -24180,12 +24154,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="169"/>
-      <c r="C6" s="170"/>
-      <c r="D6" s="170"/>
-      <c r="E6" s="170"/>
-      <c r="F6" s="170"/>
-      <c r="G6" s="171"/>
+      <c r="B6" s="168"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="169"/>
+      <c r="F6" s="169"/>
+      <c r="G6" s="170"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -24193,12 +24167,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="169"/>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="171"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="169"/>
+      <c r="G7" s="170"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -24206,12 +24180,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="169"/>
-      <c r="C8" s="170"/>
-      <c r="D8" s="170"/>
-      <c r="E8" s="170"/>
-      <c r="F8" s="170"/>
-      <c r="G8" s="171"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="169"/>
+      <c r="D8" s="169"/>
+      <c r="E8" s="169"/>
+      <c r="F8" s="169"/>
+      <c r="G8" s="170"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -24219,12 +24193,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="169"/>
-      <c r="C9" s="170"/>
-      <c r="D9" s="170"/>
-      <c r="E9" s="170"/>
-      <c r="F9" s="170"/>
-      <c r="G9" s="171"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="169"/>
+      <c r="D9" s="169"/>
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="170"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -24272,106 +24246,106 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="162" t="s">
+      <c r="B13" s="171" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="162"/>
-      <c r="D13" s="161" t="str">
+      <c r="C13" s="171"/>
+      <c r="D13" s="173" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="161"/>
-      <c r="F13" s="161"/>
-      <c r="G13" s="161"/>
-      <c r="H13" s="161"/>
-      <c r="I13" s="161"/>
-      <c r="J13" s="161"/>
-      <c r="K13" s="161"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="173"/>
+      <c r="G13" s="173"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
+      <c r="K13" s="173"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="162" t="s">
+      <c r="B14" s="171" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="162"/>
-      <c r="D14" s="161" t="str">
+      <c r="C14" s="171"/>
+      <c r="D14" s="173" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="161"/>
-      <c r="F14" s="161"/>
-      <c r="G14" s="161"/>
-      <c r="H14" s="161"/>
-      <c r="I14" s="161"/>
-      <c r="J14" s="161"/>
-      <c r="K14" s="161"/>
+      <c r="E14" s="173"/>
+      <c r="F14" s="173"/>
+      <c r="G14" s="173"/>
+      <c r="H14" s="173"/>
+      <c r="I14" s="173"/>
+      <c r="J14" s="173"/>
+      <c r="K14" s="173"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="162" t="s">
+      <c r="B15" s="171" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="162"/>
-      <c r="D15" s="161" t="str">
+      <c r="C15" s="171"/>
+      <c r="D15" s="173" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="161"/>
-      <c r="F15" s="161"/>
-      <c r="G15" s="161"/>
-      <c r="H15" s="161"/>
-      <c r="I15" s="161"/>
-      <c r="J15" s="161"/>
-      <c r="K15" s="161"/>
+      <c r="E15" s="173"/>
+      <c r="F15" s="173"/>
+      <c r="G15" s="173"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="173"/>
+      <c r="J15" s="173"/>
+      <c r="K15" s="173"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="162" t="s">
+      <c r="B16" s="171" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="162"/>
-      <c r="D16" s="161" t="str">
+      <c r="C16" s="171"/>
+      <c r="D16" s="173" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 60° gap size ans shape factor 1.2</v>
       </c>
-      <c r="E16" s="161"/>
-      <c r="F16" s="161"/>
-      <c r="G16" s="161"/>
-      <c r="H16" s="161"/>
-      <c r="I16" s="161"/>
-      <c r="J16" s="161"/>
-      <c r="K16" s="161"/>
+      <c r="E16" s="173"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="173"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="173"/>
+      <c r="J16" s="173"/>
+      <c r="K16" s="173"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="162" t="s">
+      <c r="B17" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="162"/>
-      <c r="D17" s="161">
+      <c r="C17" s="171"/>
+      <c r="D17" s="173">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="161"/>
-      <c r="F17" s="161"/>
-      <c r="G17" s="161"/>
-      <c r="H17" s="161"/>
-      <c r="I17" s="161"/>
-      <c r="J17" s="161"/>
-      <c r="K17" s="161"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="173"/>
+      <c r="J17" s="173"/>
+      <c r="K17" s="173"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="162" t="s">
+      <c r="B18" s="171" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="162"/>
+      <c r="C18" s="171"/>
       <c r="D18" s="172">
         <f>Gap30deg!D18</f>
         <v>45432</v>
@@ -24570,16 +24544,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="163"/>
-      <c r="C28" s="164"/>
-      <c r="D28" s="164"/>
-      <c r="E28" s="164"/>
-      <c r="F28" s="164"/>
-      <c r="G28" s="164"/>
-      <c r="H28" s="164"/>
-      <c r="I28" s="164"/>
-      <c r="J28" s="164"/>
-      <c r="K28" s="165"/>
+      <c r="B28" s="162"/>
+      <c r="C28" s="163"/>
+      <c r="D28" s="163"/>
+      <c r="E28" s="163"/>
+      <c r="F28" s="163"/>
+      <c r="G28" s="163"/>
+      <c r="H28" s="163"/>
+      <c r="I28" s="163"/>
+      <c r="J28" s="163"/>
+      <c r="K28" s="164"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -28561,32 +28535,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="166" t="s">
+      <c r="A3" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="167"/>
-      <c r="C3" s="167"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="167"/>
-      <c r="F3" s="167"/>
-      <c r="G3" s="167"/>
-      <c r="H3" s="167"/>
-      <c r="I3" s="167"/>
-      <c r="J3" s="167"/>
-      <c r="K3" s="167"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="168" t="s">
+      <c r="B4" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="168"/>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
-      <c r="F4" s="168"/>
-      <c r="G4" s="168"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -28602,12 +28576,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="169"/>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="171"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="170"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -28615,12 +28589,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="169"/>
-      <c r="C6" s="170"/>
-      <c r="D6" s="170"/>
-      <c r="E6" s="170"/>
-      <c r="F6" s="170"/>
-      <c r="G6" s="171"/>
+      <c r="B6" s="168"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="169"/>
+      <c r="F6" s="169"/>
+      <c r="G6" s="170"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -28628,12 +28602,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="169"/>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="171"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="169"/>
+      <c r="G7" s="170"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -28641,12 +28615,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="169"/>
-      <c r="C8" s="170"/>
-      <c r="D8" s="170"/>
-      <c r="E8" s="170"/>
-      <c r="F8" s="170"/>
-      <c r="G8" s="171"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="169"/>
+      <c r="D8" s="169"/>
+      <c r="E8" s="169"/>
+      <c r="F8" s="169"/>
+      <c r="G8" s="170"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -28654,12 +28628,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="169"/>
-      <c r="C9" s="170"/>
-      <c r="D9" s="170"/>
-      <c r="E9" s="170"/>
-      <c r="F9" s="170"/>
-      <c r="G9" s="171"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="169"/>
+      <c r="D9" s="169"/>
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="170"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -28707,106 +28681,106 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="162" t="s">
+      <c r="B13" s="171" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="162"/>
-      <c r="D13" s="161" t="str">
+      <c r="C13" s="171"/>
+      <c r="D13" s="173" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="161"/>
-      <c r="F13" s="161"/>
-      <c r="G13" s="161"/>
-      <c r="H13" s="161"/>
-      <c r="I13" s="161"/>
-      <c r="J13" s="161"/>
-      <c r="K13" s="161"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="173"/>
+      <c r="G13" s="173"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
+      <c r="K13" s="173"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="162" t="s">
+      <c r="B14" s="171" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="162"/>
-      <c r="D14" s="161" t="str">
+      <c r="C14" s="171"/>
+      <c r="D14" s="173" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="161"/>
-      <c r="F14" s="161"/>
-      <c r="G14" s="161"/>
-      <c r="H14" s="161"/>
-      <c r="I14" s="161"/>
-      <c r="J14" s="161"/>
-      <c r="K14" s="161"/>
+      <c r="E14" s="173"/>
+      <c r="F14" s="173"/>
+      <c r="G14" s="173"/>
+      <c r="H14" s="173"/>
+      <c r="I14" s="173"/>
+      <c r="J14" s="173"/>
+      <c r="K14" s="173"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="162" t="s">
+      <c r="B15" s="171" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="162"/>
-      <c r="D15" s="161" t="str">
+      <c r="C15" s="171"/>
+      <c r="D15" s="173" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="161"/>
-      <c r="F15" s="161"/>
-      <c r="G15" s="161"/>
-      <c r="H15" s="161"/>
-      <c r="I15" s="161"/>
-      <c r="J15" s="161"/>
-      <c r="K15" s="161"/>
+      <c r="E15" s="173"/>
+      <c r="F15" s="173"/>
+      <c r="G15" s="173"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="173"/>
+      <c r="J15" s="173"/>
+      <c r="K15" s="173"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="162" t="s">
+      <c r="B16" s="171" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="162"/>
-      <c r="D16" s="161" t="str">
+      <c r="C16" s="171"/>
+      <c r="D16" s="173" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 90° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="161"/>
-      <c r="F16" s="161"/>
-      <c r="G16" s="161"/>
-      <c r="H16" s="161"/>
-      <c r="I16" s="161"/>
-      <c r="J16" s="161"/>
-      <c r="K16" s="161"/>
+      <c r="E16" s="173"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="173"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="173"/>
+      <c r="J16" s="173"/>
+      <c r="K16" s="173"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="162" t="s">
+      <c r="B17" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="162"/>
-      <c r="D17" s="161">
+      <c r="C17" s="171"/>
+      <c r="D17" s="173">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="161"/>
-      <c r="F17" s="161"/>
-      <c r="G17" s="161"/>
-      <c r="H17" s="161"/>
-      <c r="I17" s="161"/>
-      <c r="J17" s="161"/>
-      <c r="K17" s="161"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="173"/>
+      <c r="J17" s="173"/>
+      <c r="K17" s="173"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="162" t="s">
+      <c r="B18" s="171" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="162"/>
+      <c r="C18" s="171"/>
       <c r="D18" s="172">
         <f>Gap30deg!D18</f>
         <v>45432</v>
@@ -29005,16 +28979,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="163"/>
-      <c r="C28" s="164"/>
-      <c r="D28" s="164"/>
-      <c r="E28" s="164"/>
-      <c r="F28" s="164"/>
-      <c r="G28" s="164"/>
-      <c r="H28" s="164"/>
-      <c r="I28" s="164"/>
-      <c r="J28" s="164"/>
-      <c r="K28" s="165"/>
+      <c r="B28" s="162"/>
+      <c r="C28" s="163"/>
+      <c r="D28" s="163"/>
+      <c r="E28" s="163"/>
+      <c r="F28" s="163"/>
+      <c r="G28" s="163"/>
+      <c r="H28" s="163"/>
+      <c r="I28" s="163"/>
+      <c r="J28" s="163"/>
+      <c r="K28" s="164"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -32997,32 +32971,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="166" t="s">
+      <c r="A3" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="167"/>
-      <c r="C3" s="167"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="167"/>
-      <c r="F3" s="167"/>
-      <c r="G3" s="167"/>
-      <c r="H3" s="167"/>
-      <c r="I3" s="167"/>
-      <c r="J3" s="167"/>
-      <c r="K3" s="167"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="168" t="s">
+      <c r="B4" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="168"/>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
-      <c r="F4" s="168"/>
-      <c r="G4" s="168"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -33038,12 +33012,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="169"/>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="171"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="170"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -33051,12 +33025,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="169"/>
-      <c r="C6" s="170"/>
-      <c r="D6" s="170"/>
-      <c r="E6" s="170"/>
-      <c r="F6" s="170"/>
-      <c r="G6" s="171"/>
+      <c r="B6" s="168"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="169"/>
+      <c r="F6" s="169"/>
+      <c r="G6" s="170"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -33064,12 +33038,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="169"/>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="171"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="169"/>
+      <c r="G7" s="170"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -33077,12 +33051,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="169"/>
-      <c r="C8" s="170"/>
-      <c r="D8" s="170"/>
-      <c r="E8" s="170"/>
-      <c r="F8" s="170"/>
-      <c r="G8" s="171"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="169"/>
+      <c r="D8" s="169"/>
+      <c r="E8" s="169"/>
+      <c r="F8" s="169"/>
+      <c r="G8" s="170"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -33090,12 +33064,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="169"/>
-      <c r="C9" s="170"/>
-      <c r="D9" s="170"/>
-      <c r="E9" s="170"/>
-      <c r="F9" s="170"/>
-      <c r="G9" s="171"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="169"/>
+      <c r="D9" s="169"/>
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="170"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -33143,106 +33117,106 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="162" t="s">
+      <c r="B13" s="171" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="162"/>
-      <c r="D13" s="161" t="str">
+      <c r="C13" s="171"/>
+      <c r="D13" s="173" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="161"/>
-      <c r="F13" s="161"/>
-      <c r="G13" s="161"/>
-      <c r="H13" s="161"/>
-      <c r="I13" s="161"/>
-      <c r="J13" s="161"/>
-      <c r="K13" s="161"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="173"/>
+      <c r="G13" s="173"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
+      <c r="K13" s="173"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="162" t="s">
+      <c r="B14" s="171" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="162"/>
-      <c r="D14" s="161" t="str">
+      <c r="C14" s="171"/>
+      <c r="D14" s="173" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="161"/>
-      <c r="F14" s="161"/>
-      <c r="G14" s="161"/>
-      <c r="H14" s="161"/>
-      <c r="I14" s="161"/>
-      <c r="J14" s="161"/>
-      <c r="K14" s="161"/>
+      <c r="E14" s="173"/>
+      <c r="F14" s="173"/>
+      <c r="G14" s="173"/>
+      <c r="H14" s="173"/>
+      <c r="I14" s="173"/>
+      <c r="J14" s="173"/>
+      <c r="K14" s="173"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="162" t="s">
+      <c r="B15" s="171" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="162"/>
-      <c r="D15" s="161" t="str">
+      <c r="C15" s="171"/>
+      <c r="D15" s="173" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="161"/>
-      <c r="F15" s="161"/>
-      <c r="G15" s="161"/>
-      <c r="H15" s="161"/>
-      <c r="I15" s="161"/>
-      <c r="J15" s="161"/>
-      <c r="K15" s="161"/>
+      <c r="E15" s="173"/>
+      <c r="F15" s="173"/>
+      <c r="G15" s="173"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="173"/>
+      <c r="J15" s="173"/>
+      <c r="K15" s="173"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="162" t="s">
+      <c r="B16" s="171" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="162"/>
-      <c r="D16" s="161" t="str">
+      <c r="C16" s="171"/>
+      <c r="D16" s="173" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 120° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="161"/>
-      <c r="F16" s="161"/>
-      <c r="G16" s="161"/>
-      <c r="H16" s="161"/>
-      <c r="I16" s="161"/>
-      <c r="J16" s="161"/>
-      <c r="K16" s="161"/>
+      <c r="E16" s="173"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="173"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="173"/>
+      <c r="J16" s="173"/>
+      <c r="K16" s="173"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="162" t="s">
+      <c r="B17" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="162"/>
-      <c r="D17" s="161">
+      <c r="C17" s="171"/>
+      <c r="D17" s="173">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="161"/>
-      <c r="F17" s="161"/>
-      <c r="G17" s="161"/>
-      <c r="H17" s="161"/>
-      <c r="I17" s="161"/>
-      <c r="J17" s="161"/>
-      <c r="K17" s="161"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="173"/>
+      <c r="J17" s="173"/>
+      <c r="K17" s="173"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="162" t="s">
+      <c r="B18" s="171" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="162"/>
+      <c r="C18" s="171"/>
       <c r="D18" s="172">
         <f>Gap30deg!D18</f>
         <v>45432</v>
@@ -33441,16 +33415,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="163"/>
-      <c r="C28" s="164"/>
-      <c r="D28" s="164"/>
-      <c r="E28" s="164"/>
-      <c r="F28" s="164"/>
-      <c r="G28" s="164"/>
-      <c r="H28" s="164"/>
-      <c r="I28" s="164"/>
-      <c r="J28" s="164"/>
-      <c r="K28" s="165"/>
+      <c r="B28" s="162"/>
+      <c r="C28" s="163"/>
+      <c r="D28" s="163"/>
+      <c r="E28" s="163"/>
+      <c r="F28" s="163"/>
+      <c r="G28" s="163"/>
+      <c r="H28" s="163"/>
+      <c r="I28" s="163"/>
+      <c r="J28" s="163"/>
+      <c r="K28" s="164"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -37505,10 +37479,10 @@
       <c r="L27" s="103" t="s">
         <v>197</v>
       </c>
-      <c r="N27" s="173"/>
-      <c r="O27" s="173"/>
-      <c r="P27" s="173"/>
-      <c r="Q27" s="173"/>
+      <c r="N27" s="104"/>
+      <c r="O27" s="104"/>
+      <c r="P27" s="104"/>
+      <c r="Q27" s="104"/>
       <c r="R27" t="str">
         <f t="shared" ref="R27:R66" si="0">IF(H27&lt;&gt;"",H27,"")</f>
         <v>Simplified formula used, therefore not evaluated</v>
@@ -37547,16 +37521,16 @@
       <c r="M28" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N28" s="174">
+      <c r="N28" s="107">
         <v>153.74071147146736</v>
       </c>
-      <c r="O28" s="174">
+      <c r="O28" s="107">
         <v>153.74071147146736</v>
       </c>
-      <c r="P28" s="174">
+      <c r="P28" s="107">
         <v>153.74071147146736</v>
       </c>
-      <c r="Q28" s="174">
+      <c r="Q28" s="107">
         <v>153.74071147146736</v>
       </c>
       <c r="R28" t="str">
@@ -37595,16 +37569,16 @@
       <c r="M29" s="103" t="s">
         <v>205</v>
       </c>
-      <c r="N29" s="174">
+      <c r="N29" s="107">
         <v>900</v>
       </c>
-      <c r="O29" s="174">
+      <c r="O29" s="107">
         <v>900</v>
       </c>
-      <c r="P29" s="174">
+      <c r="P29" s="107">
         <v>900</v>
       </c>
-      <c r="Q29" s="174">
+      <c r="Q29" s="107">
         <v>900</v>
       </c>
       <c r="R29" t="str">
@@ -37640,16 +37614,16 @@
       <c r="M30" s="103" t="s">
         <v>143</v>
       </c>
-      <c r="N30" s="174">
+      <c r="N30" s="107">
         <v>4344.0716042398344</v>
       </c>
-      <c r="O30" s="174">
+      <c r="O30" s="107">
         <v>4344.0716042398344</v>
       </c>
-      <c r="P30" s="174">
+      <c r="P30" s="107">
         <v>4344.0716042398344</v>
       </c>
-      <c r="Q30" s="174">
+      <c r="Q30" s="107">
         <v>4344.0716042398344</v>
       </c>
       <c r="R30" t="str">
@@ -37694,16 +37668,16 @@
       <c r="M31" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N31" s="174">
+      <c r="N31" s="107">
         <v>2876</v>
       </c>
-      <c r="O31" s="174">
+      <c r="O31" s="107">
         <v>2876</v>
       </c>
-      <c r="P31" s="174">
+      <c r="P31" s="107">
         <v>2876</v>
       </c>
-      <c r="Q31" s="174">
+      <c r="Q31" s="107">
         <v>2876</v>
       </c>
       <c r="R31" t="str">
@@ -37735,16 +37709,16 @@
       <c r="M32" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N32" s="174">
+      <c r="N32" s="107">
         <v>3144.2390271487925</v>
       </c>
-      <c r="O32" s="174">
+      <c r="O32" s="107">
         <v>3144.2390271487925</v>
       </c>
-      <c r="P32" s="174">
+      <c r="P32" s="107">
         <v>3144.2390271487925</v>
       </c>
-      <c r="Q32" s="174">
+      <c r="Q32" s="107">
         <v>3144.2390271487925</v>
       </c>
       <c r="R32" t="str">
@@ -37776,16 +37750,16 @@
       <c r="M33" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N33" s="176">
+      <c r="N33" s="109">
         <v>0.03</v>
       </c>
-      <c r="O33" s="176">
+      <c r="O33" s="109">
         <v>0.03</v>
       </c>
-      <c r="P33" s="176">
+      <c r="P33" s="109">
         <v>0.03</v>
       </c>
-      <c r="Q33" s="176">
+      <c r="Q33" s="109">
         <v>0.03</v>
       </c>
       <c r="R33" t="str">
@@ -37820,16 +37794,16 @@
       <c r="M34" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N34" s="174">
+      <c r="N34" s="107">
         <v>3074.8142294293471</v>
       </c>
-      <c r="O34" s="174">
+      <c r="O34" s="107">
         <v>3074.8142294293471</v>
       </c>
-      <c r="P34" s="174">
+      <c r="P34" s="107">
         <v>3074.8142294293471</v>
       </c>
-      <c r="Q34" s="174">
+      <c r="Q34" s="107">
         <v>3074.8142294293471</v>
       </c>
       <c r="R34" t="str">
@@ -37871,16 +37845,16 @@
       <c r="M35" s="134" t="s">
         <v>127</v>
       </c>
-      <c r="N35" s="182">
+      <c r="N35" s="133">
         <v>2466</v>
       </c>
-      <c r="O35" s="182">
+      <c r="O35" s="133">
         <v>2466</v>
       </c>
-      <c r="P35" s="182">
+      <c r="P35" s="133">
         <v>2466</v>
       </c>
-      <c r="Q35" s="182">
+      <c r="Q35" s="133">
         <v>2466</v>
       </c>
       <c r="R35" t="str">
@@ -37917,16 +37891,16 @@
       <c r="M36" s="103" t="s">
         <v>275</v>
       </c>
-      <c r="N36" s="180">
+      <c r="N36" s="114">
         <v>5.8458922294713925E-10</v>
       </c>
-      <c r="O36" s="180">
+      <c r="O36" s="114">
         <v>5.8458922294713925E-10</v>
       </c>
-      <c r="P36" s="180">
+      <c r="P36" s="114">
         <v>5.8458922294713925E-10</v>
       </c>
-      <c r="Q36" s="180">
+      <c r="Q36" s="114">
         <v>5.8458922294713925E-10</v>
       </c>
       <c r="R36" t="str">
@@ -37964,16 +37938,16 @@
       <c r="M37" s="103" t="s">
         <v>275</v>
       </c>
-      <c r="N37" s="180">
+      <c r="N37" s="114">
         <v>9.6993208304588435E-11</v>
       </c>
-      <c r="O37" s="180">
+      <c r="O37" s="114">
         <v>9.6993208304588435E-11</v>
       </c>
-      <c r="P37" s="180">
+      <c r="P37" s="114">
         <v>9.6993208304588435E-11</v>
       </c>
-      <c r="Q37" s="180">
+      <c r="Q37" s="114">
         <v>9.6993208304588435E-11</v>
       </c>
       <c r="R37" t="str">
@@ -38011,16 +37985,16 @@
       <c r="M38" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N38" s="176">
+      <c r="N38" s="109">
         <v>0.1423059102718657</v>
       </c>
-      <c r="O38" s="176">
+      <c r="O38" s="109">
         <v>0.1423059102718657</v>
       </c>
-      <c r="P38" s="176">
+      <c r="P38" s="109">
         <v>0.1423059102718657</v>
       </c>
-      <c r="Q38" s="176">
+      <c r="Q38" s="109">
         <v>0.1423059102718657</v>
       </c>
       <c r="R38" t="str">
@@ -38059,16 +38033,16 @@
       <c r="M39" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N39" s="175">
+      <c r="N39" s="108">
         <v>48.860015706266829</v>
       </c>
-      <c r="O39" s="175">
+      <c r="O39" s="108">
         <v>48.860015706266829</v>
       </c>
-      <c r="P39" s="175">
+      <c r="P39" s="108">
         <v>48.860015706266829</v>
       </c>
-      <c r="Q39" s="175">
+      <c r="Q39" s="108">
         <v>48.860015706266829</v>
       </c>
       <c r="R39" t="str">
@@ -38101,16 +38075,16 @@
       <c r="M40" s="103" t="s">
         <v>274</v>
       </c>
-      <c r="N40" s="174">
+      <c r="N40" s="107">
         <v>200</v>
       </c>
-      <c r="O40" s="174">
+      <c r="O40" s="107">
         <v>200</v>
       </c>
-      <c r="P40" s="174">
+      <c r="P40" s="107">
         <v>200</v>
       </c>
-      <c r="Q40" s="174">
+      <c r="Q40" s="107">
         <v>200</v>
       </c>
       <c r="R40" t="str">
@@ -38152,16 +38126,16 @@
       <c r="M41" s="103" t="s">
         <v>274</v>
       </c>
-      <c r="N41" s="174">
+      <c r="N41" s="107">
         <v>33.30212829607494</v>
       </c>
-      <c r="O41" s="174">
+      <c r="O41" s="107">
         <v>33.30212829607494</v>
       </c>
-      <c r="P41" s="174">
+      <c r="P41" s="107">
         <v>33.30212829607494</v>
       </c>
-      <c r="Q41" s="174">
+      <c r="Q41" s="107">
         <v>33.30212829607494</v>
       </c>
       <c r="R41" t="str">
@@ -38200,16 +38174,16 @@
       <c r="M42" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N42" s="178">
+      <c r="N42" s="111">
         <v>3323.2147772434732</v>
       </c>
-      <c r="O42" s="178">
+      <c r="O42" s="111">
         <v>3323.2147772434732</v>
       </c>
-      <c r="P42" s="178">
+      <c r="P42" s="111">
         <v>3323.2147772434732</v>
       </c>
-      <c r="Q42" s="178">
+      <c r="Q42" s="111">
         <v>3323.2147772434732</v>
       </c>
       <c r="R42" t="str">
@@ -38251,16 +38225,16 @@
       <c r="M43" s="103" t="s">
         <v>183</v>
       </c>
-      <c r="N43" s="174">
+      <c r="N43" s="107">
         <v>321.69550000000004</v>
       </c>
-      <c r="O43" s="174">
+      <c r="O43" s="107">
         <v>321.69550000000004</v>
       </c>
-      <c r="P43" s="174">
+      <c r="P43" s="107">
         <v>321.69550000000004</v>
       </c>
-      <c r="Q43" s="174">
+      <c r="Q43" s="107">
         <v>321.69550000000004</v>
       </c>
       <c r="R43" t="str">
@@ -38299,16 +38273,16 @@
       <c r="M44" s="103" t="s">
         <v>183</v>
       </c>
-      <c r="N44" s="174">
+      <c r="N44" s="107">
         <v>321.69550000000004</v>
       </c>
-      <c r="O44" s="174">
+      <c r="O44" s="107">
         <v>321.69550000000004</v>
       </c>
-      <c r="P44" s="174">
+      <c r="P44" s="107">
         <v>321.69550000000004</v>
       </c>
-      <c r="Q44" s="174">
+      <c r="Q44" s="107">
         <v>321.69550000000004</v>
       </c>
       <c r="R44" t="str">
@@ -38347,16 +38321,16 @@
       <c r="M45" s="103" t="s">
         <v>183</v>
       </c>
-      <c r="N45" s="174">
+      <c r="N45" s="107">
         <v>-318.4495</v>
       </c>
-      <c r="O45" s="174">
+      <c r="O45" s="107">
         <v>-318.4495</v>
       </c>
-      <c r="P45" s="174">
+      <c r="P45" s="107">
         <v>-318.4495</v>
       </c>
-      <c r="Q45" s="174">
+      <c r="Q45" s="107">
         <v>-318.4495</v>
       </c>
       <c r="R45" t="str">
@@ -38389,16 +38363,16 @@
       <c r="M46" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N46" s="178">
+      <c r="N46" s="111">
         <v>1320.324829474062</v>
       </c>
-      <c r="O46" s="178">
+      <c r="O46" s="111">
         <v>1320.324829474062</v>
       </c>
-      <c r="P46" s="178">
+      <c r="P46" s="111">
         <v>1320.324829474062</v>
       </c>
-      <c r="Q46" s="178">
+      <c r="Q46" s="111">
         <v>1320.324829474062</v>
       </c>
       <c r="R46" t="str">
@@ -38437,10 +38411,10 @@
       <c r="M47" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N47" s="173"/>
-      <c r="O47" s="173"/>
-      <c r="P47" s="173"/>
-      <c r="Q47" s="173"/>
+      <c r="N47" s="104"/>
+      <c r="O47" s="104"/>
+      <c r="P47" s="104"/>
+      <c r="Q47" s="104"/>
       <c r="R47" t="str">
         <f t="shared" si="0"/>
         <v>(valid in case L-Flange is calculated)</v>
@@ -38475,16 +38449,16 @@
       <c r="M48" s="103" t="s">
         <v>179</v>
       </c>
-      <c r="N48" s="177">
+      <c r="N48" s="110">
         <v>30</v>
       </c>
-      <c r="O48" s="177">
+      <c r="O48" s="110">
         <v>60</v>
       </c>
-      <c r="P48" s="177">
+      <c r="P48" s="110">
         <v>90</v>
       </c>
-      <c r="Q48" s="177">
+      <c r="Q48" s="110">
         <v>120</v>
       </c>
       <c r="R48" t="str">
@@ -38524,16 +38498,16 @@
       <c r="M49" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="N49" s="176">
+      <c r="N49" s="109">
         <v>1.9634954084936207</v>
       </c>
-      <c r="O49" s="176">
+      <c r="O49" s="109">
         <v>3.9269908169872414</v>
       </c>
-      <c r="P49" s="176">
+      <c r="P49" s="109">
         <v>5.8904862254808625</v>
       </c>
-      <c r="Q49" s="176">
+      <c r="Q49" s="109">
         <v>7.8539816339744828</v>
       </c>
       <c r="R49" t="str">
@@ -38570,16 +38544,16 @@
       <c r="M50" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="N50" s="176">
+      <c r="N50" s="109">
         <v>7.5</v>
       </c>
-      <c r="O50" s="176">
+      <c r="O50" s="109">
         <v>7.5</v>
       </c>
-      <c r="P50" s="176">
+      <c r="P50" s="109">
         <v>7.5</v>
       </c>
-      <c r="Q50" s="176">
+      <c r="Q50" s="109">
         <v>7.5</v>
       </c>
       <c r="R50" t="str">
@@ -38616,16 +38590,16 @@
       <c r="M51" s="103" t="s">
         <v>176</v>
       </c>
-      <c r="N51" s="175">
+      <c r="N51" s="108">
         <v>1.4</v>
       </c>
-      <c r="O51" s="175">
+      <c r="O51" s="108">
         <v>1.4</v>
       </c>
-      <c r="P51" s="175">
+      <c r="P51" s="108">
         <v>1.4</v>
       </c>
-      <c r="Q51" s="175">
+      <c r="Q51" s="108">
         <v>1.4</v>
       </c>
       <c r="R51" t="str">
@@ -38668,16 +38642,16 @@
       <c r="M52" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N52" s="176">
+      <c r="N52" s="109">
         <v>0.28773533056547307</v>
       </c>
-      <c r="O52" s="176">
+      <c r="O52" s="109">
         <v>0.74253427729521915</v>
       </c>
-      <c r="P52" s="176">
+      <c r="P52" s="109">
         <v>1.3643968401892383</v>
       </c>
-      <c r="Q52" s="176">
+      <c r="Q52" s="109">
         <v>2.1533230192475301</v>
       </c>
       <c r="R52" t="str">
@@ -38720,16 +38694,16 @@
       <c r="M53" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N53" s="176">
+      <c r="N53" s="109">
         <v>1.2162355202035975</v>
       </c>
-      <c r="O53" s="176">
+      <c r="O53" s="109">
         <v>0.63575115537527993</v>
       </c>
-      <c r="P53" s="176">
+      <c r="P53" s="109">
         <v>0.4993626397773579</v>
       </c>
-      <c r="Q53" s="176">
+      <c r="Q53" s="109">
         <v>0.44426272750754409</v>
       </c>
       <c r="R53" t="str">
@@ -38762,16 +38736,16 @@
       <c r="M54" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="N54" s="176">
+      <c r="N54" s="109">
         <v>1.9634954084936205</v>
       </c>
-      <c r="O54" s="176">
+      <c r="O54" s="109">
         <v>1.9634954084936205</v>
       </c>
-      <c r="P54" s="176">
+      <c r="P54" s="109">
         <v>1.9634954084936205</v>
       </c>
-      <c r="Q54" s="176">
+      <c r="Q54" s="109">
         <v>1.9634954084936205</v>
       </c>
       <c r="R54" t="str">
@@ -38810,16 +38784,16 @@
       <c r="M55" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N55" s="176">
+      <c r="N55" s="109">
         <v>1.9617469257392748</v>
       </c>
-      <c r="O55" s="176">
+      <c r="O55" s="109">
         <v>1.9617469257392748</v>
       </c>
-      <c r="P55" s="176">
+      <c r="P55" s="109">
         <v>1.9617469257392748</v>
       </c>
-      <c r="Q55" s="176">
+      <c r="Q55" s="109">
         <v>1.9617469257392748</v>
       </c>
       <c r="R55" t="str">
@@ -38858,16 +38832,16 @@
       <c r="M56" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N56" s="176">
+      <c r="N56" s="109">
         <v>2.942620388608912</v>
       </c>
-      <c r="O56" s="176">
+      <c r="O56" s="109">
         <v>2.942620388608912</v>
       </c>
-      <c r="P56" s="176">
+      <c r="P56" s="109">
         <v>2.942620388608912</v>
       </c>
-      <c r="Q56" s="176">
+      <c r="Q56" s="109">
         <v>2.942620388608912</v>
       </c>
       <c r="R56" t="str">
@@ -38902,16 +38876,16 @@
         <v>169</v>
       </c>
       <c r="M57" s="103"/>
-      <c r="N57" s="176">
+      <c r="N57" s="109">
         <v>0.95286282352314688</v>
       </c>
-      <c r="O57" s="176">
+      <c r="O57" s="109">
         <v>0.58262609700472079</v>
       </c>
-      <c r="P57" s="176">
+      <c r="P57" s="109">
         <v>0.47184092472685457</v>
       </c>
-      <c r="Q57" s="176">
+      <c r="Q57" s="109">
         <v>0.42441366570439232</v>
       </c>
       <c r="R57" t="str">
@@ -38946,16 +38920,16 @@
         <v>168</v>
       </c>
       <c r="M58" s="103"/>
-      <c r="N58" s="176">
+      <c r="N58" s="109">
         <v>-1.6996879926957522</v>
       </c>
-      <c r="O58" s="176">
+      <c r="O58" s="109">
         <v>-0.46741282911895099</v>
       </c>
-      <c r="P58" s="176">
+      <c r="P58" s="109">
         <v>0.19939552653846943</v>
       </c>
-      <c r="Q58" s="176">
+      <c r="Q58" s="109">
         <v>0.67694875947348121</v>
       </c>
       <c r="R58" t="str">
@@ -38990,16 +38964,16 @@
         <v>167</v>
       </c>
       <c r="M59" s="103"/>
-      <c r="N59" s="176">
+      <c r="N59" s="109">
         <v>-0.13232393428252798</v>
       </c>
-      <c r="O59" s="176">
+      <c r="O59" s="109">
         <v>0.49094883784411425</v>
       </c>
-      <c r="P59" s="176">
+      <c r="P59" s="109">
         <v>0.97552666362167262</v>
       </c>
-      <c r="Q59" s="176">
+      <c r="Q59" s="109">
         <v>1.3750667981906362</v>
       </c>
       <c r="R59" t="str">
@@ -39042,16 +39016,16 @@
       <c r="M60" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N60" s="176">
+      <c r="N60" s="109">
         <v>0.87601845454409977</v>
       </c>
-      <c r="O60" s="176">
+      <c r="O60" s="109">
         <v>1.6338216149415525</v>
       </c>
-      <c r="P60" s="176">
+      <c r="P60" s="109">
         <v>2.6525058127308667</v>
       </c>
-      <c r="Q60" s="176">
+      <c r="Q60" s="109">
         <v>3.9552630780086151</v>
       </c>
       <c r="R60" t="str">
@@ -39091,16 +39065,16 @@
       <c r="M61" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N61" s="176">
+      <c r="N61" s="109">
         <v>0.87601845454409977</v>
       </c>
-      <c r="O61" s="176">
+      <c r="O61" s="109">
         <v>1.6338216149415525</v>
       </c>
-      <c r="P61" s="176">
+      <c r="P61" s="109">
         <v>2.6525058127308667</v>
       </c>
-      <c r="Q61" s="176">
+      <c r="Q61" s="109">
         <v>3.9552630780086151</v>
       </c>
       <c r="R61" t="str">
@@ -39133,10 +39107,10 @@
         <v>163</v>
       </c>
       <c r="M62" s="103"/>
-      <c r="N62" s="181"/>
-      <c r="O62" s="181"/>
-      <c r="P62" s="181"/>
-      <c r="Q62" s="181"/>
+      <c r="N62" s="132"/>
+      <c r="O62" s="132"/>
+      <c r="P62" s="132"/>
+      <c r="Q62" s="132"/>
       <c r="R62" t="str">
         <f t="shared" si="0"/>
         <v>Gap shape formula</v>
@@ -39167,10 +39141,10 @@
         <v>161</v>
       </c>
       <c r="M63" s="103"/>
-      <c r="N63" s="181"/>
-      <c r="O63" s="181"/>
-      <c r="P63" s="181"/>
-      <c r="Q63" s="181"/>
+      <c r="N63" s="132"/>
+      <c r="O63" s="132"/>
+      <c r="P63" s="132"/>
+      <c r="Q63" s="132"/>
       <c r="R63" t="str">
         <f t="shared" si="0"/>
         <v>Stress range formula</v>
@@ -39198,10 +39172,10 @@
         <v>159</v>
       </c>
       <c r="M64" s="103"/>
-      <c r="N64" s="173"/>
-      <c r="O64" s="173"/>
-      <c r="P64" s="173"/>
-      <c r="Q64" s="173"/>
+      <c r="N64" s="104"/>
+      <c r="O64" s="104"/>
+      <c r="P64" s="104"/>
+      <c r="Q64" s="104"/>
       <c r="R64" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -39229,10 +39203,10 @@
         <v>158</v>
       </c>
       <c r="M65" s="103"/>
-      <c r="N65" s="173"/>
-      <c r="O65" s="173"/>
-      <c r="P65" s="173"/>
-      <c r="Q65" s="173"/>
+      <c r="N65" s="104"/>
+      <c r="O65" s="104"/>
+      <c r="P65" s="104"/>
+      <c r="Q65" s="104"/>
       <c r="R65" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -39263,10 +39237,10 @@
         <v>157</v>
       </c>
       <c r="M66" s="103"/>
-      <c r="N66" s="181"/>
-      <c r="O66" s="181"/>
-      <c r="P66" s="181"/>
-      <c r="Q66" s="181"/>
+      <c r="N66" s="132"/>
+      <c r="O66" s="132"/>
+      <c r="P66" s="132"/>
+      <c r="Q66" s="132"/>
       <c r="R66" t="str">
         <f t="shared" si="0"/>
         <v>Summarized formula for bolt force curve</v>
@@ -39299,16 +39273,16 @@
       <c r="M67" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N67" s="176">
+      <c r="N67" s="109">
         <v>-123.29166666666667</v>
       </c>
-      <c r="O67" s="176">
+      <c r="O67" s="109">
         <v>-123.29166666666667</v>
       </c>
-      <c r="P67" s="176">
+      <c r="P67" s="109">
         <v>-123.29166666666667</v>
       </c>
-      <c r="Q67" s="176">
+      <c r="Q67" s="109">
         <v>-123.29166666666667</v>
       </c>
     </row>
@@ -39339,16 +39313,16 @@
       <c r="M68" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N68" s="176">
+      <c r="N68" s="109">
         <v>2876</v>
       </c>
-      <c r="O68" s="176">
+      <c r="O68" s="109">
         <v>2876</v>
       </c>
-      <c r="P68" s="176">
+      <c r="P68" s="109">
         <v>2876</v>
       </c>
-      <c r="Q68" s="176">
+      <c r="Q68" s="109">
         <v>2876</v>
       </c>
     </row>
@@ -39379,16 +39353,16 @@
       <c r="M69" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N69" s="176">
+      <c r="N69" s="109">
         <v>2000.9202638759255</v>
       </c>
-      <c r="O69" s="176">
+      <c r="O69" s="109">
         <v>1696.4363831333353</v>
       </c>
-      <c r="P69" s="176">
+      <c r="P69" s="109">
         <v>1595.2085396502491</v>
       </c>
-      <c r="Q69" s="176">
+      <c r="Q69" s="109">
         <v>1541.2016094157079</v>
       </c>
     </row>
@@ -39419,16 +39393,16 @@
       <c r="M70" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N70" s="176">
+      <c r="N70" s="109">
         <v>3738.8</v>
       </c>
-      <c r="O70" s="176">
+      <c r="O70" s="109">
         <v>3738.8</v>
       </c>
-      <c r="P70" s="176">
+      <c r="P70" s="109">
         <v>3738.8</v>
       </c>
-      <c r="Q70" s="176">
+      <c r="Q70" s="109">
         <v>3738.8</v>
       </c>
     </row>
@@ -39459,16 +39433,16 @@
       <c r="M71" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N71" s="176">
+      <c r="N71" s="109">
         <v>251.14925721102841</v>
       </c>
-      <c r="O71" s="176">
+      <c r="O71" s="109">
         <v>139.05186524303502</v>
       </c>
-      <c r="P71" s="176">
+      <c r="P71" s="109">
         <v>121.69300747304081</v>
       </c>
-      <c r="Q71" s="176">
+      <c r="Q71" s="109">
         <v>114.91573803665135</v>
       </c>
     </row>
@@ -39499,16 +39473,16 @@
       <c r="M72" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N72" s="176">
+      <c r="N72" s="109">
         <v>2939.9421878185444</v>
       </c>
-      <c r="O72" s="176">
+      <c r="O72" s="109">
         <v>2920.7996421348157</v>
       </c>
-      <c r="P72" s="176">
+      <c r="P72" s="109">
         <v>2917.835320467329</v>
       </c>
-      <c r="Q72" s="176">
+      <c r="Q72" s="109">
         <v>2916.677985871765</v>
       </c>
     </row>
@@ -39531,16 +39505,16 @@
         <v>309</v>
       </c>
       <c r="M73" s="103"/>
-      <c r="N73" s="177">
+      <c r="N73" s="110">
         <v>1391753646.6838758</v>
       </c>
-      <c r="O73" s="177">
+      <c r="O73" s="110">
         <v>743485843.40941381</v>
       </c>
-      <c r="P73" s="177">
+      <c r="P73" s="110">
         <v>620359194.07754183</v>
       </c>
-      <c r="Q73" s="177">
+      <c r="Q73" s="110">
         <v>565514679.49266434</v>
       </c>
     </row>
@@ -39563,16 +39537,16 @@
         <v>308</v>
       </c>
       <c r="M74" s="103"/>
-      <c r="N74" s="178">
+      <c r="N74" s="111">
         <v>187240.87089252812</v>
       </c>
-      <c r="O74" s="178">
+      <c r="O74" s="111">
         <v>144826.83391796448</v>
       </c>
-      <c r="P74" s="178">
+      <c r="P74" s="111">
         <v>139478.76999330049</v>
       </c>
-      <c r="Q74" s="178">
+      <c r="Q74" s="111">
         <v>137817.1148098961</v>
       </c>
     </row>
@@ -39595,16 +39569,16 @@
         <v>307</v>
       </c>
       <c r="M75" s="103"/>
-      <c r="N75" s="178">
+      <c r="N75" s="111">
         <v>213725556.87489808</v>
       </c>
-      <c r="O75" s="178">
+      <c r="O75" s="111">
         <v>124680416.00301333</v>
       </c>
-      <c r="P75" s="178">
+      <c r="P75" s="111">
         <v>106159914.78843617</v>
       </c>
-      <c r="Q75" s="178">
+      <c r="Q75" s="111">
         <v>97725643.802408978</v>
       </c>
     </row>
@@ -39631,16 +39605,16 @@
         <v>306</v>
       </c>
       <c r="M76" s="103"/>
-      <c r="N76" s="184">
+      <c r="N76" s="161">
         <v>1.3453592978805262E-4</v>
       </c>
-      <c r="O76" s="184">
+      <c r="O76" s="161">
         <v>1.9479433966601163E-4</v>
       </c>
-      <c r="P76" s="184">
+      <c r="P76" s="161">
         <v>2.2483550066619361E-4</v>
       </c>
-      <c r="Q76" s="184">
+      <c r="Q76" s="161">
         <v>2.4370209971124864E-4</v>
       </c>
     </row>
@@ -39667,16 +39641,16 @@
         <v>305</v>
       </c>
       <c r="M77" s="103"/>
-      <c r="N77" s="184">
+      <c r="N77" s="161">
         <v>0.15356565250189275</v>
       </c>
-      <c r="O77" s="184">
+      <c r="O77" s="161">
         <v>0.16769709485155029</v>
       </c>
-      <c r="P77" s="184">
+      <c r="P77" s="161">
         <v>0.17112652766643241</v>
       </c>
-      <c r="Q77" s="184">
+      <c r="Q77" s="161">
         <v>0.17280832372040422</v>
       </c>
     </row>
@@ -39703,16 +39677,16 @@
         <v>304</v>
       </c>
       <c r="M78" s="103"/>
-      <c r="N78" s="175">
+      <c r="N78" s="108">
         <v>2892.88830676009</v>
       </c>
-      <c r="O78" s="175">
+      <c r="O78" s="108">
         <v>2893.7146176896813</v>
       </c>
-      <c r="P78" s="175">
+      <c r="P78" s="108">
         <v>2893.6807874434912</v>
       </c>
-      <c r="Q78" s="175">
+      <c r="Q78" s="108">
         <v>2893.6013508215733</v>
       </c>
     </row>
@@ -39750,16 +39724,16 @@
       <c r="M79" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N79" s="174">
+      <c r="N79" s="107">
         <v>1244.3580111747735</v>
       </c>
-      <c r="O79" s="174">
+      <c r="O79" s="107">
         <v>806.61559168592612</v>
       </c>
-      <c r="P79" s="174">
+      <c r="P79" s="107">
         <v>712.67155159683637</v>
       </c>
-      <c r="Q79" s="174">
+      <c r="Q79" s="107">
         <v>681.32565393551567</v>
       </c>
       <c r="R79" t="str">
@@ -39791,16 +39765,16 @@
       <c r="M80" s="103" t="s">
         <v>143</v>
       </c>
-      <c r="N80" s="178">
+      <c r="N80" s="111">
         <v>37149.333128699305</v>
       </c>
-      <c r="O80" s="178">
+      <c r="O80" s="111">
         <v>37149.333128699305</v>
       </c>
-      <c r="P80" s="178">
+      <c r="P80" s="111">
         <v>37149.333128699305</v>
       </c>
-      <c r="Q80" s="178">
+      <c r="Q80" s="111">
         <v>37149.333128699305</v>
       </c>
       <c r="R80" t="str">
@@ -39836,16 +39810,16 @@
       <c r="M81" s="103" t="s">
         <v>273</v>
       </c>
-      <c r="N81" s="183">
+      <c r="N81" s="160">
         <v>123831110.42899768</v>
       </c>
-      <c r="O81" s="183">
+      <c r="O81" s="160">
         <v>123831110.42899768</v>
       </c>
-      <c r="P81" s="183">
+      <c r="P81" s="160">
         <v>123831110.42899768</v>
       </c>
-      <c r="Q81" s="183">
+      <c r="Q81" s="160">
         <v>123831110.42899768</v>
       </c>
       <c r="R81" t="str">
@@ -39881,16 +39855,16 @@
       <c r="M82" s="103" t="s">
         <v>143</v>
       </c>
-      <c r="N82" s="178">
+      <c r="N82" s="111">
         <v>87000</v>
       </c>
-      <c r="O82" s="178">
+      <c r="O82" s="111">
         <v>87000</v>
       </c>
-      <c r="P82" s="178">
+      <c r="P82" s="111">
         <v>87000</v>
       </c>
-      <c r="Q82" s="178">
+      <c r="Q82" s="111">
         <v>87000</v>
       </c>
       <c r="R82" t="str">
@@ -39926,16 +39900,16 @@
       <c r="M83" s="103" t="s">
         <v>273</v>
       </c>
-      <c r="N83" s="183">
+      <c r="N83" s="160">
         <v>290000000</v>
       </c>
-      <c r="O83" s="183">
+      <c r="O83" s="160">
         <v>290000000</v>
       </c>
-      <c r="P83" s="183">
+      <c r="P83" s="160">
         <v>290000000</v>
       </c>
-      <c r="Q83" s="183">
+      <c r="Q83" s="160">
         <v>290000000</v>
       </c>
       <c r="R83" t="str">
@@ -39977,16 +39951,16 @@
       <c r="M84" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="N84" s="178">
+      <c r="N84" s="111">
         <v>14636.622779298261</v>
       </c>
-      <c r="O84" s="178">
+      <c r="O84" s="111">
         <v>5087.1057121717786</v>
       </c>
-      <c r="P84" s="178">
+      <c r="P84" s="111">
         <v>2768.4830316768875</v>
       </c>
-      <c r="Q84" s="178">
+      <c r="Q84" s="111">
         <v>1774.9582977160969</v>
       </c>
       <c r="R84" t="str">
@@ -40027,16 +40001,16 @@
       <c r="M85" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="N85" s="178">
+      <c r="N85" s="111">
         <v>4797.9387029107638</v>
       </c>
-      <c r="O85" s="178">
+      <c r="O85" s="111">
         <v>2010.5727094753945</v>
       </c>
-      <c r="P85" s="178">
+      <c r="P85" s="111">
         <v>1058.7224915491406</v>
       </c>
-      <c r="Q85" s="178">
+      <c r="Q85" s="111">
         <v>594.89447044033909</v>
       </c>
       <c r="R85" t="str">
@@ -40075,16 +40049,16 @@
       <c r="M86" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="N86" s="178">
+      <c r="N86" s="111">
         <v>5169.2082946490964</v>
       </c>
-      <c r="O86" s="178">
+      <c r="O86" s="111">
         <v>2212.1093218994611</v>
       </c>
-      <c r="P86" s="178">
+      <c r="P86" s="111">
         <v>1238.3066227426382</v>
       </c>
-      <c r="Q86" s="178">
+      <c r="Q86" s="111">
         <v>800.4072256196913</v>
       </c>
       <c r="R86" t="str">
@@ -40123,16 +40097,16 @@
       <c r="M87" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="N87" s="178">
+      <c r="N87" s="111">
         <v>5169.2082946490964</v>
       </c>
-      <c r="O87" s="178">
+      <c r="O87" s="111">
         <v>2212.1093218994611</v>
       </c>
-      <c r="P87" s="178">
+      <c r="P87" s="111">
         <v>1238.3066227426382</v>
       </c>
-      <c r="Q87" s="178">
+      <c r="Q87" s="111">
         <v>800.4072256196913</v>
       </c>
       <c r="R87" t="str">
@@ -40174,16 +40148,16 @@
       <c r="M88" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N88" s="176">
+      <c r="N88" s="109">
         <v>1.8</v>
       </c>
-      <c r="O88" s="176">
+      <c r="O88" s="109">
         <v>2.1031001583544837</v>
       </c>
-      <c r="P88" s="176">
+      <c r="P88" s="109">
         <v>2.5046502375317257</v>
       </c>
-      <c r="Q88" s="176">
+      <c r="Q88" s="109">
         <v>2.9062003167089676</v>
       </c>
       <c r="R88" t="str">
@@ -40225,16 +40199,16 @@
       <c r="M89" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="N89" s="174">
+      <c r="N89" s="107">
         <v>1483.8020595773849</v>
       </c>
-      <c r="O89" s="174">
+      <c r="O89" s="107">
         <v>100.21145636043828</v>
       </c>
-      <c r="P89" s="174">
+      <c r="P89" s="107">
         <v>20.094755292310523</v>
       </c>
-      <c r="Q89" s="174">
+      <c r="Q89" s="107">
         <v>6.3920006148981718</v>
       </c>
       <c r="R89" t="str">
@@ -40275,16 +40249,16 @@
       <c r="M90" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N90" s="174">
+      <c r="N90" s="107">
         <v>549.79614201309175</v>
       </c>
-      <c r="O90" s="174">
+      <c r="O90" s="107">
         <v>572.34578129959584</v>
       </c>
-      <c r="P90" s="174">
+      <c r="P90" s="107">
         <v>577.93880888131434</v>
       </c>
-      <c r="Q90" s="174">
+      <c r="Q90" s="107">
         <v>579.62119250410046</v>
       </c>
       <c r="R90" t="str">
@@ -40325,16 +40299,16 @@
       <c r="M91" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N91" s="174">
+      <c r="N91" s="107">
         <v>431.02794916761809</v>
       </c>
-      <c r="O91" s="174">
+      <c r="O91" s="107">
         <v>330.74852994509934</v>
       </c>
-      <c r="P91" s="174">
+      <c r="P91" s="107">
         <v>305.87604526965976</v>
       </c>
-      <c r="Q91" s="174">
+      <c r="Q91" s="107">
         <v>298.39439776040422</v>
       </c>
       <c r="R91" t="str">
@@ -40370,16 +40344,16 @@
       <c r="M92" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N92" s="175">
+      <c r="N92" s="108">
         <v>0</v>
       </c>
-      <c r="O92" s="175">
+      <c r="O92" s="108">
         <v>0</v>
       </c>
-      <c r="P92" s="175">
+      <c r="P92" s="108">
         <v>0</v>
       </c>
-      <c r="Q92" s="175">
+      <c r="Q92" s="108">
         <v>0</v>
       </c>
       <c r="R92" t="str">
@@ -40417,16 +40391,16 @@
       <c r="M93" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N93" s="174">
+      <c r="N93" s="107">
         <v>1794.1541531878652</v>
       </c>
-      <c r="O93" s="174">
+      <c r="O93" s="107">
         <v>1378.9613729855218</v>
       </c>
-      <c r="P93" s="174">
+      <c r="P93" s="107">
         <v>1290.6103604781506</v>
       </c>
-      <c r="Q93" s="174">
+      <c r="Q93" s="107">
         <v>1260.9468464396161</v>
       </c>
       <c r="R93" t="str">
@@ -40464,16 +40438,16 @@
       <c r="M94" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N94" s="174">
+      <c r="N94" s="107">
         <v>3595</v>
       </c>
-      <c r="O94" s="174">
+      <c r="O94" s="107">
         <v>3595</v>
       </c>
-      <c r="P94" s="174">
+      <c r="P94" s="107">
         <v>3595</v>
       </c>
-      <c r="Q94" s="174">
+      <c r="Q94" s="107">
         <v>3595</v>
       </c>
       <c r="R94" t="str">
@@ -40518,16 +40492,16 @@
       <c r="M95" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N95" s="174">
+      <c r="N95" s="107">
         <v>2068.2520235998149</v>
       </c>
-      <c r="O95" s="174">
+      <c r="O95" s="107">
         <v>2068.2520235998149</v>
       </c>
-      <c r="P95" s="174">
+      <c r="P95" s="107">
         <v>2068.2520235998149</v>
       </c>
-      <c r="Q95" s="174">
+      <c r="Q95" s="107">
         <v>2068.2520235998149</v>
       </c>
       <c r="R95" t="str">
@@ -40568,16 +40542,16 @@
       <c r="M96" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N96" s="175">
+      <c r="N96" s="108">
         <v>2068.2520235998149</v>
       </c>
-      <c r="O96" s="175">
+      <c r="O96" s="108">
         <v>2068.2520235998149</v>
       </c>
-      <c r="P96" s="175">
+      <c r="P96" s="108">
         <v>2068.2520235998149</v>
       </c>
-      <c r="Q96" s="175">
+      <c r="Q96" s="108">
         <v>2068.2520235998149</v>
       </c>
       <c r="R96" t="str">
@@ -40619,16 +40593,16 @@
       <c r="M97" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N97" s="176">
+      <c r="N97" s="109">
         <v>2.4286136732398829</v>
       </c>
-      <c r="O97" s="176">
+      <c r="O97" s="109">
         <v>1.3446317340090279</v>
       </c>
-      <c r="P97" s="176">
+      <c r="P97" s="109">
         <v>1.176771554766646</v>
       </c>
-      <c r="Q97" s="176">
+      <c r="Q97" s="109">
         <v>1.1112353497098411</v>
       </c>
       <c r="R97" t="str">
@@ -40660,16 +40634,16 @@
       <c r="M98" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N98" s="174">
+      <c r="N98" s="107">
         <v>194.0980661142894</v>
       </c>
-      <c r="O98" s="174">
+      <c r="O98" s="107">
         <v>194.0980661142894</v>
       </c>
-      <c r="P98" s="174">
+      <c r="P98" s="107">
         <v>194.0980661142894</v>
       </c>
-      <c r="Q98" s="174">
+      <c r="Q98" s="107">
         <v>194.0980661142894</v>
       </c>
       <c r="R98" t="str">
@@ -40711,16 +40685,16 @@
       <c r="M99" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="N99" s="174">
+      <c r="N99" s="107">
         <v>10245.332978022379</v>
       </c>
-      <c r="O99" s="174">
+      <c r="O99" s="107">
         <v>14760.990385286221</v>
       </c>
-      <c r="P99" s="174">
+      <c r="P99" s="107">
         <v>15661.360422673919</v>
       </c>
-      <c r="Q99" s="174">
+      <c r="Q99" s="107">
         <v>15956.782644600848</v>
       </c>
       <c r="R99" t="str">
@@ -40762,16 +40736,16 @@
       <c r="M100" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N100" s="178">
+      <c r="N100" s="111">
         <v>823.89401242504141</v>
       </c>
-      <c r="O100" s="178">
+      <c r="O100" s="111">
         <v>1261.6364319138888</v>
       </c>
-      <c r="P100" s="178">
+      <c r="P100" s="111">
         <v>1355.5804720029787</v>
       </c>
-      <c r="Q100" s="178">
+      <c r="Q100" s="111">
         <v>1386.9263696642993</v>
       </c>
       <c r="R100" t="str">
@@ -40816,16 +40790,16 @@
       <c r="M101" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N101" s="176">
+      <c r="N101" s="109">
         <v>0.41430870717841117</v>
       </c>
-      <c r="O101" s="176">
+      <c r="O101" s="109">
         <v>0.4403495083656086</v>
       </c>
-      <c r="P101" s="176">
+      <c r="P101" s="109">
         <v>0.44593813300367485</v>
       </c>
-      <c r="Q101" s="176">
+      <c r="Q101" s="109">
         <v>0.44780286498460981</v>
       </c>
       <c r="R101" t="str">
@@ -40864,16 +40838,16 @@
       <c r="M102" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N102" s="176">
+      <c r="N102" s="109">
         <v>0.41430870717841117</v>
       </c>
-      <c r="O102" s="176">
+      <c r="O102" s="109">
         <v>0.4403495083656086</v>
       </c>
-      <c r="P102" s="176">
+      <c r="P102" s="109">
         <v>0.44593813300367485</v>
       </c>
-      <c r="Q102" s="176">
+      <c r="Q102" s="109">
         <v>0.44780286498460981</v>
       </c>
       <c r="R102" t="str">
@@ -40905,16 +40879,16 @@
       <c r="M103" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N103" s="177">
+      <c r="N103" s="110">
         <v>14795</v>
       </c>
-      <c r="O103" s="177">
+      <c r="O103" s="110">
         <v>14795</v>
       </c>
-      <c r="P103" s="177">
+      <c r="P103" s="110">
         <v>14795</v>
       </c>
-      <c r="Q103" s="177">
+      <c r="Q103" s="110">
         <v>14795</v>
       </c>
       <c r="R103" t="str">
@@ -40956,16 +40930,16 @@
       <c r="M104" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N104" s="174">
+      <c r="N104" s="107">
         <v>-123.29166666666667</v>
       </c>
-      <c r="O104" s="174">
+      <c r="O104" s="107">
         <v>-123.29166666666667</v>
       </c>
-      <c r="P104" s="174">
+      <c r="P104" s="107">
         <v>-123.29166666666667</v>
       </c>
-      <c r="Q104" s="174">
+      <c r="Q104" s="107">
         <v>-123.29166666666667</v>
       </c>
       <c r="R104" t="str">
@@ -40987,10 +40961,10 @@
         <v>42</v>
       </c>
       <c r="M105" s="103"/>
-      <c r="N105" s="173"/>
-      <c r="O105" s="173"/>
-      <c r="P105" s="173"/>
-      <c r="Q105" s="173"/>
+      <c r="N105" s="104"/>
+      <c r="O105" s="104"/>
+      <c r="P105" s="104"/>
+      <c r="Q105" s="104"/>
       <c r="R105" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -41030,16 +41004,16 @@
       <c r="M106" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N106" s="174">
+      <c r="N106" s="107">
         <v>-1367.6496778414403</v>
       </c>
-      <c r="O106" s="174">
+      <c r="O106" s="107">
         <v>-929.90725835259275</v>
       </c>
-      <c r="P106" s="174">
+      <c r="P106" s="107">
         <v>-835.96321826350299</v>
       </c>
-      <c r="Q106" s="174">
+      <c r="Q106" s="107">
         <v>-804.6173206021823</v>
       </c>
       <c r="R106" t="str">
@@ -41081,16 +41055,16 @@
       <c r="M107" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N107" s="176">
+      <c r="N107" s="109">
         <v>0.12040478807649153</v>
       </c>
-      <c r="O107" s="176">
+      <c r="O107" s="109">
         <v>0.11968353670000167</v>
       </c>
-      <c r="P107" s="176">
+      <c r="P107" s="109">
         <v>0.1157083240104905</v>
       </c>
-      <c r="Q107" s="176">
+      <c r="Q107" s="109">
         <v>0.11273981784143602</v>
       </c>
       <c r="R107" t="str">
@@ -41132,16 +41106,16 @@
       <c r="M108" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N108" s="175">
+      <c r="N108" s="108">
         <v>2801.0866686866084</v>
       </c>
-      <c r="O108" s="175">
+      <c r="O108" s="108">
         <v>2827.7306966148312</v>
       </c>
-      <c r="P108" s="175">
+      <c r="P108" s="108">
         <v>2834.7689845973864</v>
       </c>
-      <c r="Q108" s="175">
+      <c r="Q108" s="108">
         <v>2837.5937349423066</v>
       </c>
       <c r="R108" t="str">
@@ -41180,16 +41154,16 @@
       <c r="M109" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N109" s="179">
+      <c r="N109" s="113">
         <v>0.1423059102718657</v>
       </c>
-      <c r="O109" s="179">
+      <c r="O109" s="113">
         <v>0.1423059102718657</v>
       </c>
-      <c r="P109" s="179">
+      <c r="P109" s="113">
         <v>0.1423059102718657</v>
       </c>
-      <c r="Q109" s="179">
+      <c r="Q109" s="113">
         <v>0.1423059102718657</v>
       </c>
       <c r="R109" t="str">
@@ -41228,16 +41202,16 @@
       <c r="M110" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N110" s="179">
+      <c r="N110" s="113">
         <v>0.1423059102718657</v>
       </c>
-      <c r="O110" s="179">
+      <c r="O110" s="113">
         <v>0.1423059102718657</v>
       </c>
-      <c r="P110" s="179">
+      <c r="P110" s="113">
         <v>0.1423059102718657</v>
       </c>
-      <c r="Q110" s="179">
+      <c r="Q110" s="113">
         <v>0.1423059102718657</v>
       </c>
       <c r="R110" t="str">
@@ -41273,10 +41247,10 @@
       <c r="M111" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N111" s="181"/>
-      <c r="O111" s="181"/>
-      <c r="P111" s="181"/>
-      <c r="Q111" s="181"/>
+      <c r="N111" s="132"/>
+      <c r="O111" s="132"/>
+      <c r="P111" s="132"/>
+      <c r="Q111" s="132"/>
       <c r="R111" t="str">
         <f t="shared" si="6"/>
         <v>Bending moment L-Flange as a function of external force Z</v>
@@ -41316,16 +41290,16 @@
       <c r="M112" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N112" s="174">
+      <c r="N112" s="107">
         <v>112.77695050276786</v>
       </c>
-      <c r="O112" s="174">
+      <c r="O112" s="107">
         <v>112.77695050276786</v>
       </c>
-      <c r="P112" s="174">
+      <c r="P112" s="107">
         <v>112.77695050276786</v>
       </c>
-      <c r="Q112" s="174">
+      <c r="Q112" s="107">
         <v>112.77695050276786</v>
       </c>
       <c r="R112" t="str">
@@ -41364,16 +41338,16 @@
       <c r="M113" s="103" t="s">
         <v>268</v>
       </c>
-      <c r="N113" s="180">
+      <c r="N113" s="114">
         <v>1.6641565715404047E-9</v>
       </c>
-      <c r="O113" s="180">
+      <c r="O113" s="114">
         <v>1.6641565715404047E-9</v>
       </c>
-      <c r="P113" s="180">
+      <c r="P113" s="114">
         <v>1.6641565715404047E-9</v>
       </c>
-      <c r="Q113" s="180">
+      <c r="Q113" s="114">
         <v>1.6641565715404047E-9</v>
       </c>
       <c r="R113" t="str">
@@ -41409,10 +41383,10 @@
       <c r="M114" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N114" s="181"/>
-      <c r="O114" s="181"/>
-      <c r="P114" s="181"/>
-      <c r="Q114" s="181"/>
+      <c r="N114" s="132"/>
+      <c r="O114" s="132"/>
+      <c r="P114" s="132"/>
+      <c r="Q114" s="132"/>
       <c r="R114" t="str">
         <f t="shared" si="6"/>
         <v>Bending moment for T-Flange as a function of external force Z</v>
@@ -41446,10 +41420,10 @@
       <c r="M115" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N115" s="181"/>
-      <c r="O115" s="181"/>
-      <c r="P115" s="181"/>
-      <c r="Q115" s="181"/>
+      <c r="N115" s="132"/>
+      <c r="O115" s="132"/>
+      <c r="P115" s="132"/>
+      <c r="Q115" s="132"/>
       <c r="R115" t="str">
         <f t="shared" si="6"/>
         <v>Intermediate values as function of Z</v>
@@ -41483,10 +41457,10 @@
       <c r="M116" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N116" s="181"/>
-      <c r="O116" s="181"/>
-      <c r="P116" s="181"/>
-      <c r="Q116" s="181"/>
+      <c r="N116" s="132"/>
+      <c r="O116" s="132"/>
+      <c r="P116" s="132"/>
+      <c r="Q116" s="132"/>
       <c r="R116" t="str">
         <f t="shared" si="6"/>
         <v>Intermediate values as function of Z</v>
@@ -41529,16 +41503,16 @@
       <c r="M117" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N117" s="176">
+      <c r="N117" s="109">
         <v>0.49415030308522712</v>
       </c>
-      <c r="O117" s="176">
+      <c r="O117" s="109">
         <v>0.58792341515434787</v>
       </c>
-      <c r="P117" s="176">
+      <c r="P117" s="109">
         <v>0.60622809380095677</v>
       </c>
-      <c r="Q117" s="176">
+      <c r="Q117" s="109">
         <v>0.61147882833072409</v>
       </c>
       <c r="R117" t="str">
@@ -41572,16 +41546,16 @@
       <c r="M118" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N118" s="180">
+      <c r="N118" s="114">
         <v>0.1234684985175353</v>
       </c>
-      <c r="O118" s="180">
+      <c r="O118" s="114">
         <v>0.11428595240035409</v>
       </c>
-      <c r="P118" s="180">
+      <c r="P118" s="114">
         <v>0.1071879967338283</v>
       </c>
-      <c r="Q118" s="180">
+      <c r="Q118" s="114">
         <v>0.10262233004223215</v>
       </c>
       <c r="R118" t="str">
@@ -41626,16 +41600,16 @@
       <c r="M119" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N119" s="175">
+      <c r="N119" s="108">
         <v>-322.13499207144736</v>
       </c>
-      <c r="O119" s="175">
+      <c r="O119" s="108">
         <v>-263.63757311066729</v>
       </c>
-      <c r="P119" s="175">
+      <c r="P119" s="108">
         <v>-246.3276668322757</v>
       </c>
-      <c r="Q119" s="175">
+      <c r="Q119" s="108">
         <v>-240.40239495744856</v>
       </c>
       <c r="R119" t="str">
@@ -41669,16 +41643,16 @@
       <c r="M120" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N120" s="175">
+      <c r="N120" s="108">
         <v>-76.819507629007845</v>
       </c>
-      <c r="O120" s="175">
+      <c r="O120" s="108">
         <v>-46.092415558401107</v>
       </c>
-      <c r="P120" s="175">
+      <c r="P120" s="108">
         <v>-38.194917972427533</v>
       </c>
-      <c r="Q120" s="175">
+      <c r="Q120" s="108">
         <v>-34.959613062205065</v>
       </c>
       <c r="R120" t="str">
@@ -41687,184 +41661,184 @@
       </c>
     </row>
     <row r="121" spans="2:18">
-      <c r="N121" s="176">
+      <c r="N121" s="109">
         <v>-123.19166666666668</v>
       </c>
-      <c r="O121" s="176">
+      <c r="O121" s="109">
         <v>-123.19166666666668</v>
       </c>
-      <c r="P121" s="176">
+      <c r="P121" s="109">
         <v>-123.19166666666668</v>
       </c>
-      <c r="Q121" s="176">
+      <c r="Q121" s="109">
         <v>-123.19166666666668</v>
       </c>
     </row>
     <row r="122" spans="2:18">
-      <c r="N122" s="179">
+      <c r="N122" s="113">
         <v>0</v>
       </c>
-      <c r="O122" s="179">
+      <c r="O122" s="113">
         <v>-5.0559479414750573E-13</v>
       </c>
-      <c r="P122" s="179">
+      <c r="P122" s="113">
         <v>-5.0559479414750573E-13</v>
       </c>
-      <c r="Q122" s="179">
+      <c r="Q122" s="113">
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="2:18">
-      <c r="N123" s="176">
+      <c r="N123" s="109">
         <v>-40.182316327404109</v>
       </c>
-      <c r="O123" s="176">
+      <c r="O123" s="109">
         <v>-72.575501817309217</v>
       </c>
-      <c r="P123" s="176">
+      <c r="P123" s="109">
         <v>-82.928009654801173</v>
       </c>
-      <c r="Q123" s="176">
+      <c r="Q123" s="109">
         <v>-87.818771136704058</v>
       </c>
     </row>
     <row r="124" spans="2:18">
-      <c r="N124" s="179">
+      <c r="N124" s="113">
         <v>0</v>
       </c>
-      <c r="O124" s="179">
+      <c r="O124" s="113">
         <v>-5.0559479414750573E-13</v>
       </c>
-      <c r="P124" s="179">
+      <c r="P124" s="113">
         <v>-5.0559479414750573E-13</v>
       </c>
-      <c r="Q124" s="179">
+      <c r="Q124" s="113">
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="2:18">
-      <c r="N125" s="179">
+      <c r="N125" s="113">
         <v>1.3386781456392284E-2</v>
       </c>
-      <c r="O125" s="179">
+      <c r="O125" s="113">
         <v>1.3306591666872168E-2</v>
       </c>
-      <c r="P125" s="179">
+      <c r="P125" s="113">
         <v>1.2864621672428456E-2</v>
       </c>
-      <c r="Q125" s="179">
+      <c r="Q125" s="113">
         <v>1.2534578790321781E-2</v>
       </c>
     </row>
     <row r="126" spans="2:18">
-      <c r="N126" s="176">
+      <c r="N126" s="109">
         <v>-40.149725060359245</v>
       </c>
-      <c r="O126" s="176">
+      <c r="O126" s="109">
         <v>-72.516636929049142</v>
       </c>
-      <c r="P126" s="176">
+      <c r="P126" s="109">
         <v>-82.860748004523572</v>
       </c>
-      <c r="Q126" s="176">
+      <c r="Q126" s="109">
         <v>-87.747542664001102</v>
       </c>
     </row>
     <row r="127" spans="2:18">
-      <c r="N127" s="179">
+      <c r="N127" s="113">
         <v>1.2346849851752828E-2</v>
       </c>
-      <c r="O127" s="179">
+      <c r="O127" s="113">
         <v>1.1428595239529164E-2</v>
       </c>
-      <c r="P127" s="179">
+      <c r="P127" s="113">
         <v>1.0718799672876625E-2</v>
       </c>
-      <c r="Q127" s="179">
+      <c r="Q127" s="113">
         <v>1.0262233004222632E-2</v>
       </c>
     </row>
     <row r="128" spans="2:18">
-      <c r="N128" s="179">
+      <c r="N128" s="113">
         <v>-14.685047887174937</v>
       </c>
-      <c r="O128" s="179">
+      <c r="O128" s="113">
         <v>-26.523476420299968</v>
       </c>
-      <c r="P128" s="179">
+      <c r="P128" s="113">
         <v>-30.306908716915537</v>
       </c>
-      <c r="Q128" s="179">
+      <c r="Q128" s="113">
         <v>-32.094288667371821</v>
       </c>
     </row>
     <row r="129" spans="14:17">
-      <c r="N129" s="179">
+      <c r="N129" s="113">
         <v>2925.8132343674552</v>
       </c>
-      <c r="O129" s="179">
+      <c r="O129" s="113">
         <v>3052.4380171708826</v>
       </c>
-      <c r="P129" s="179">
+      <c r="P129" s="113">
         <v>3079.6130021445742</v>
       </c>
-      <c r="Q129" s="179">
+      <c r="Q129" s="113">
         <v>3088.6803607244869</v>
       </c>
     </row>
     <row r="130" spans="14:17">
-      <c r="N130" s="179">
+      <c r="N130" s="113">
         <v>229.08386220142413</v>
       </c>
-      <c r="O130" s="179">
+      <c r="O130" s="113">
         <v>169.45782240535738</v>
       </c>
-      <c r="P130" s="179">
+      <c r="P130" s="113">
         <v>160.22442342937131</v>
       </c>
-      <c r="Q130" s="179">
+      <c r="Q130" s="113">
         <v>156.61950693641407</v>
       </c>
     </row>
     <row r="131" spans="14:17">
-      <c r="N131" s="183">
+      <c r="N131" s="160">
         <v>4.1905840717736343E-4</v>
       </c>
-      <c r="O131" s="183">
+      <c r="O131" s="160">
         <v>6.0675394176265703E-4</v>
       </c>
-      <c r="P131" s="183">
+      <c r="P131" s="160">
         <v>7.0032746593815128E-4</v>
       </c>
-      <c r="Q131" s="183">
+      <c r="Q131" s="160">
         <v>7.5909397505679655E-4</v>
       </c>
     </row>
     <row r="132" spans="14:17">
-      <c r="N132" s="183">
+      <c r="N132" s="160">
         <v>0.59744121614189982</v>
       </c>
-      <c r="O132" s="183">
+      <c r="O132" s="160">
         <v>0.73747814923545729</v>
       </c>
-      <c r="P132" s="183">
+      <c r="P132" s="160">
         <v>0.77884714204471928</v>
       </c>
-      <c r="Q132" s="183">
+      <c r="Q132" s="160">
         <v>0.79858284162159954</v>
       </c>
     </row>
     <row r="133" spans="14:17">
-      <c r="N133" s="183">
+      <c r="N133" s="160">
         <v>52.604437654353092</v>
       </c>
-      <c r="O133" s="183">
+      <c r="O133" s="160">
         <v>55.178267132717792</v>
       </c>
-      <c r="P133" s="183">
+      <c r="P133" s="160">
         <v>55.072891200019058</v>
       </c>
-      <c r="Q133" s="183">
+      <c r="Q133" s="160">
         <v>54.825458530511014</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Created logger module and implemented logging of variables locally scoped in functions
</commit_message>
<xml_diff>
--- a/tests/validation/BnB_ReferenceFlange-Results-ShapeFactor-1.2.xlsx
+++ b/tests/validation/BnB_ReferenceFlange-Results-ShapeFactor-1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelloB\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\tests\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CEBE36-FF1C-4E65-B0A4-5DD4F2343FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96193662-29FA-42C7-B7CC-EB5A42AF331A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
+    <workbookView xWindow="-28920" yWindow="-9165" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Gap30deg" sheetId="2" r:id="rId1"/>
@@ -4211,7 +4211,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -4545,32 +4545,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF0095D3"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF0095D3"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF0095D3"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF0095D3"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF0095D3"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF0095D3"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4580,7 +4554,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4952,19 +4926,7 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="8" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="8" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="8" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -4981,15 +4943,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="8" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="7" fillId="8" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="8" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4998,18 +4951,6 @@
     </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="8" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="8" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="8" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="7" fillId="8" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5049,6 +4990,15 @@
     <xf numFmtId="171" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5076,17 +5026,14 @@
     <xf numFmtId="0" fontId="22" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="2" fontId="7" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="11" fontId="7" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -19218,7 +19165,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -19586,8 +19533,8 @@
   <dimension ref="A1:DJ178"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O137" sqref="O137"/>
+      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J127" sqref="J127:J164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -19632,32 +19579,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="157" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
+      <c r="B3" s="158"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="158"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="159" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="167"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
-      <c r="G4" s="167"/>
+      <c r="C4" s="159"/>
+      <c r="D4" s="159"/>
+      <c r="E4" s="159"/>
+      <c r="F4" s="159"/>
+      <c r="G4" s="159"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -19673,12 +19620,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="168"/>
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="170"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="161"/>
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="162"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -19686,12 +19633,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="169"/>
-      <c r="D6" s="169"/>
-      <c r="E6" s="169"/>
-      <c r="F6" s="169"/>
-      <c r="G6" s="170"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="161"/>
+      <c r="D6" s="161"/>
+      <c r="E6" s="161"/>
+      <c r="F6" s="161"/>
+      <c r="G6" s="162"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -19699,12 +19646,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="168"/>
-      <c r="C7" s="169"/>
-      <c r="D7" s="169"/>
-      <c r="E7" s="169"/>
-      <c r="F7" s="169"/>
-      <c r="G7" s="170"/>
+      <c r="B7" s="160"/>
+      <c r="C7" s="161"/>
+      <c r="D7" s="161"/>
+      <c r="E7" s="161"/>
+      <c r="F7" s="161"/>
+      <c r="G7" s="162"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -19712,12 +19659,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="B8" s="160"/>
+      <c r="C8" s="161"/>
+      <c r="D8" s="161"/>
+      <c r="E8" s="161"/>
+      <c r="F8" s="161"/>
+      <c r="G8" s="162"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -19725,12 +19672,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="168"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="160"/>
+      <c r="C9" s="161"/>
+      <c r="D9" s="161"/>
+      <c r="E9" s="161"/>
+      <c r="F9" s="161"/>
+      <c r="G9" s="162"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -19778,112 +19725,112 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="171" t="s">
+      <c r="B13" s="153" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="171"/>
-      <c r="D13" s="173" t="s">
+      <c r="C13" s="153"/>
+      <c r="D13" s="152" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="173"/>
-      <c r="F13" s="173"/>
-      <c r="G13" s="173"/>
-      <c r="H13" s="173"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="173"/>
-      <c r="K13" s="173"/>
+      <c r="E13" s="152"/>
+      <c r="F13" s="152"/>
+      <c r="G13" s="152"/>
+      <c r="H13" s="152"/>
+      <c r="I13" s="152"/>
+      <c r="J13" s="152"/>
+      <c r="K13" s="152"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="171" t="s">
+      <c r="B14" s="153" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="171"/>
-      <c r="D14" s="173" t="s">
+      <c r="C14" s="153"/>
+      <c r="D14" s="152" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="173"/>
-      <c r="F14" s="173"/>
-      <c r="G14" s="173"/>
-      <c r="H14" s="173"/>
-      <c r="I14" s="173"/>
-      <c r="J14" s="173"/>
-      <c r="K14" s="173"/>
+      <c r="E14" s="152"/>
+      <c r="F14" s="152"/>
+      <c r="G14" s="152"/>
+      <c r="H14" s="152"/>
+      <c r="I14" s="152"/>
+      <c r="J14" s="152"/>
+      <c r="K14" s="152"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="171" t="s">
+      <c r="B15" s="153" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="173" t="s">
+      <c r="C15" s="153"/>
+      <c r="D15" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="173"/>
-      <c r="F15" s="173"/>
-      <c r="G15" s="173"/>
-      <c r="H15" s="173"/>
-      <c r="I15" s="173"/>
-      <c r="J15" s="173"/>
-      <c r="K15" s="173"/>
+      <c r="E15" s="152"/>
+      <c r="F15" s="152"/>
+      <c r="G15" s="152"/>
+      <c r="H15" s="152"/>
+      <c r="I15" s="152"/>
+      <c r="J15" s="152"/>
+      <c r="K15" s="152"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="171" t="s">
+      <c r="B16" s="153" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="173" t="str">
+      <c r="C16" s="153"/>
+      <c r="D16" s="152" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 30° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="173"/>
-      <c r="F16" s="173"/>
-      <c r="G16" s="173"/>
-      <c r="H16" s="173"/>
-      <c r="I16" s="173"/>
-      <c r="J16" s="173"/>
-      <c r="K16" s="173"/>
+      <c r="E16" s="152"/>
+      <c r="F16" s="152"/>
+      <c r="G16" s="152"/>
+      <c r="H16" s="152"/>
+      <c r="I16" s="152"/>
+      <c r="J16" s="152"/>
+      <c r="K16" s="152"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="171" t="s">
+      <c r="B17" s="153" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="171"/>
-      <c r="D17" s="174">
+      <c r="C17" s="153"/>
+      <c r="D17" s="151">
         <v>0.1</v>
       </c>
-      <c r="E17" s="173"/>
-      <c r="F17" s="173"/>
-      <c r="G17" s="173"/>
-      <c r="H17" s="173"/>
-      <c r="I17" s="173"/>
-      <c r="J17" s="173"/>
-      <c r="K17" s="173"/>
+      <c r="E17" s="152"/>
+      <c r="F17" s="152"/>
+      <c r="G17" s="152"/>
+      <c r="H17" s="152"/>
+      <c r="I17" s="152"/>
+      <c r="J17" s="152"/>
+      <c r="K17" s="152"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="171" t="s">
+      <c r="B18" s="153" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="172">
+      <c r="C18" s="153"/>
+      <c r="D18" s="163">
         <v>45432</v>
       </c>
-      <c r="E18" s="172"/>
-      <c r="F18" s="172"/>
-      <c r="G18" s="172"/>
-      <c r="H18" s="172"/>
-      <c r="I18" s="172"/>
-      <c r="J18" s="172"/>
-      <c r="K18" s="172"/>
+      <c r="E18" s="163"/>
+      <c r="F18" s="163"/>
+      <c r="G18" s="163"/>
+      <c r="H18" s="163"/>
+      <c r="I18" s="163"/>
+      <c r="J18" s="163"/>
+      <c r="K18" s="163"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -20071,16 +20018,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="164"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="155"/>
+      <c r="D28" s="155"/>
+      <c r="E28" s="155"/>
+      <c r="F28" s="155"/>
+      <c r="G28" s="155"/>
+      <c r="H28" s="155"/>
+      <c r="I28" s="155"/>
+      <c r="J28" s="155"/>
+      <c r="K28" s="156"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -22565,7 +22512,7 @@
       <c r="Q111" s="70" t="s">
         <v>297</v>
       </c>
-      <c r="R111" s="148">
+      <c r="R111" s="137">
         <v>0.45</v>
       </c>
     </row>
@@ -22594,7 +22541,7 @@
       <c r="Q112" s="70" t="s">
         <v>298</v>
       </c>
-      <c r="R112" s="148">
+      <c r="R112" s="137">
         <f>R111/2/(J113-J116)</f>
         <v>1.808160804193029E-4</v>
       </c>
@@ -22922,7 +22869,7 @@
       <c r="I127" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="J127" s="130">
+      <c r="J127" s="127">
         <v>1.4</v>
       </c>
       <c r="K127" s="93" t="s">
@@ -22947,8 +22894,8 @@
       <c r="I128" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="J128" s="130">
-        <v>0.28799999999999998</v>
+      <c r="J128" s="97">
+        <v>0.28773533056547312</v>
       </c>
       <c r="K128" s="93" t="s">
         <v>7</v>
@@ -22972,9 +22919,8 @@
       <c r="I129" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="J129" s="131">
-        <f>1216/1000</f>
-        <v>1.216</v>
+      <c r="J129" s="67">
+        <v>1.2162355202035973</v>
       </c>
       <c r="K129" s="5" t="s">
         <v>85</v>
@@ -23012,7 +22958,7 @@
       <c r="G131" s="12"/>
       <c r="H131" s="12"/>
       <c r="I131" s="12"/>
-      <c r="J131" s="126"/>
+      <c r="J131" s="12"/>
       <c r="K131" s="12"/>
       <c r="L131" s="3"/>
       <c r="U131" s="99"/>
@@ -23033,7 +22979,7 @@
       <c r="I132" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="J132" s="127">
+      <c r="J132" s="97">
         <v>1.8</v>
       </c>
       <c r="K132" s="5" t="s">
@@ -23058,8 +23004,8 @@
       <c r="I133" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="J133" s="129">
-        <v>5169.21</v>
+      <c r="J133" s="164">
+        <v>5169.2082946490964</v>
       </c>
       <c r="K133" s="5" t="s">
         <v>80</v>
@@ -23083,8 +23029,8 @@
       <c r="I134" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="J134" s="138">
-        <v>87000</v>
+      <c r="J134" s="98">
+        <v>87000.000000000029</v>
       </c>
       <c r="K134" s="5" t="s">
         <v>218</v>
@@ -23108,8 +23054,8 @@
       <c r="I135" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="J135" s="139">
-        <v>290000000</v>
+      <c r="J135" s="165">
+        <v>290000000.00000006</v>
       </c>
       <c r="K135" s="5" t="s">
         <v>288</v>
@@ -23133,8 +23079,8 @@
       <c r="I136" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="J136" s="128">
-        <v>1483.8</v>
+      <c r="J136" s="164">
+        <v>1483.8038863767938</v>
       </c>
       <c r="K136" s="5" t="s">
         <v>80</v>
@@ -23223,8 +23169,8 @@
       <c r="I140" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="J140" s="130">
-        <v>0.41399999999999998</v>
+      <c r="J140" s="67">
+        <v>0.41432340368180404</v>
       </c>
       <c r="K140" s="5" t="s">
         <v>7</v>
@@ -23248,8 +23194,8 @@
       <c r="I141" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="J141" s="140">
-        <v>10244.9653</v>
+      <c r="J141" s="62">
+        <v>10244.96531616569</v>
       </c>
       <c r="K141" s="5" t="s">
         <v>80</v>
@@ -23618,19 +23564,19 @@
         <v>218</v>
       </c>
       <c r="L155" s="3"/>
-      <c r="N155" s="137">
+      <c r="N155" s="133">
         <v>94.7</v>
       </c>
-      <c r="O155" s="137">
+      <c r="O155" s="133">
         <v>781</v>
       </c>
-      <c r="P155" s="137">
+      <c r="P155" s="133">
         <v>453</v>
       </c>
-      <c r="Q155" s="137">
+      <c r="Q155" s="133">
         <v>139</v>
       </c>
-      <c r="R155" s="137">
+      <c r="R155" s="133">
         <v>75.8</v>
       </c>
       <c r="U155" s="99"/>
@@ -23736,8 +23682,8 @@
       <c r="I160" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="J160" s="145">
-        <v>112.77695050276699</v>
+      <c r="J160" s="64">
+        <v>112.77695050276785</v>
       </c>
       <c r="K160" s="5" t="s">
         <v>7</v>
@@ -23761,8 +23707,8 @@
       <c r="I161" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="J161" s="147">
-        <v>123831110</v>
+      <c r="J161" s="165">
+        <v>123831110.42899768</v>
       </c>
       <c r="K161" s="5" t="s">
         <v>288</v>
@@ -23995,16 +23941,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B18:C18"/>
@@ -24015,6 +23951,16 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B28:K28"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="26" priority="5" stopIfTrue="1" operator="between">
@@ -24054,8 +24000,8 @@
   <dimension ref="A1:DJ178"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J127" sqref="J127:J164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -24100,32 +24046,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="157" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
+      <c r="B3" s="158"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="158"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="159" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="167"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
-      <c r="G4" s="167"/>
+      <c r="C4" s="159"/>
+      <c r="D4" s="159"/>
+      <c r="E4" s="159"/>
+      <c r="F4" s="159"/>
+      <c r="G4" s="159"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -24141,12 +24087,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="168"/>
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="170"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="161"/>
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="162"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -24154,12 +24100,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="169"/>
-      <c r="D6" s="169"/>
-      <c r="E6" s="169"/>
-      <c r="F6" s="169"/>
-      <c r="G6" s="170"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="161"/>
+      <c r="D6" s="161"/>
+      <c r="E6" s="161"/>
+      <c r="F6" s="161"/>
+      <c r="G6" s="162"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -24167,12 +24113,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="168"/>
-      <c r="C7" s="169"/>
-      <c r="D7" s="169"/>
-      <c r="E7" s="169"/>
-      <c r="F7" s="169"/>
-      <c r="G7" s="170"/>
+      <c r="B7" s="160"/>
+      <c r="C7" s="161"/>
+      <c r="D7" s="161"/>
+      <c r="E7" s="161"/>
+      <c r="F7" s="161"/>
+      <c r="G7" s="162"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -24180,12 +24126,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="B8" s="160"/>
+      <c r="C8" s="161"/>
+      <c r="D8" s="161"/>
+      <c r="E8" s="161"/>
+      <c r="F8" s="161"/>
+      <c r="G8" s="162"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -24193,12 +24139,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="168"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="160"/>
+      <c r="C9" s="161"/>
+      <c r="D9" s="161"/>
+      <c r="E9" s="161"/>
+      <c r="F9" s="161"/>
+      <c r="G9" s="162"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -24246,117 +24192,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="171" t="s">
+      <c r="B13" s="153" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="171"/>
-      <c r="D13" s="173" t="str">
+      <c r="C13" s="153"/>
+      <c r="D13" s="152" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="173"/>
-      <c r="F13" s="173"/>
-      <c r="G13" s="173"/>
-      <c r="H13" s="173"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="173"/>
-      <c r="K13" s="173"/>
+      <c r="E13" s="152"/>
+      <c r="F13" s="152"/>
+      <c r="G13" s="152"/>
+      <c r="H13" s="152"/>
+      <c r="I13" s="152"/>
+      <c r="J13" s="152"/>
+      <c r="K13" s="152"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="171" t="s">
+      <c r="B14" s="153" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="171"/>
-      <c r="D14" s="173" t="str">
+      <c r="C14" s="153"/>
+      <c r="D14" s="152" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="173"/>
-      <c r="F14" s="173"/>
-      <c r="G14" s="173"/>
-      <c r="H14" s="173"/>
-      <c r="I14" s="173"/>
-      <c r="J14" s="173"/>
-      <c r="K14" s="173"/>
+      <c r="E14" s="152"/>
+      <c r="F14" s="152"/>
+      <c r="G14" s="152"/>
+      <c r="H14" s="152"/>
+      <c r="I14" s="152"/>
+      <c r="J14" s="152"/>
+      <c r="K14" s="152"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="171" t="s">
+      <c r="B15" s="153" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="173" t="str">
+      <c r="C15" s="153"/>
+      <c r="D15" s="152" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="173"/>
-      <c r="F15" s="173"/>
-      <c r="G15" s="173"/>
-      <c r="H15" s="173"/>
-      <c r="I15" s="173"/>
-      <c r="J15" s="173"/>
-      <c r="K15" s="173"/>
+      <c r="E15" s="152"/>
+      <c r="F15" s="152"/>
+      <c r="G15" s="152"/>
+      <c r="H15" s="152"/>
+      <c r="I15" s="152"/>
+      <c r="J15" s="152"/>
+      <c r="K15" s="152"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="171" t="s">
+      <c r="B16" s="153" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="173" t="str">
+      <c r="C16" s="153"/>
+      <c r="D16" s="152" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 60° gap size ans shape factor 1.2</v>
       </c>
-      <c r="E16" s="173"/>
-      <c r="F16" s="173"/>
-      <c r="G16" s="173"/>
-      <c r="H16" s="173"/>
-      <c r="I16" s="173"/>
-      <c r="J16" s="173"/>
-      <c r="K16" s="173"/>
+      <c r="E16" s="152"/>
+      <c r="F16" s="152"/>
+      <c r="G16" s="152"/>
+      <c r="H16" s="152"/>
+      <c r="I16" s="152"/>
+      <c r="J16" s="152"/>
+      <c r="K16" s="152"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="171" t="s">
+      <c r="B17" s="153" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="171"/>
-      <c r="D17" s="173">
+      <c r="C17" s="153"/>
+      <c r="D17" s="152">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="173"/>
-      <c r="F17" s="173"/>
-      <c r="G17" s="173"/>
-      <c r="H17" s="173"/>
-      <c r="I17" s="173"/>
-      <c r="J17" s="173"/>
-      <c r="K17" s="173"/>
+      <c r="E17" s="152"/>
+      <c r="F17" s="152"/>
+      <c r="G17" s="152"/>
+      <c r="H17" s="152"/>
+      <c r="I17" s="152"/>
+      <c r="J17" s="152"/>
+      <c r="K17" s="152"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="171" t="s">
+      <c r="B18" s="153" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="172">
+      <c r="C18" s="153"/>
+      <c r="D18" s="163">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="172"/>
-      <c r="F18" s="172"/>
-      <c r="G18" s="172"/>
-      <c r="H18" s="172"/>
-      <c r="I18" s="172"/>
-      <c r="J18" s="172"/>
-      <c r="K18" s="172"/>
+      <c r="E18" s="163"/>
+      <c r="F18" s="163"/>
+      <c r="G18" s="163"/>
+      <c r="H18" s="163"/>
+      <c r="I18" s="163"/>
+      <c r="J18" s="163"/>
+      <c r="K18" s="163"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -24544,16 +24490,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="164"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="155"/>
+      <c r="D28" s="155"/>
+      <c r="E28" s="155"/>
+      <c r="F28" s="155"/>
+      <c r="G28" s="155"/>
+      <c r="H28" s="155"/>
+      <c r="I28" s="155"/>
+      <c r="J28" s="155"/>
+      <c r="K28" s="156"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -27358,7 +27304,7 @@
       <c r="I127" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="J127" s="130">
+      <c r="J127" s="127">
         <v>1.4</v>
       </c>
       <c r="K127" s="93" t="s">
@@ -27383,8 +27329,8 @@
       <c r="I128" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="J128" s="130">
-        <v>0.74299999999999999</v>
+      <c r="J128" s="97">
+        <v>0.74253427729521959</v>
       </c>
       <c r="K128" s="93" t="s">
         <v>7</v>
@@ -27408,8 +27354,8 @@
       <c r="I129" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="J129" s="131">
-        <v>0.63600000000000001</v>
+      <c r="J129" s="67">
+        <v>0.63575115537527982</v>
       </c>
       <c r="K129" s="5" t="s">
         <v>85</v>
@@ -27447,7 +27393,7 @@
       <c r="G131" s="12"/>
       <c r="H131" s="12"/>
       <c r="I131" s="12"/>
-      <c r="J131" s="126"/>
+      <c r="J131" s="12"/>
       <c r="K131" s="12"/>
       <c r="L131" s="3"/>
       <c r="U131" s="99"/>
@@ -27468,8 +27414,8 @@
       <c r="I132" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="J132" s="144">
-        <v>2.1031</v>
+      <c r="J132" s="97">
+        <v>2.1031001583544837</v>
       </c>
       <c r="K132" s="5" t="s">
         <v>85</v>
@@ -27493,8 +27439,8 @@
       <c r="I133" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="J133" s="129">
-        <v>2212.11</v>
+      <c r="J133" s="164">
+        <v>2212.1093218994611</v>
       </c>
       <c r="K133" s="5" t="s">
         <v>80</v>
@@ -27518,8 +27464,8 @@
       <c r="I134" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="J134" s="138">
-        <v>87000</v>
+      <c r="J134" s="98">
+        <v>87000.000000000029</v>
       </c>
       <c r="K134" s="5" t="s">
         <v>218</v>
@@ -27543,8 +27489,8 @@
       <c r="I135" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="J135" s="139">
-        <v>290000000</v>
+      <c r="J135" s="165">
+        <v>290000000.00000006</v>
       </c>
       <c r="K135" s="5" t="s">
         <v>288</v>
@@ -27568,8 +27514,8 @@
       <c r="I136" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="J136" s="128">
-        <v>100.21</v>
+      <c r="J136" s="164">
+        <v>100.21148969028162</v>
       </c>
       <c r="K136" s="5" t="s">
         <v>80</v>
@@ -27658,8 +27604,8 @@
       <c r="I140" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="J140" s="130">
-        <v>0.44</v>
+      <c r="J140" s="67">
+        <v>0.44036422450343377</v>
       </c>
       <c r="K140" s="5" t="s">
         <v>7</v>
@@ -27683,8 +27629,8 @@
       <c r="I141" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="J141" s="140">
-        <v>14760.496965</v>
+      <c r="J141" s="62">
+        <v>14760.496964936936</v>
       </c>
       <c r="K141" s="5" t="s">
         <v>80</v>
@@ -28053,19 +27999,19 @@
         <v>218</v>
       </c>
       <c r="L155" s="3"/>
-      <c r="N155" s="137">
+      <c r="N155" s="133">
         <v>94.7</v>
       </c>
-      <c r="O155" s="137">
+      <c r="O155" s="133">
         <v>781</v>
       </c>
-      <c r="P155" s="137">
+      <c r="P155" s="133">
         <v>453</v>
       </c>
-      <c r="Q155" s="137">
+      <c r="Q155" s="133">
         <v>139</v>
       </c>
-      <c r="R155" s="137">
+      <c r="R155" s="133">
         <v>75.8</v>
       </c>
       <c r="U155" s="99"/>
@@ -28146,7 +28092,7 @@
       <c r="I159" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J159" s="62">
+      <c r="J159" s="64">
         <v>225.55390100553569</v>
       </c>
       <c r="K159" s="5" t="s">
@@ -28171,8 +28117,8 @@
       <c r="I160" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="J160" s="146">
-        <v>112.77695050276699</v>
+      <c r="J160" s="64">
+        <v>112.77695050276785</v>
       </c>
       <c r="K160" s="5" t="s">
         <v>7</v>
@@ -28196,8 +28142,8 @@
       <c r="I161" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="J161" s="147">
-        <v>123831110</v>
+      <c r="J161" s="165">
+        <v>123831110.42899768</v>
       </c>
       <c r="K161" s="5" t="s">
         <v>288</v>
@@ -28430,6 +28376,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -28443,13 +28396,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="23" priority="3" stopIfTrue="1" operator="between">
@@ -28489,8 +28435,8 @@
   <dimension ref="A1:DJ178"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J127" sqref="J127:J164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -28535,32 +28481,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="157" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
+      <c r="B3" s="158"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="158"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="159" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="167"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
-      <c r="G4" s="167"/>
+      <c r="C4" s="159"/>
+      <c r="D4" s="159"/>
+      <c r="E4" s="159"/>
+      <c r="F4" s="159"/>
+      <c r="G4" s="159"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -28576,12 +28522,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="168"/>
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="170"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="161"/>
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="162"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -28589,12 +28535,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="169"/>
-      <c r="D6" s="169"/>
-      <c r="E6" s="169"/>
-      <c r="F6" s="169"/>
-      <c r="G6" s="170"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="161"/>
+      <c r="D6" s="161"/>
+      <c r="E6" s="161"/>
+      <c r="F6" s="161"/>
+      <c r="G6" s="162"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -28602,12 +28548,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="168"/>
-      <c r="C7" s="169"/>
-      <c r="D7" s="169"/>
-      <c r="E7" s="169"/>
-      <c r="F7" s="169"/>
-      <c r="G7" s="170"/>
+      <c r="B7" s="160"/>
+      <c r="C7" s="161"/>
+      <c r="D7" s="161"/>
+      <c r="E7" s="161"/>
+      <c r="F7" s="161"/>
+      <c r="G7" s="162"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -28615,12 +28561,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="B8" s="160"/>
+      <c r="C8" s="161"/>
+      <c r="D8" s="161"/>
+      <c r="E8" s="161"/>
+      <c r="F8" s="161"/>
+      <c r="G8" s="162"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -28628,12 +28574,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="168"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="160"/>
+      <c r="C9" s="161"/>
+      <c r="D9" s="161"/>
+      <c r="E9" s="161"/>
+      <c r="F9" s="161"/>
+      <c r="G9" s="162"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -28681,117 +28627,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="171" t="s">
+      <c r="B13" s="153" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="171"/>
-      <c r="D13" s="173" t="str">
+      <c r="C13" s="153"/>
+      <c r="D13" s="152" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="173"/>
-      <c r="F13" s="173"/>
-      <c r="G13" s="173"/>
-      <c r="H13" s="173"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="173"/>
-      <c r="K13" s="173"/>
+      <c r="E13" s="152"/>
+      <c r="F13" s="152"/>
+      <c r="G13" s="152"/>
+      <c r="H13" s="152"/>
+      <c r="I13" s="152"/>
+      <c r="J13" s="152"/>
+      <c r="K13" s="152"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="171" t="s">
+      <c r="B14" s="153" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="171"/>
-      <c r="D14" s="173" t="str">
+      <c r="C14" s="153"/>
+      <c r="D14" s="152" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="173"/>
-      <c r="F14" s="173"/>
-      <c r="G14" s="173"/>
-      <c r="H14" s="173"/>
-      <c r="I14" s="173"/>
-      <c r="J14" s="173"/>
-      <c r="K14" s="173"/>
+      <c r="E14" s="152"/>
+      <c r="F14" s="152"/>
+      <c r="G14" s="152"/>
+      <c r="H14" s="152"/>
+      <c r="I14" s="152"/>
+      <c r="J14" s="152"/>
+      <c r="K14" s="152"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="171" t="s">
+      <c r="B15" s="153" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="173" t="str">
+      <c r="C15" s="153"/>
+      <c r="D15" s="152" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="173"/>
-      <c r="F15" s="173"/>
-      <c r="G15" s="173"/>
-      <c r="H15" s="173"/>
-      <c r="I15" s="173"/>
-      <c r="J15" s="173"/>
-      <c r="K15" s="173"/>
+      <c r="E15" s="152"/>
+      <c r="F15" s="152"/>
+      <c r="G15" s="152"/>
+      <c r="H15" s="152"/>
+      <c r="I15" s="152"/>
+      <c r="J15" s="152"/>
+      <c r="K15" s="152"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="171" t="s">
+      <c r="B16" s="153" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="173" t="str">
+      <c r="C16" s="153"/>
+      <c r="D16" s="152" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 90° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="173"/>
-      <c r="F16" s="173"/>
-      <c r="G16" s="173"/>
-      <c r="H16" s="173"/>
-      <c r="I16" s="173"/>
-      <c r="J16" s="173"/>
-      <c r="K16" s="173"/>
+      <c r="E16" s="152"/>
+      <c r="F16" s="152"/>
+      <c r="G16" s="152"/>
+      <c r="H16" s="152"/>
+      <c r="I16" s="152"/>
+      <c r="J16" s="152"/>
+      <c r="K16" s="152"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="171" t="s">
+      <c r="B17" s="153" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="171"/>
-      <c r="D17" s="173">
+      <c r="C17" s="153"/>
+      <c r="D17" s="152">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="173"/>
-      <c r="F17" s="173"/>
-      <c r="G17" s="173"/>
-      <c r="H17" s="173"/>
-      <c r="I17" s="173"/>
-      <c r="J17" s="173"/>
-      <c r="K17" s="173"/>
+      <c r="E17" s="152"/>
+      <c r="F17" s="152"/>
+      <c r="G17" s="152"/>
+      <c r="H17" s="152"/>
+      <c r="I17" s="152"/>
+      <c r="J17" s="152"/>
+      <c r="K17" s="152"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="171" t="s">
+      <c r="B18" s="153" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="172">
+      <c r="C18" s="153"/>
+      <c r="D18" s="163">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="172"/>
-      <c r="F18" s="172"/>
-      <c r="G18" s="172"/>
-      <c r="H18" s="172"/>
-      <c r="I18" s="172"/>
-      <c r="J18" s="172"/>
-      <c r="K18" s="172"/>
+      <c r="E18" s="163"/>
+      <c r="F18" s="163"/>
+      <c r="G18" s="163"/>
+      <c r="H18" s="163"/>
+      <c r="I18" s="163"/>
+      <c r="J18" s="163"/>
+      <c r="K18" s="163"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -28979,16 +28925,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="164"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="155"/>
+      <c r="D28" s="155"/>
+      <c r="E28" s="155"/>
+      <c r="F28" s="155"/>
+      <c r="G28" s="155"/>
+      <c r="H28" s="155"/>
+      <c r="I28" s="155"/>
+      <c r="J28" s="155"/>
+      <c r="K28" s="156"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -31793,7 +31739,7 @@
       <c r="I127" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="J127" s="130">
+      <c r="J127" s="127">
         <v>1.4</v>
       </c>
       <c r="K127" s="93" t="s">
@@ -31818,9 +31764,8 @@
       <c r="I128" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="J128" s="131">
-        <f>1364/1000</f>
-        <v>1.3640000000000001</v>
+      <c r="J128" s="97">
+        <v>1.3643968401892375</v>
       </c>
       <c r="K128" s="93" t="s">
         <v>7</v>
@@ -31844,8 +31789,8 @@
       <c r="I129" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="J129" s="131">
-        <v>0.499</v>
+      <c r="J129" s="67">
+        <v>0.4993626397773579</v>
       </c>
       <c r="K129" s="5" t="s">
         <v>85</v>
@@ -31883,7 +31828,7 @@
       <c r="G131" s="12"/>
       <c r="H131" s="12"/>
       <c r="I131" s="12"/>
-      <c r="J131" s="126"/>
+      <c r="J131" s="12"/>
       <c r="K131" s="12"/>
       <c r="L131" s="3"/>
       <c r="U131" s="99"/>
@@ -31904,8 +31849,8 @@
       <c r="I132" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="J132" s="144">
-        <v>2.5046499999999998</v>
+      <c r="J132" s="97">
+        <v>2.5046502375317257</v>
       </c>
       <c r="K132" s="5" t="s">
         <v>85</v>
@@ -31929,8 +31874,8 @@
       <c r="I133" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="J133" s="129">
-        <v>1238.31</v>
+      <c r="J133" s="164">
+        <v>1238.3066227426382</v>
       </c>
       <c r="K133" s="5" t="s">
         <v>80</v>
@@ -31954,8 +31899,8 @@
       <c r="I134" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="J134" s="138">
-        <v>87000</v>
+      <c r="J134" s="98">
+        <v>87000.000000000029</v>
       </c>
       <c r="K134" s="5" t="s">
         <v>218</v>
@@ -31979,8 +31924,8 @@
       <c r="I135" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="J135" s="139">
-        <v>290000000</v>
+      <c r="J135" s="165">
+        <v>290000000.00000006</v>
       </c>
       <c r="K135" s="5" t="s">
         <v>288</v>
@@ -32004,8 +31949,8 @@
       <c r="I136" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="J136" s="128">
-        <v>20.09</v>
+      <c r="J136" s="164">
+        <v>20.094758307720781</v>
       </c>
       <c r="K136" s="5" t="s">
         <v>80</v>
@@ -32094,8 +32039,8 @@
       <c r="I140" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="J140" s="130">
-        <v>0.44600000000000001</v>
+      <c r="J140" s="67">
+        <v>0.44595284973156152</v>
       </c>
       <c r="K140" s="5" t="s">
         <v>7</v>
@@ -32119,8 +32064,8 @@
       <c r="I141" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="J141" s="140">
-        <v>15660.843568</v>
+      <c r="J141" s="62">
+        <v>15660.843568082577</v>
       </c>
       <c r="K141" s="5" t="s">
         <v>80</v>
@@ -32489,19 +32434,19 @@
         <v>218</v>
       </c>
       <c r="L155" s="3"/>
-      <c r="N155" s="137">
+      <c r="N155" s="133">
         <v>94.7</v>
       </c>
-      <c r="O155" s="137">
+      <c r="O155" s="133">
         <v>781</v>
       </c>
-      <c r="P155" s="137">
+      <c r="P155" s="133">
         <v>453</v>
       </c>
-      <c r="Q155" s="137">
+      <c r="Q155" s="133">
         <v>139</v>
       </c>
-      <c r="R155" s="137">
+      <c r="R155" s="133">
         <v>75.8</v>
       </c>
       <c r="U155" s="99"/>
@@ -32582,7 +32527,7 @@
       <c r="I159" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J159" s="62">
+      <c r="J159" s="64">
         <v>225.55390100553569</v>
       </c>
       <c r="K159" s="5" t="s">
@@ -32607,8 +32552,8 @@
       <c r="I160" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="J160" s="145">
-        <v>112.77695050276699</v>
+      <c r="J160" s="64">
+        <v>112.77695050276785</v>
       </c>
       <c r="K160" s="5" t="s">
         <v>7</v>
@@ -32632,8 +32577,8 @@
       <c r="I161" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="J161" s="147">
-        <v>123831110</v>
+      <c r="J161" s="165">
+        <v>123831110.42899768</v>
       </c>
       <c r="K161" s="5" t="s">
         <v>288</v>
@@ -32657,7 +32602,7 @@
       <c r="I162" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="J162" s="62">
+      <c r="J162" s="92">
         <v>10310.000230734646</v>
       </c>
       <c r="K162" s="5" t="s">
@@ -32866,6 +32811,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -32879,13 +32831,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="20" priority="3" stopIfTrue="1" operator="between">
@@ -32924,9 +32869,9 @@
   </sheetPr>
   <dimension ref="A1:DJ178"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -32971,32 +32916,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="157" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
+      <c r="B3" s="158"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="158"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="159" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="167"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
-      <c r="G4" s="167"/>
+      <c r="C4" s="159"/>
+      <c r="D4" s="159"/>
+      <c r="E4" s="159"/>
+      <c r="F4" s="159"/>
+      <c r="G4" s="159"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -33012,12 +32957,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="168"/>
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="170"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="161"/>
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="162"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -33025,12 +32970,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="169"/>
-      <c r="D6" s="169"/>
-      <c r="E6" s="169"/>
-      <c r="F6" s="169"/>
-      <c r="G6" s="170"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="161"/>
+      <c r="D6" s="161"/>
+      <c r="E6" s="161"/>
+      <c r="F6" s="161"/>
+      <c r="G6" s="162"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -33038,12 +32983,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="168"/>
-      <c r="C7" s="169"/>
-      <c r="D7" s="169"/>
-      <c r="E7" s="169"/>
-      <c r="F7" s="169"/>
-      <c r="G7" s="170"/>
+      <c r="B7" s="160"/>
+      <c r="C7" s="161"/>
+      <c r="D7" s="161"/>
+      <c r="E7" s="161"/>
+      <c r="F7" s="161"/>
+      <c r="G7" s="162"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -33051,12 +32996,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="B8" s="160"/>
+      <c r="C8" s="161"/>
+      <c r="D8" s="161"/>
+      <c r="E8" s="161"/>
+      <c r="F8" s="161"/>
+      <c r="G8" s="162"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -33064,12 +33009,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="168"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="160"/>
+      <c r="C9" s="161"/>
+      <c r="D9" s="161"/>
+      <c r="E9" s="161"/>
+      <c r="F9" s="161"/>
+      <c r="G9" s="162"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -33117,117 +33062,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="171" t="s">
+      <c r="B13" s="153" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="171"/>
-      <c r="D13" s="173" t="str">
+      <c r="C13" s="153"/>
+      <c r="D13" s="152" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="173"/>
-      <c r="F13" s="173"/>
-      <c r="G13" s="173"/>
-      <c r="H13" s="173"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="173"/>
-      <c r="K13" s="173"/>
+      <c r="E13" s="152"/>
+      <c r="F13" s="152"/>
+      <c r="G13" s="152"/>
+      <c r="H13" s="152"/>
+      <c r="I13" s="152"/>
+      <c r="J13" s="152"/>
+      <c r="K13" s="152"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="171" t="s">
+      <c r="B14" s="153" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="171"/>
-      <c r="D14" s="173" t="str">
+      <c r="C14" s="153"/>
+      <c r="D14" s="152" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="173"/>
-      <c r="F14" s="173"/>
-      <c r="G14" s="173"/>
-      <c r="H14" s="173"/>
-      <c r="I14" s="173"/>
-      <c r="J14" s="173"/>
-      <c r="K14" s="173"/>
+      <c r="E14" s="152"/>
+      <c r="F14" s="152"/>
+      <c r="G14" s="152"/>
+      <c r="H14" s="152"/>
+      <c r="I14" s="152"/>
+      <c r="J14" s="152"/>
+      <c r="K14" s="152"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="171" t="s">
+      <c r="B15" s="153" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="173" t="str">
+      <c r="C15" s="153"/>
+      <c r="D15" s="152" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="173"/>
-      <c r="F15" s="173"/>
-      <c r="G15" s="173"/>
-      <c r="H15" s="173"/>
-      <c r="I15" s="173"/>
-      <c r="J15" s="173"/>
-      <c r="K15" s="173"/>
+      <c r="E15" s="152"/>
+      <c r="F15" s="152"/>
+      <c r="G15" s="152"/>
+      <c r="H15" s="152"/>
+      <c r="I15" s="152"/>
+      <c r="J15" s="152"/>
+      <c r="K15" s="152"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="171" t="s">
+      <c r="B16" s="153" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="173" t="str">
+      <c r="C16" s="153"/>
+      <c r="D16" s="152" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 120° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="173"/>
-      <c r="F16" s="173"/>
-      <c r="G16" s="173"/>
-      <c r="H16" s="173"/>
-      <c r="I16" s="173"/>
-      <c r="J16" s="173"/>
-      <c r="K16" s="173"/>
+      <c r="E16" s="152"/>
+      <c r="F16" s="152"/>
+      <c r="G16" s="152"/>
+      <c r="H16" s="152"/>
+      <c r="I16" s="152"/>
+      <c r="J16" s="152"/>
+      <c r="K16" s="152"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="171" t="s">
+      <c r="B17" s="153" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="171"/>
-      <c r="D17" s="173">
+      <c r="C17" s="153"/>
+      <c r="D17" s="152">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="173"/>
-      <c r="F17" s="173"/>
-      <c r="G17" s="173"/>
-      <c r="H17" s="173"/>
-      <c r="I17" s="173"/>
-      <c r="J17" s="173"/>
-      <c r="K17" s="173"/>
+      <c r="E17" s="152"/>
+      <c r="F17" s="152"/>
+      <c r="G17" s="152"/>
+      <c r="H17" s="152"/>
+      <c r="I17" s="152"/>
+      <c r="J17" s="152"/>
+      <c r="K17" s="152"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="171" t="s">
+      <c r="B18" s="153" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="172">
+      <c r="C18" s="153"/>
+      <c r="D18" s="163">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="172"/>
-      <c r="F18" s="172"/>
-      <c r="G18" s="172"/>
-      <c r="H18" s="172"/>
-      <c r="I18" s="172"/>
-      <c r="J18" s="172"/>
-      <c r="K18" s="172"/>
+      <c r="E18" s="163"/>
+      <c r="F18" s="163"/>
+      <c r="G18" s="163"/>
+      <c r="H18" s="163"/>
+      <c r="I18" s="163"/>
+      <c r="J18" s="163"/>
+      <c r="K18" s="163"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -33415,16 +33360,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="164"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="155"/>
+      <c r="D28" s="155"/>
+      <c r="E28" s="155"/>
+      <c r="F28" s="155"/>
+      <c r="G28" s="155"/>
+      <c r="H28" s="155"/>
+      <c r="I28" s="155"/>
+      <c r="J28" s="155"/>
+      <c r="K28" s="156"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -36077,7 +36022,7 @@
       <c r="J119" s="80">
         <v>7.9852229242372876E-4</v>
       </c>
-      <c r="K119" s="158">
+      <c r="K119" s="147">
         <v>7.5907182981623907E-10</v>
       </c>
       <c r="L119" s="3"/>
@@ -36229,7 +36174,7 @@
       <c r="I127" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="J127" s="130">
+      <c r="J127" s="127">
         <v>1.4</v>
       </c>
       <c r="K127" s="93" t="s">
@@ -36254,9 +36199,8 @@
       <c r="I128" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="J128" s="131">
-        <f>2153/1000</f>
-        <v>2.153</v>
+      <c r="J128" s="97">
+        <v>2.1533230192475297</v>
       </c>
       <c r="K128" s="93" t="s">
         <v>7</v>
@@ -36280,8 +36224,8 @@
       <c r="I129" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="J129" s="131">
-        <v>0.44400000000000001</v>
+      <c r="J129" s="67">
+        <v>0.44426272750754392</v>
       </c>
       <c r="K129" s="5" t="s">
         <v>85</v>
@@ -36319,7 +36263,7 @@
       <c r="G131" s="12"/>
       <c r="H131" s="12"/>
       <c r="I131" s="12"/>
-      <c r="J131" s="126"/>
+      <c r="J131" s="12"/>
       <c r="K131" s="12"/>
       <c r="L131" s="3"/>
       <c r="U131" s="99"/>
@@ -36340,8 +36284,8 @@
       <c r="I132" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="J132" s="144">
-        <v>2.9062000000000001</v>
+      <c r="J132" s="97">
+        <v>2.9062003167089676</v>
       </c>
       <c r="K132" s="5" t="s">
         <v>85</v>
@@ -36365,8 +36309,8 @@
       <c r="I133" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="J133" s="129">
-        <v>800.41</v>
+      <c r="J133" s="164">
+        <v>800.40722561969153</v>
       </c>
       <c r="K133" s="5" t="s">
         <v>80</v>
@@ -36390,8 +36334,8 @@
       <c r="I134" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="J134" s="138">
-        <v>87000</v>
+      <c r="J134" s="98">
+        <v>87000.000000000029</v>
       </c>
       <c r="K134" s="5" t="s">
         <v>218</v>
@@ -36415,8 +36359,8 @@
       <c r="I135" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="J135" s="139">
-        <v>290000000</v>
+      <c r="J135" s="165">
+        <v>290000000.00000006</v>
       </c>
       <c r="K135" s="5" t="s">
         <v>288</v>
@@ -36440,8 +36384,8 @@
       <c r="I136" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="J136" s="128">
-        <v>6.39</v>
+      <c r="J136" s="164">
+        <v>6.3920011573135929</v>
       </c>
       <c r="K136" s="5" t="s">
         <v>80</v>
@@ -36530,8 +36474,8 @@
       <c r="I140" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="J140" s="130">
-        <v>0.44800000000000001</v>
+      <c r="J140" s="67">
+        <v>0.44781758178683745</v>
       </c>
       <c r="K140" s="5" t="s">
         <v>7</v>
@@ -36555,8 +36499,8 @@
       <c r="I141" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="J141" s="140">
-        <v>15956.288200000001</v>
+      <c r="J141" s="62">
+        <v>15956.258245417217</v>
       </c>
       <c r="K141" s="5" t="s">
         <v>80</v>
@@ -36925,19 +36869,19 @@
         <v>218</v>
       </c>
       <c r="L155" s="3"/>
-      <c r="N155" s="137">
+      <c r="N155" s="133">
         <v>94.7</v>
       </c>
-      <c r="O155" s="137">
+      <c r="O155" s="133">
         <v>781</v>
       </c>
-      <c r="P155" s="137">
+      <c r="P155" s="133">
         <v>453</v>
       </c>
-      <c r="Q155" s="137">
+      <c r="Q155" s="133">
         <v>139</v>
       </c>
-      <c r="R155" s="137">
+      <c r="R155" s="133">
         <v>75.8</v>
       </c>
       <c r="U155" s="99"/>
@@ -37018,7 +36962,7 @@
       <c r="I159" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J159" s="62">
+      <c r="J159" s="64">
         <v>225.55390100553569</v>
       </c>
       <c r="K159" s="5" t="s">
@@ -37043,8 +36987,8 @@
       <c r="I160" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="J160" s="145">
-        <v>112.77695050276699</v>
+      <c r="J160" s="64">
+        <v>112.77695050276785</v>
       </c>
       <c r="K160" s="5" t="s">
         <v>7</v>
@@ -37068,8 +37012,8 @@
       <c r="I161" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="J161" s="147">
-        <v>123831110</v>
+      <c r="J161" s="165">
+        <v>123831110.42899768</v>
       </c>
       <c r="K161" s="5" t="s">
         <v>288</v>
@@ -37093,7 +37037,7 @@
       <c r="I162" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="J162" s="62">
+      <c r="J162" s="92">
         <v>10310.000230734646</v>
       </c>
       <c r="K162" s="5" t="s">
@@ -37302,6 +37246,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -37315,13 +37266,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="17" priority="3" stopIfTrue="1" operator="between">
@@ -37358,7 +37302,7 @@
   <sheetPr codeName="Tabelle12"/>
   <dimension ref="B2:R133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
@@ -37385,23 +37329,23 @@
       </c>
     </row>
     <row r="20" spans="2:18" ht="13.8">
-      <c r="G20" s="141" t="s">
+      <c r="G20" s="134" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="18">
-      <c r="G21" s="142">
+      <c r="G21" s="135">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="2:18">
-      <c r="G22" s="143">
+      <c r="G22" s="136">
         <f>MATCH(gap_angle,N48:Q48,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:18">
-      <c r="G23" s="143" t="str">
+      <c r="G23" s="136" t="str">
         <f>"Gap"&amp;gap_angle&amp;"deg"</f>
         <v>Gap30deg</v>
       </c>
@@ -37472,7 +37416,7 @@
       <c r="H27" t="s">
         <v>209</v>
       </c>
-      <c r="I27" s="149"/>
+      <c r="I27" s="138"/>
       <c r="K27" s="106">
         <v>1</v>
       </c>
@@ -37510,7 +37454,7 @@
       <c r="H28" t="s">
         <v>207</v>
       </c>
-      <c r="I28" s="150"/>
+      <c r="I28" s="139"/>
       <c r="K28" s="106">
         <f>K27+1</f>
         <v>2</v>
@@ -37561,7 +37505,7 @@
       <c r="H29" t="s">
         <v>204</v>
       </c>
-      <c r="I29" s="150"/>
+      <c r="I29" s="139"/>
       <c r="K29" s="106"/>
       <c r="L29" s="105" t="s">
         <v>206</v>
@@ -37606,7 +37550,7 @@
         <f ca="1">(F30-E30)/E30</f>
         <v>-4.0989759090784605E-6</v>
       </c>
-      <c r="I30" s="150"/>
+      <c r="I30" s="139"/>
       <c r="K30" s="106"/>
       <c r="L30" s="105" t="s">
         <v>203</v>
@@ -37657,7 +37601,7 @@
       <c r="H31" t="s">
         <v>202</v>
       </c>
-      <c r="I31" s="149"/>
+      <c r="I31" s="138"/>
       <c r="K31" s="106">
         <f>K28+1</f>
         <v>3</v>
@@ -37701,7 +37645,7 @@
         <v>85</v>
       </c>
       <c r="G32" s="107"/>
-      <c r="I32" s="149"/>
+      <c r="I32" s="138"/>
       <c r="K32" s="106"/>
       <c r="L32" s="103" t="s">
         <v>201</v>
@@ -37742,7 +37686,7 @@
         <v>85</v>
       </c>
       <c r="G33" s="109"/>
-      <c r="I33" s="149"/>
+      <c r="I33" s="138"/>
       <c r="K33" s="106"/>
       <c r="L33" s="103" t="s">
         <v>200</v>
@@ -37786,7 +37730,7 @@
       <c r="H34" t="s">
         <v>198</v>
       </c>
-      <c r="I34" s="149"/>
+      <c r="I34" s="138"/>
       <c r="K34" s="106"/>
       <c r="L34" s="103" t="s">
         <v>199</v>
@@ -37812,49 +37756,49 @@
       </c>
     </row>
     <row r="35" spans="2:18" ht="15.6">
-      <c r="B35" s="135">
+      <c r="B35" s="131">
         <f>B31+1</f>
         <v>4</v>
       </c>
-      <c r="C35" s="134" t="s">
+      <c r="C35" s="130" t="s">
         <v>276</v>
       </c>
-      <c r="D35" s="134" t="s">
+      <c r="D35" s="130" t="s">
         <v>127</v>
       </c>
-      <c r="E35" s="133" cm="1">
+      <c r="E35" s="129" cm="1">
         <f t="array" ref="E35">INDEX(N35:Q35,case_number)</f>
         <v>2466</v>
       </c>
-      <c r="F35" s="133" t="s">
+      <c r="F35" s="129" t="s">
         <v>85</v>
       </c>
-      <c r="G35" s="133"/>
-      <c r="H35" s="136" t="s">
+      <c r="G35" s="129"/>
+      <c r="H35" s="132" t="s">
         <v>196</v>
       </c>
-      <c r="I35" s="151"/>
-      <c r="J35" s="136"/>
-      <c r="K35" s="135">
+      <c r="I35" s="140"/>
+      <c r="J35" s="132"/>
+      <c r="K35" s="131">
         <f>K31+1</f>
         <v>4</v>
       </c>
-      <c r="L35" s="134" t="s">
+      <c r="L35" s="130" t="s">
         <v>276</v>
       </c>
-      <c r="M35" s="134" t="s">
+      <c r="M35" s="130" t="s">
         <v>127</v>
       </c>
-      <c r="N35" s="133">
+      <c r="N35" s="129">
         <v>2466</v>
       </c>
-      <c r="O35" s="133">
+      <c r="O35" s="129">
         <v>2466</v>
       </c>
-      <c r="P35" s="133">
+      <c r="P35" s="129">
         <v>2466</v>
       </c>
-      <c r="Q35" s="133">
+      <c r="Q35" s="129">
         <v>2466</v>
       </c>
       <c r="R35" t="str">
@@ -37882,9 +37826,9 @@
         <f ca="1">(F36-E36)/E36</f>
         <v>4.0287388955891572E-5</v>
       </c>
-      <c r="I36" s="152"/>
-      <c r="J36" s="153"/>
-      <c r="K36" s="154"/>
+      <c r="I36" s="141"/>
+      <c r="J36" s="142"/>
+      <c r="K36" s="143"/>
       <c r="L36" s="105" t="s">
         <v>195</v>
       </c>
@@ -37928,10 +37872,10 @@
         <f ca="1">(F37-E37)/E37</f>
         <v>-3.9976088935691896E-16</v>
       </c>
-      <c r="H37" s="159"/>
-      <c r="I37" s="152"/>
-      <c r="J37" s="153"/>
-      <c r="K37" s="154"/>
+      <c r="H37" s="148"/>
+      <c r="I37" s="141"/>
+      <c r="J37" s="142"/>
+      <c r="K37" s="143"/>
       <c r="L37" s="105" t="s">
         <v>194</v>
       </c>
@@ -37975,10 +37919,10 @@
         <f ca="1">(F38-E38)/E38</f>
         <v>-3.4553061442869523E-5</v>
       </c>
-      <c r="H38" s="159"/>
-      <c r="I38" s="152"/>
-      <c r="J38" s="153"/>
-      <c r="K38" s="154"/>
+      <c r="H38" s="148"/>
+      <c r="I38" s="141"/>
+      <c r="J38" s="142"/>
+      <c r="K38" s="143"/>
       <c r="L38" s="105" t="s">
         <v>193</v>
       </c>
@@ -38021,9 +37965,9 @@
         <v>85</v>
       </c>
       <c r="G39" s="108"/>
-      <c r="I39" s="152"/>
-      <c r="J39" s="153"/>
-      <c r="K39" s="154">
+      <c r="I39" s="141"/>
+      <c r="J39" s="142"/>
+      <c r="K39" s="143">
         <f>K35+1</f>
         <v>5</v>
       </c>
@@ -38066,9 +38010,9 @@
         <v>85</v>
       </c>
       <c r="G40" s="107"/>
-      <c r="I40" s="152"/>
-      <c r="J40" s="153"/>
-      <c r="K40" s="154"/>
+      <c r="I40" s="141"/>
+      <c r="J40" s="142"/>
+      <c r="K40" s="143"/>
       <c r="L40" s="105" t="s">
         <v>191</v>
       </c>
@@ -38114,9 +38058,9 @@
       <c r="H41" t="s">
         <v>189</v>
       </c>
-      <c r="I41" s="155"/>
-      <c r="J41" s="153"/>
-      <c r="K41" s="154">
+      <c r="I41" s="144"/>
+      <c r="J41" s="142"/>
+      <c r="K41" s="143">
         <f>K39+1</f>
         <v>6</v>
       </c>
@@ -38162,9 +38106,9 @@
         <v>85</v>
       </c>
       <c r="G42" s="111"/>
-      <c r="I42" s="155"/>
-      <c r="J42" s="153"/>
-      <c r="K42" s="154">
+      <c r="I42" s="144"/>
+      <c r="J42" s="142"/>
+      <c r="K42" s="143">
         <f>K41+1</f>
         <v>7</v>
       </c>
@@ -38213,9 +38157,9 @@
       <c r="H43" t="s">
         <v>186</v>
       </c>
-      <c r="I43" s="155"/>
-      <c r="J43" s="153"/>
-      <c r="K43" s="154">
+      <c r="I43" s="144"/>
+      <c r="J43" s="142"/>
+      <c r="K43" s="143">
         <f>K42+1</f>
         <v>8</v>
       </c>
@@ -38261,9 +38205,9 @@
         <v>85</v>
       </c>
       <c r="G44" s="107"/>
-      <c r="I44" s="155"/>
-      <c r="J44" s="153"/>
-      <c r="K44" s="154">
+      <c r="I44" s="144"/>
+      <c r="J44" s="142"/>
+      <c r="K44" s="143">
         <f>K43+1</f>
         <v>9</v>
       </c>
@@ -38309,9 +38253,9 @@
         <v>85</v>
       </c>
       <c r="G45" s="107"/>
-      <c r="I45" s="155"/>
-      <c r="J45" s="153"/>
-      <c r="K45" s="154">
+      <c r="I45" s="144"/>
+      <c r="J45" s="142"/>
+      <c r="K45" s="143">
         <f>K44+1</f>
         <v>10</v>
       </c>
@@ -38354,9 +38298,9 @@
         <v>85</v>
       </c>
       <c r="G46" s="111"/>
-      <c r="I46" s="155"/>
-      <c r="J46" s="153"/>
-      <c r="K46" s="154"/>
+      <c r="I46" s="144"/>
+      <c r="J46" s="142"/>
+      <c r="K46" s="143"/>
       <c r="L46" s="103" t="s">
         <v>182</v>
       </c>
@@ -38399,9 +38343,9 @@
       <c r="H47" t="s">
         <v>303</v>
       </c>
-      <c r="I47" s="155"/>
-      <c r="J47" s="153"/>
-      <c r="K47" s="154">
+      <c r="I47" s="144"/>
+      <c r="J47" s="142"/>
+      <c r="K47" s="143">
         <f>K45+1</f>
         <v>11</v>
       </c>
@@ -38440,9 +38384,9 @@
         <f t="shared" ref="G48:G53" ca="1" si="1">(F48-E48)/E48</f>
         <v>-1.1842378929335003E-16</v>
       </c>
-      <c r="I48" s="152"/>
-      <c r="J48" s="153"/>
-      <c r="K48" s="154"/>
+      <c r="I48" s="141"/>
+      <c r="J48" s="142"/>
+      <c r="K48" s="143"/>
       <c r="L48" s="105" t="s">
         <v>180</v>
       </c>
@@ -38489,9 +38433,9 @@
       <c r="H49" t="s">
         <v>316</v>
       </c>
-      <c r="I49" s="155"/>
-      <c r="J49" s="153"/>
-      <c r="K49" s="154"/>
+      <c r="I49" s="144"/>
+      <c r="J49" s="142"/>
+      <c r="K49" s="143"/>
       <c r="L49" s="103" t="s">
         <v>178</v>
       </c>
@@ -38535,9 +38479,9 @@
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="I50" s="155"/>
-      <c r="J50" s="153"/>
-      <c r="K50" s="154"/>
+      <c r="I50" s="144"/>
+      <c r="J50" s="142"/>
+      <c r="K50" s="143"/>
       <c r="L50" s="103" t="s">
         <v>92</v>
       </c>
@@ -38581,9 +38525,9 @@
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="I51" s="155"/>
-      <c r="J51" s="153"/>
-      <c r="K51" s="154"/>
+      <c r="I51" s="144"/>
+      <c r="J51" s="142"/>
+      <c r="K51" s="143"/>
       <c r="L51" s="103" t="s">
         <v>177</v>
       </c>
@@ -38624,15 +38568,15 @@
       </c>
       <c r="F52" s="109" cm="1">
         <f t="array" aca="1" ref="F52" ca="1">INDIRECT(sheet_name&amp;"!gap.k_mean")</f>
-        <v>0.28799999999999998</v>
+        <v>0.28773533056547312</v>
       </c>
       <c r="G52" s="118">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1983641357759886E-4</v>
-      </c>
-      <c r="I52" s="155"/>
-      <c r="J52" s="153"/>
-      <c r="K52" s="154">
+        <v>1.9292434864416651E-16</v>
+      </c>
+      <c r="I52" s="144"/>
+      <c r="J52" s="142"/>
+      <c r="K52" s="143">
         <f>K47+1</f>
         <v>12</v>
       </c>
@@ -38676,15 +38620,15 @@
       </c>
       <c r="F53" s="109" cm="1">
         <f t="array" aca="1" ref="F53" ca="1">INDIRECT(sheet_name&amp;"!gap.COV")</f>
-        <v>1.216</v>
+        <v>1.2162355202035973</v>
       </c>
       <c r="G53" s="118">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.9364687158461775E-4</v>
-      </c>
-      <c r="I53" s="155"/>
-      <c r="J53" s="153"/>
-      <c r="K53" s="154">
+        <v>-1.825671107581705E-16</v>
+      </c>
+      <c r="I53" s="144"/>
+      <c r="J53" s="142"/>
+      <c r="K53" s="143">
         <f>K52+1</f>
         <v>13</v>
       </c>
@@ -38727,9 +38671,9 @@
         <v>85</v>
       </c>
       <c r="G54" s="109"/>
-      <c r="I54" s="155"/>
-      <c r="J54" s="153"/>
-      <c r="K54" s="154"/>
+      <c r="I54" s="144"/>
+      <c r="J54" s="142"/>
+      <c r="K54" s="143"/>
       <c r="L54" s="103" t="s">
         <v>173</v>
       </c>
@@ -38772,9 +38716,9 @@
         <v>85</v>
       </c>
       <c r="G55" s="109"/>
-      <c r="I55" s="155"/>
-      <c r="J55" s="153"/>
-      <c r="K55" s="154">
+      <c r="I55" s="144"/>
+      <c r="J55" s="142"/>
+      <c r="K55" s="143">
         <f>K53+1</f>
         <v>14</v>
       </c>
@@ -38820,9 +38764,9 @@
         <v>85</v>
       </c>
       <c r="G56" s="109"/>
-      <c r="I56" s="155"/>
-      <c r="J56" s="153"/>
-      <c r="K56" s="154">
+      <c r="I56" s="144"/>
+      <c r="J56" s="142"/>
+      <c r="K56" s="143">
         <f>K55+1</f>
         <v>15</v>
       </c>
@@ -38866,9 +38810,9 @@
         <v>85</v>
       </c>
       <c r="G57" s="109"/>
-      <c r="I57" s="152"/>
-      <c r="J57" s="153"/>
-      <c r="K57" s="154">
+      <c r="I57" s="141"/>
+      <c r="J57" s="142"/>
+      <c r="K57" s="143">
         <f>K56+1</f>
         <v>16</v>
       </c>
@@ -38910,9 +38854,9 @@
         <v>85</v>
       </c>
       <c r="G58" s="109"/>
-      <c r="I58" s="152"/>
-      <c r="J58" s="153"/>
-      <c r="K58" s="154">
+      <c r="I58" s="141"/>
+      <c r="J58" s="142"/>
+      <c r="K58" s="143">
         <f>K57+1</f>
         <v>17</v>
       </c>
@@ -38954,9 +38898,9 @@
         <v>85</v>
       </c>
       <c r="G59" s="109"/>
-      <c r="I59" s="155"/>
-      <c r="J59" s="153"/>
-      <c r="K59" s="154">
+      <c r="I59" s="144"/>
+      <c r="J59" s="142"/>
+      <c r="K59" s="143">
         <f>K58+1</f>
         <v>18</v>
       </c>
@@ -39004,9 +38948,9 @@
         <f t="shared" ref="G60:G61" ca="1" si="2">(F60-E60)/E60</f>
         <v>6.3367559145939581E-16</v>
       </c>
-      <c r="I60" s="155"/>
-      <c r="J60" s="153"/>
-      <c r="K60" s="154">
+      <c r="I60" s="144"/>
+      <c r="J60" s="142"/>
+      <c r="K60" s="143">
         <f>K59+1</f>
         <v>19</v>
       </c>
@@ -39056,9 +39000,9 @@
       <c r="H61" t="s">
         <v>164</v>
       </c>
-      <c r="I61" s="155"/>
-      <c r="J61" s="153"/>
-      <c r="K61" s="154"/>
+      <c r="I61" s="144"/>
+      <c r="J61" s="142"/>
+      <c r="K61" s="143"/>
       <c r="L61" s="103" t="s">
         <v>165</v>
       </c>
@@ -39091,15 +39035,15 @@
         <v>163</v>
       </c>
       <c r="D62" s="103"/>
-      <c r="E62" s="132"/>
-      <c r="F62" s="132"/>
-      <c r="G62" s="132"/>
+      <c r="E62" s="128"/>
+      <c r="F62" s="128"/>
+      <c r="G62" s="128"/>
       <c r="H62" t="s">
         <v>162</v>
       </c>
-      <c r="I62" s="155"/>
-      <c r="J62" s="153"/>
-      <c r="K62" s="154">
+      <c r="I62" s="144"/>
+      <c r="J62" s="142"/>
+      <c r="K62" s="143">
         <f>K60+1</f>
         <v>20</v>
       </c>
@@ -39107,10 +39051,10 @@
         <v>163</v>
       </c>
       <c r="M62" s="103"/>
-      <c r="N62" s="132"/>
-      <c r="O62" s="132"/>
-      <c r="P62" s="132"/>
-      <c r="Q62" s="132"/>
+      <c r="N62" s="128"/>
+      <c r="O62" s="128"/>
+      <c r="P62" s="128"/>
+      <c r="Q62" s="128"/>
       <c r="R62" t="str">
         <f t="shared" si="0"/>
         <v>Gap shape formula</v>
@@ -39125,15 +39069,15 @@
         <v>161</v>
       </c>
       <c r="D63" s="103"/>
-      <c r="E63" s="132"/>
-      <c r="F63" s="132"/>
-      <c r="G63" s="132"/>
+      <c r="E63" s="128"/>
+      <c r="F63" s="128"/>
+      <c r="G63" s="128"/>
       <c r="H63" t="s">
         <v>160</v>
       </c>
-      <c r="I63" s="156"/>
-      <c r="J63" s="153"/>
-      <c r="K63" s="154">
+      <c r="I63" s="145"/>
+      <c r="J63" s="142"/>
+      <c r="K63" s="143">
         <f>K62+1</f>
         <v>21</v>
       </c>
@@ -39141,10 +39085,10 @@
         <v>161</v>
       </c>
       <c r="M63" s="103"/>
-      <c r="N63" s="132"/>
-      <c r="O63" s="132"/>
-      <c r="P63" s="132"/>
-      <c r="Q63" s="132"/>
+      <c r="N63" s="128"/>
+      <c r="O63" s="128"/>
+      <c r="P63" s="128"/>
+      <c r="Q63" s="128"/>
       <c r="R63" t="str">
         <f t="shared" si="0"/>
         <v>Stress range formula</v>
@@ -39162,9 +39106,9 @@
       <c r="E64" s="104"/>
       <c r="F64" s="104"/>
       <c r="G64" s="104"/>
-      <c r="I64" s="155"/>
-      <c r="J64" s="153"/>
-      <c r="K64" s="154">
+      <c r="I64" s="144"/>
+      <c r="J64" s="142"/>
+      <c r="K64" s="143">
         <f>K63+1</f>
         <v>22</v>
       </c>
@@ -39193,9 +39137,9 @@
       <c r="E65" s="104"/>
       <c r="F65" s="104"/>
       <c r="G65" s="104"/>
-      <c r="I65" s="155"/>
-      <c r="J65" s="153"/>
-      <c r="K65" s="154">
+      <c r="I65" s="144"/>
+      <c r="J65" s="142"/>
+      <c r="K65" s="143">
         <f>K64+1</f>
         <v>23</v>
       </c>
@@ -39221,15 +39165,15 @@
         <v>157</v>
       </c>
       <c r="D66" s="103"/>
-      <c r="E66" s="132"/>
-      <c r="F66" s="132"/>
-      <c r="G66" s="132"/>
+      <c r="E66" s="128"/>
+      <c r="F66" s="128"/>
+      <c r="G66" s="128"/>
       <c r="H66" t="s">
         <v>156</v>
       </c>
-      <c r="I66" s="155"/>
-      <c r="J66" s="153"/>
-      <c r="K66" s="154">
+      <c r="I66" s="144"/>
+      <c r="J66" s="142"/>
+      <c r="K66" s="143">
         <f>K65+1</f>
         <v>24</v>
       </c>
@@ -39237,10 +39181,10 @@
         <v>157</v>
       </c>
       <c r="M66" s="103"/>
-      <c r="N66" s="132"/>
-      <c r="O66" s="132"/>
-      <c r="P66" s="132"/>
-      <c r="Q66" s="132"/>
+      <c r="N66" s="128"/>
+      <c r="O66" s="128"/>
+      <c r="P66" s="128"/>
+      <c r="Q66" s="128"/>
       <c r="R66" t="str">
         <f t="shared" si="0"/>
         <v>Summarized formula for bolt force curve</v>
@@ -39588,11 +39532,11 @@
         <v>306</v>
       </c>
       <c r="D76" s="103"/>
-      <c r="E76" s="157" cm="1">
+      <c r="E76" s="146" cm="1">
         <f t="array" ref="E76">INDEX(N76:Q76,case_number)</f>
         <v>1.3453592978805262E-4</v>
       </c>
-      <c r="F76" s="157" cm="1">
+      <c r="F76" s="146" cm="1">
         <f t="array" aca="1" ref="F76" ca="1">INDIRECT(sheet_name&amp;"!Fs_coeff.tens.2")*1000</f>
         <v>1.3453194356000459E-4</v>
       </c>
@@ -39605,16 +39549,16 @@
         <v>306</v>
       </c>
       <c r="M76" s="103"/>
-      <c r="N76" s="161">
+      <c r="N76" s="150">
         <v>1.3453592978805262E-4</v>
       </c>
-      <c r="O76" s="161">
+      <c r="O76" s="150">
         <v>1.9479433966601163E-4</v>
       </c>
-      <c r="P76" s="161">
+      <c r="P76" s="150">
         <v>2.2483550066619361E-4</v>
       </c>
-      <c r="Q76" s="161">
+      <c r="Q76" s="150">
         <v>2.4370209971124864E-4</v>
       </c>
     </row>
@@ -39624,11 +39568,11 @@
         <v>305</v>
       </c>
       <c r="D77" s="103"/>
-      <c r="E77" s="157" cm="1">
+      <c r="E77" s="146" cm="1">
         <f t="array" ref="E77">INDEX(N77:Q77,case_number)</f>
         <v>0.15356565250189275</v>
       </c>
-      <c r="F77" s="157" cm="1">
+      <c r="F77" s="146" cm="1">
         <f t="array" aca="1" ref="F77" ca="1">INDIRECT(sheet_name&amp;"!Fs_coeff.tens.1")</f>
         <v>0.15355954292157073</v>
       </c>
@@ -39641,16 +39585,16 @@
         <v>305</v>
       </c>
       <c r="M77" s="103"/>
-      <c r="N77" s="161">
+      <c r="N77" s="150">
         <v>0.15356565250189275</v>
       </c>
-      <c r="O77" s="161">
+      <c r="O77" s="150">
         <v>0.16769709485155029</v>
       </c>
-      <c r="P77" s="161">
+      <c r="P77" s="150">
         <v>0.17112652766643241</v>
       </c>
-      <c r="Q77" s="161">
+      <c r="Q77" s="150">
         <v>0.17280832372040422</v>
       </c>
     </row>
@@ -39713,7 +39657,7 @@
         <f ca="1">(F79-E79)/E79</f>
         <v>2.7458237906393814E-7</v>
       </c>
-      <c r="I79" s="150"/>
+      <c r="I79" s="139"/>
       <c r="K79" s="106">
         <f>K66+1</f>
         <v>25</v>
@@ -39757,7 +39701,7 @@
         <v>85</v>
       </c>
       <c r="G80" s="111"/>
-      <c r="I80" s="149"/>
+      <c r="I80" s="138"/>
       <c r="K80" s="106"/>
       <c r="L80" s="103" t="s">
         <v>144</v>
@@ -39796,13 +39740,13 @@
       </c>
       <c r="F81" s="114" cm="1">
         <f t="array" aca="1" ref="F81" ca="1">INDIRECT(sheet_name&amp;"!I_tg")</f>
-        <v>123831110</v>
+        <v>123831110.42899768</v>
       </c>
       <c r="G81" s="118">
         <f t="shared" ref="G81:G83" ca="1" si="7">(F81-E81)/E81</f>
-        <v>-3.4643772397634438E-9</v>
-      </c>
-      <c r="I81" s="149"/>
+        <v>0</v>
+      </c>
+      <c r="I81" s="138"/>
       <c r="K81" s="106"/>
       <c r="L81" s="103" t="s">
         <v>142</v>
@@ -39810,16 +39754,16 @@
       <c r="M81" s="103" t="s">
         <v>273</v>
       </c>
-      <c r="N81" s="160">
+      <c r="N81" s="149">
         <v>123831110.42899768</v>
       </c>
-      <c r="O81" s="160">
+      <c r="O81" s="149">
         <v>123831110.42899768</v>
       </c>
-      <c r="P81" s="160">
+      <c r="P81" s="149">
         <v>123831110.42899768</v>
       </c>
-      <c r="Q81" s="160">
+      <c r="Q81" s="149">
         <v>123831110.42899768</v>
       </c>
       <c r="R81" t="str">
@@ -39841,13 +39785,13 @@
       </c>
       <c r="F82" s="111" cm="1">
         <f t="array" aca="1" ref="F82" ca="1">INDIRECT(sheet_name&amp;"!flange.A_cf")</f>
-        <v>87000</v>
+        <v>87000.000000000029</v>
       </c>
       <c r="G82" s="118">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I82" s="149"/>
+        <v>3.3452678685900808E-16</v>
+      </c>
+      <c r="I82" s="138"/>
       <c r="K82" s="106"/>
       <c r="L82" s="103" t="s">
         <v>148</v>
@@ -39886,13 +39830,13 @@
       </c>
       <c r="F83" s="114" cm="1">
         <f t="array" aca="1" ref="F83" ca="1">INDIRECT(sheet_name&amp;"!flange.I_cf")</f>
-        <v>290000000</v>
+        <v>290000000.00000006</v>
       </c>
       <c r="G83" s="118">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I83" s="149"/>
+        <v>2.0553325784617456E-16</v>
+      </c>
+      <c r="I83" s="138"/>
       <c r="K83" s="106"/>
       <c r="L83" s="103" t="s">
         <v>147</v>
@@ -39900,16 +39844,16 @@
       <c r="M83" s="103" t="s">
         <v>273</v>
       </c>
-      <c r="N83" s="160">
+      <c r="N83" s="149">
         <v>290000000</v>
       </c>
-      <c r="O83" s="160">
+      <c r="O83" s="149">
         <v>290000000</v>
       </c>
-      <c r="P83" s="160">
+      <c r="P83" s="149">
         <v>290000000</v>
       </c>
-      <c r="Q83" s="160">
+      <c r="Q83" s="149">
         <v>290000000</v>
       </c>
       <c r="R83" t="str">
@@ -39940,7 +39884,7 @@
         <f ca="1">(F84-E84)/E84</f>
         <v>2.7458237876438642E-7</v>
       </c>
-      <c r="I84" s="149"/>
+      <c r="I84" s="138"/>
       <c r="K84" s="106">
         <f>K79+1</f>
         <v>26</v>
@@ -39990,7 +39934,7 @@
       <c r="H85" t="s">
         <v>153</v>
       </c>
-      <c r="I85" s="149"/>
+      <c r="I85" s="138"/>
       <c r="K85" s="106">
         <f>K84+1</f>
         <v>27</v>
@@ -40032,16 +39976,16 @@
       </c>
       <c r="F86" s="111" cm="1">
         <f t="array" aca="1" ref="F86" ca="1">INDIRECT(sheet_name&amp;"!gap.k_shell")</f>
-        <v>5169.21</v>
+        <v>5169.2082946490964</v>
       </c>
       <c r="G86" s="118">
         <f ca="1">(F86-E86)/E86</f>
-        <v>3.2990562702105532E-7</v>
+        <v>0</v>
       </c>
       <c r="H86" t="s">
         <v>152</v>
       </c>
-      <c r="I86" s="149"/>
+      <c r="I86" s="138"/>
       <c r="K86" s="106"/>
       <c r="L86" s="103" t="s">
         <v>151</v>
@@ -40080,16 +40024,16 @@
       </c>
       <c r="F87" s="111" cm="1">
         <f t="array" aca="1" ref="F87" ca="1">INDIRECT(sheet_name&amp;"!gap.k_shell")</f>
-        <v>5169.21</v>
+        <v>5169.2082946490964</v>
       </c>
       <c r="G87" s="118">
         <f ca="1">(F87-E87)/E87</f>
-        <v>3.2990562702105532E-7</v>
+        <v>0</v>
       </c>
       <c r="H87" t="s">
         <v>150</v>
       </c>
-      <c r="I87" s="149"/>
+      <c r="I87" s="138"/>
       <c r="K87" s="106"/>
       <c r="L87" s="103" t="s">
         <v>151</v>
@@ -40137,7 +40081,7 @@
         <f ca="1">(F88-E88)/E88</f>
         <v>0</v>
       </c>
-      <c r="I88" s="149"/>
+      <c r="I88" s="138"/>
       <c r="K88" s="106">
         <f>K85+1</f>
         <v>28</v>
@@ -40182,13 +40126,13 @@
       </c>
       <c r="F89" s="107" cm="1">
         <f t="array" aca="1" ref="F89" ca="1">INDIRECT(sheet_name&amp;"!gap.k_fl")</f>
-        <v>1483.8</v>
+        <v>1483.8038863767938</v>
       </c>
       <c r="G89" s="118">
         <f ca="1">(F89-E89)/E89</f>
-        <v>-1.3880405217153795E-6</v>
-      </c>
-      <c r="I89" s="149"/>
+        <v>1.2311611223035349E-6</v>
+      </c>
+      <c r="I89" s="138"/>
       <c r="K89" s="106">
         <f>K88+1</f>
         <v>29</v>
@@ -40238,7 +40182,7 @@
       <c r="H90" t="s">
         <v>302</v>
       </c>
-      <c r="I90" s="150"/>
+      <c r="I90" s="139"/>
       <c r="K90" s="106">
         <f>K89+1</f>
         <v>30</v>
@@ -40288,7 +40232,7 @@
       <c r="H91" t="s">
         <v>302</v>
       </c>
-      <c r="I91" s="149"/>
+      <c r="I91" s="138"/>
       <c r="K91" s="106">
         <f>K90+1</f>
         <v>31</v>
@@ -40336,7 +40280,7 @@
         <f>"Inclination used: "&amp;E92&amp;"deg"</f>
         <v>Inclination used: 0deg</v>
       </c>
-      <c r="I92" s="150"/>
+      <c r="I92" s="139"/>
       <c r="K92" s="106"/>
       <c r="L92" s="105" t="s">
         <v>140</v>
@@ -40380,7 +40324,7 @@
         <v>85</v>
       </c>
       <c r="G93" s="107"/>
-      <c r="I93" s="150"/>
+      <c r="I93" s="139"/>
       <c r="K93" s="106">
         <f>K91+1</f>
         <v>32</v>
@@ -40427,7 +40371,7 @@
         <v>85</v>
       </c>
       <c r="G94" s="118"/>
-      <c r="I94" s="149"/>
+      <c r="I94" s="138"/>
       <c r="K94" s="106">
         <f>K93+1</f>
         <v>33</v>
@@ -40481,7 +40425,7 @@
       <c r="H95" t="s">
         <v>303</v>
       </c>
-      <c r="I95" s="149"/>
+      <c r="I95" s="138"/>
       <c r="K95" s="106">
         <f>K94+1</f>
         <v>34</v>
@@ -40531,7 +40475,7 @@
       <c r="H96" t="s">
         <v>302</v>
       </c>
-      <c r="I96" s="149"/>
+      <c r="I96" s="138"/>
       <c r="K96" s="106">
         <f>K95+1</f>
         <v>35</v>
@@ -40582,7 +40526,7 @@
         <f ca="1">(F97-E97)/E97</f>
         <v>2.1271829001672139E-5</v>
       </c>
-      <c r="I97" s="150"/>
+      <c r="I97" s="139"/>
       <c r="K97" s="106">
         <f>K96+1</f>
         <v>36</v>
@@ -40626,7 +40570,7 @@
         <v>85</v>
       </c>
       <c r="G98" s="118"/>
-      <c r="I98" s="150"/>
+      <c r="I98" s="139"/>
       <c r="K98" s="106"/>
       <c r="L98" s="105" t="s">
         <v>272</v>
@@ -40668,13 +40612,13 @@
       </c>
       <c r="F99" s="107" cm="1">
         <f t="array" aca="1" ref="F99" ca="1">INDIRECT(sheet_name&amp;"!k_seg")</f>
-        <v>10244.9653</v>
+        <v>10244.96531616569</v>
       </c>
       <c r="G99" s="118">
         <f ca="1">(F99-E99)/E99</f>
-        <v>-3.5887366781369556E-5</v>
-      </c>
-      <c r="I99" s="149"/>
+        <v>-3.5885788922463456E-5</v>
+      </c>
+      <c r="I99" s="138"/>
       <c r="K99" s="106">
         <f>K97+1</f>
         <v>37</v>
@@ -40725,7 +40669,7 @@
         <f ca="1">(F100-E100)/E100</f>
         <v>1.2864224446373524E-4</v>
       </c>
-      <c r="I100" s="149"/>
+      <c r="I100" s="138"/>
       <c r="K100" s="106">
         <f>K99+1</f>
         <v>38</v>
@@ -40770,16 +40714,16 @@
       </c>
       <c r="F101" s="109" cm="1">
         <f t="array" aca="1" ref="F101" ca="1">INDIRECT(sheet_name&amp;"!u")</f>
-        <v>0.41399999999999998</v>
+        <v>0.41432340368180404</v>
       </c>
       <c r="G101" s="118">
         <f ca="1">(F101-E101)/E101</f>
-        <v>-7.4511390434827925E-4</v>
+        <v>3.5472349816039453E-5</v>
       </c>
       <c r="H101" t="s">
         <v>303</v>
       </c>
-      <c r="I101" s="149"/>
+      <c r="I101" s="138"/>
       <c r="K101" s="106">
         <f>K100+1</f>
         <v>39</v>
@@ -40827,7 +40771,7 @@
       <c r="H102" t="s">
         <v>302</v>
       </c>
-      <c r="I102" s="149"/>
+      <c r="I102" s="138"/>
       <c r="K102" s="106">
         <f>K101+1</f>
         <v>40</v>
@@ -40871,7 +40815,7 @@
         <v>85</v>
       </c>
       <c r="G103" s="110"/>
-      <c r="I103" s="149"/>
+      <c r="I103" s="138"/>
       <c r="K103" s="106"/>
       <c r="L103" s="103" t="s">
         <v>132</v>
@@ -40919,7 +40863,7 @@
         <f ca="1">(F104-E104)/E104</f>
         <v>0</v>
       </c>
-      <c r="I104" s="150"/>
+      <c r="I104" s="139"/>
       <c r="K104" s="106">
         <f>K102+1</f>
         <v>41</v>
@@ -41230,9 +41174,9 @@
       <c r="D111" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="E111" s="132"/>
-      <c r="F111" s="132"/>
-      <c r="G111" s="132"/>
+      <c r="E111" s="128"/>
+      <c r="F111" s="128"/>
+      <c r="G111" s="128"/>
       <c r="H111" t="s">
         <v>271</v>
       </c>
@@ -41247,10 +41191,10 @@
       <c r="M111" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N111" s="132"/>
-      <c r="O111" s="132"/>
-      <c r="P111" s="132"/>
-      <c r="Q111" s="132"/>
+      <c r="N111" s="128"/>
+      <c r="O111" s="128"/>
+      <c r="P111" s="128"/>
+      <c r="Q111" s="128"/>
       <c r="R111" t="str">
         <f t="shared" si="6"/>
         <v>Bending moment L-Flange as a function of external force Z</v>
@@ -41273,11 +41217,11 @@
       </c>
       <c r="F112" s="107" cm="1">
         <f t="array" aca="1" ref="F112" ca="1">INDIRECT(sheet_name&amp;"!a_star")</f>
-        <v>112.77695050276699</v>
+        <v>112.77695050276785</v>
       </c>
       <c r="G112" s="118">
         <f ca="1">(F112-E112)/E112</f>
-        <v>-7.6865186881076997E-15</v>
+        <v>-1.2600850308373279E-16</v>
       </c>
       <c r="I112" s="105"/>
       <c r="K112" s="106">
@@ -41366,9 +41310,9 @@
       <c r="D114" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="E114" s="132"/>
-      <c r="F114" s="132"/>
-      <c r="G114" s="132"/>
+      <c r="E114" s="128"/>
+      <c r="F114" s="128"/>
+      <c r="G114" s="128"/>
       <c r="H114" t="s">
         <v>267</v>
       </c>
@@ -41383,10 +41327,10 @@
       <c r="M114" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N114" s="132"/>
-      <c r="O114" s="132"/>
-      <c r="P114" s="132"/>
-      <c r="Q114" s="132"/>
+      <c r="N114" s="128"/>
+      <c r="O114" s="128"/>
+      <c r="P114" s="128"/>
+      <c r="Q114" s="128"/>
       <c r="R114" t="str">
         <f t="shared" si="6"/>
         <v>Bending moment for T-Flange as a function of external force Z</v>
@@ -41403,9 +41347,9 @@
       <c r="D115" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="E115" s="132"/>
-      <c r="F115" s="132"/>
-      <c r="G115" s="132"/>
+      <c r="E115" s="128"/>
+      <c r="F115" s="128"/>
+      <c r="G115" s="128"/>
       <c r="H115" t="s">
         <v>265</v>
       </c>
@@ -41420,10 +41364,10 @@
       <c r="M115" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N115" s="132"/>
-      <c r="O115" s="132"/>
-      <c r="P115" s="132"/>
-      <c r="Q115" s="132"/>
+      <c r="N115" s="128"/>
+      <c r="O115" s="128"/>
+      <c r="P115" s="128"/>
+      <c r="Q115" s="128"/>
       <c r="R115" t="str">
         <f t="shared" si="6"/>
         <v>Intermediate values as function of Z</v>
@@ -41440,9 +41384,9 @@
       <c r="D116" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="E116" s="132"/>
-      <c r="F116" s="132"/>
-      <c r="G116" s="132"/>
+      <c r="E116" s="128"/>
+      <c r="F116" s="128"/>
+      <c r="G116" s="128"/>
       <c r="H116" t="s">
         <v>265</v>
       </c>
@@ -41457,10 +41401,10 @@
       <c r="M116" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N116" s="132"/>
-      <c r="O116" s="132"/>
-      <c r="P116" s="132"/>
-      <c r="Q116" s="132"/>
+      <c r="N116" s="128"/>
+      <c r="O116" s="128"/>
+      <c r="P116" s="128"/>
+      <c r="Q116" s="128"/>
       <c r="R116" t="str">
         <f t="shared" si="6"/>
         <v>Intermediate values as function of Z</v>
@@ -41801,44 +41745,44 @@
       </c>
     </row>
     <row r="131" spans="14:17">
-      <c r="N131" s="160">
+      <c r="N131" s="149">
         <v>4.1905840717736343E-4</v>
       </c>
-      <c r="O131" s="160">
+      <c r="O131" s="149">
         <v>6.0675394176265703E-4</v>
       </c>
-      <c r="P131" s="160">
+      <c r="P131" s="149">
         <v>7.0032746593815128E-4</v>
       </c>
-      <c r="Q131" s="160">
+      <c r="Q131" s="149">
         <v>7.5909397505679655E-4</v>
       </c>
     </row>
     <row r="132" spans="14:17">
-      <c r="N132" s="160">
+      <c r="N132" s="149">
         <v>0.59744121614189982</v>
       </c>
-      <c r="O132" s="160">
+      <c r="O132" s="149">
         <v>0.73747814923545729</v>
       </c>
-      <c r="P132" s="160">
+      <c r="P132" s="149">
         <v>0.77884714204471928</v>
       </c>
-      <c r="Q132" s="160">
+      <c r="Q132" s="149">
         <v>0.79858284162159954</v>
       </c>
     </row>
     <row r="133" spans="14:17">
-      <c r="N133" s="160">
+      <c r="N133" s="149">
         <v>52.604437654353092</v>
       </c>
-      <c r="O133" s="160">
+      <c r="O133" s="149">
         <v>55.178267132717792</v>
       </c>
-      <c r="P133" s="160">
+      <c r="P133" s="149">
         <v>55.072891200019058</v>
       </c>
-      <c r="Q133" s="160">
+      <c r="Q133" s="149">
         <v>54.825458530511014</v>
       </c>
     </row>
@@ -41974,12 +41918,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -42236,17 +42179,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
+    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -42271,18 +42224,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
-    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
PolynomialLFlangeSegment: debugged calculation of tilt neutralization force
</commit_message>
<xml_diff>
--- a/tests/validation/BnB_ReferenceFlange-Results-ShapeFactor-1.2.xlsx
+++ b/tests/validation/BnB_ReferenceFlange-Results-ShapeFactor-1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelloB\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\tests\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F14A29-14B3-47D2-B04A-AE190BAC6E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C0025C-04D0-4CDA-A378-104D612A047B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-9165" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
   </bookViews>
@@ -339,6 +339,10 @@
     <definedName name="u_tol" localSheetId="0">Gap30deg!$J$127</definedName>
     <definedName name="u_tol" localSheetId="1">Gap60deg!$J$127</definedName>
     <definedName name="u_tol" localSheetId="2">Gap90deg!$J$127</definedName>
+    <definedName name="Z_2_td" localSheetId="3">Gap120deg!$J$146</definedName>
+    <definedName name="Z_2_td" localSheetId="0">Gap30deg!$J$146</definedName>
+    <definedName name="Z_2_td" localSheetId="1">Gap60deg!$J$146</definedName>
+    <definedName name="Z_2_td" localSheetId="2">Gap90deg!$J$146</definedName>
     <definedName name="Z_dw" localSheetId="3">Gap120deg!$J$42</definedName>
     <definedName name="Z_dw" localSheetId="0">Gap30deg!$J$42</definedName>
     <definedName name="Z_dw" localSheetId="1">Gap60deg!$J$42</definedName>
@@ -347,10 +351,6 @@
     <definedName name="Z0" localSheetId="0">Gap30deg!$J$145</definedName>
     <definedName name="Z0" localSheetId="1">Gap60deg!$J$145</definedName>
     <definedName name="Z0" localSheetId="2">Gap90deg!$J$145</definedName>
-    <definedName name="Z2_tilde" localSheetId="3">Gap120deg!$J$146</definedName>
-    <definedName name="Z2_tilde" localSheetId="0">Gap30deg!$J$146</definedName>
-    <definedName name="Z2_tilde" localSheetId="1">Gap60deg!$J$146</definedName>
-    <definedName name="Z2_tilde" localSheetId="2">Gap90deg!$J$146</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="autoNoTable"/>
   <extLst>
@@ -395,7 +395,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="346">
   <si>
     <t>u</t>
   </si>
@@ -3774,6 +3774,317 @@
       <t xml:space="preserve"> =</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>dw</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Z</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s,T,low</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s,T,high</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s,T</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2,M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1,M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0,M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Value at </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>dw</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Value at </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>dw</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Z</t>
+    </r>
+  </si>
+  <si>
+    <t>Polynomial coefficients for bending moment</t>
+  </si>
+  <si>
+    <t>Note that these don't provide an exact match to</t>
+  </si>
+  <si>
+    <t>the interpolated values, but usually good enough</t>
+  </si>
 </sst>
 </file>
 
@@ -3791,12 +4102,19 @@
     <numFmt numFmtId="172" formatCode="0.000000"/>
     <numFmt numFmtId="173" formatCode="0.00000000000000000000"/>
   </numFmts>
-  <fonts count="60">
+  <fonts count="64">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4201,6 +4519,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="2"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -4592,325 +4930,328 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="41" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="40" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="3" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="18" fillId="3" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="23" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="24" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="3" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="10" fillId="3" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="29" fillId="6" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="30" fillId="6" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="9" fillId="3" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="10" fillId="3" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="4" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="37" fillId="4" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -4931,7 +5272,7 @@
     <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -4941,68 +5282,65 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="4" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="37" fillId="4" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="4" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="40" fillId="4" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="39" fillId="4" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="40" fillId="4" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="37" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="40" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5013,20 +5351,23 @@
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="172" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="3" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="3" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -5036,68 +5377,70 @@
     <xf numFmtId="171" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="7" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="8" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{441ACF27-160B-4F68-B601-75E0F5333046}"/>
     <cellStyle name="Normal 2 2" xfId="4" xr:uid="{C1D30E0C-7C3D-4B1D-9133-FEEA7CD75A88}"/>
+    <cellStyle name="Normal 2 3" xfId="6" xr:uid="{B53E3B6D-8252-4B0F-BB8A-4F69B2AB4309}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{E743A38D-16A7-497B-BF78-6D533003511F}"/>
     <cellStyle name="Normal 3 2" xfId="5" xr:uid="{2FBB15B9-17A9-4CFA-8BD1-0C9FAB04D83A}"/>
+    <cellStyle name="Normal 3 3" xfId="7" xr:uid="{E7F3BA36-62F5-4014-9448-A14F8B1B99DD}"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Standard 2" xfId="8" xr:uid="{01EB1CCF-760D-42B9-8631-D2AD57BA2130}"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <font>
         <b/>
@@ -19593,8 +19936,8 @@
   <dimension ref="A1:DJ179"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J147" sqref="J147"/>
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J146" sqref="J146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -19639,32 +19982,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="159"/>
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="160" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -19680,12 +20023,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="B5" s="161"/>
+      <c r="C5" s="162"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="163"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -19693,12 +20036,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="B6" s="161"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="163"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -19706,12 +20049,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="B7" s="161"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="162"/>
+      <c r="E7" s="162"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="163"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -19719,12 +20062,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
+      <c r="B8" s="161"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="163"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -19732,12 +20075,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
+      <c r="B9" s="161"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="162"/>
+      <c r="E9" s="162"/>
+      <c r="F9" s="162"/>
+      <c r="G9" s="163"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -19785,102 +20128,102 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="155"/>
-      <c r="D13" s="154" t="s">
+      <c r="C13" s="164"/>
+      <c r="D13" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="154"/>
-      <c r="F13" s="154"/>
-      <c r="G13" s="154"/>
-      <c r="H13" s="154"/>
-      <c r="I13" s="154"/>
-      <c r="J13" s="154"/>
-      <c r="K13" s="154"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="166"/>
+      <c r="G13" s="166"/>
+      <c r="H13" s="166"/>
+      <c r="I13" s="166"/>
+      <c r="J13" s="166"/>
+      <c r="K13" s="166"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="155" t="s">
+      <c r="B14" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="155"/>
-      <c r="D14" s="154" t="s">
+      <c r="C14" s="164"/>
+      <c r="D14" s="166" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="154"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="154"/>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="154"/>
-      <c r="K14" s="154"/>
+      <c r="E14" s="166"/>
+      <c r="F14" s="166"/>
+      <c r="G14" s="166"/>
+      <c r="H14" s="166"/>
+      <c r="I14" s="166"/>
+      <c r="J14" s="166"/>
+      <c r="K14" s="166"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="155" t="s">
+      <c r="B15" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="155"/>
-      <c r="D15" s="154" t="s">
+      <c r="C15" s="164"/>
+      <c r="D15" s="166" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="154"/>
-      <c r="F15" s="154"/>
-      <c r="G15" s="154"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
-      <c r="K15" s="154"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="166"/>
+      <c r="G15" s="166"/>
+      <c r="H15" s="166"/>
+      <c r="I15" s="166"/>
+      <c r="J15" s="166"/>
+      <c r="K15" s="166"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="155" t="s">
+      <c r="B16" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="155"/>
-      <c r="D16" s="154" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="166" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 30° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
+      <c r="E16" s="166"/>
+      <c r="F16" s="166"/>
+      <c r="G16" s="166"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="166"/>
+      <c r="J16" s="166"/>
+      <c r="K16" s="166"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="155" t="s">
+      <c r="B17" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="155"/>
-      <c r="D17" s="153">
+      <c r="C17" s="164"/>
+      <c r="D17" s="167">
         <v>0.1</v>
       </c>
-      <c r="E17" s="154"/>
-      <c r="F17" s="154"/>
-      <c r="G17" s="154"/>
-      <c r="H17" s="154"/>
-      <c r="I17" s="154"/>
-      <c r="J17" s="154"/>
-      <c r="K17" s="154"/>
+      <c r="E17" s="166"/>
+      <c r="F17" s="166"/>
+      <c r="G17" s="166"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="166"/>
+      <c r="J17" s="166"/>
+      <c r="K17" s="166"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="155" t="s">
+      <c r="B18" s="164" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="155"/>
+      <c r="C18" s="164"/>
       <c r="D18" s="165">
         <v>45432</v>
       </c>
@@ -20078,16 +20421,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="156"/>
-      <c r="C28" s="157"/>
-      <c r="D28" s="157"/>
-      <c r="E28" s="157"/>
-      <c r="F28" s="157"/>
-      <c r="G28" s="157"/>
-      <c r="H28" s="157"/>
-      <c r="I28" s="157"/>
-      <c r="J28" s="157"/>
-      <c r="K28" s="158"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
+      <c r="K28" s="157"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -24026,6 +24369,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B18:C18"/>
@@ -24036,31 +24389,21 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B28:K28"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
-    <cfRule type="cellIs" dxfId="28" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="5" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K94">
-    <cfRule type="cellIs" dxfId="27" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="2" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K124">
-    <cfRule type="cellIs" dxfId="26" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="1" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
@@ -24086,7 +24429,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J147" sqref="J147"/>
+      <selection pane="bottomLeft" activeCell="J146" sqref="J146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -24131,32 +24474,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="159"/>
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="160" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -24172,12 +24515,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="B5" s="161"/>
+      <c r="C5" s="162"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="163"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -24185,12 +24528,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="B6" s="161"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="163"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -24198,12 +24541,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="B7" s="161"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="162"/>
+      <c r="E7" s="162"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="163"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -24211,12 +24554,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
+      <c r="B8" s="161"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="163"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -24224,12 +24567,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
+      <c r="B9" s="161"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="162"/>
+      <c r="E9" s="162"/>
+      <c r="F9" s="162"/>
+      <c r="G9" s="163"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -24277,106 +24620,106 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="155"/>
-      <c r="D13" s="154" t="str">
+      <c r="C13" s="164"/>
+      <c r="D13" s="166" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="154"/>
-      <c r="F13" s="154"/>
-      <c r="G13" s="154"/>
-      <c r="H13" s="154"/>
-      <c r="I13" s="154"/>
-      <c r="J13" s="154"/>
-      <c r="K13" s="154"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="166"/>
+      <c r="G13" s="166"/>
+      <c r="H13" s="166"/>
+      <c r="I13" s="166"/>
+      <c r="J13" s="166"/>
+      <c r="K13" s="166"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="155" t="s">
+      <c r="B14" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="155"/>
-      <c r="D14" s="154" t="str">
+      <c r="C14" s="164"/>
+      <c r="D14" s="166" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="154"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="154"/>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="154"/>
-      <c r="K14" s="154"/>
+      <c r="E14" s="166"/>
+      <c r="F14" s="166"/>
+      <c r="G14" s="166"/>
+      <c r="H14" s="166"/>
+      <c r="I14" s="166"/>
+      <c r="J14" s="166"/>
+      <c r="K14" s="166"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="155" t="s">
+      <c r="B15" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="155"/>
-      <c r="D15" s="154" t="str">
+      <c r="C15" s="164"/>
+      <c r="D15" s="166" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="154"/>
-      <c r="F15" s="154"/>
-      <c r="G15" s="154"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
-      <c r="K15" s="154"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="166"/>
+      <c r="G15" s="166"/>
+      <c r="H15" s="166"/>
+      <c r="I15" s="166"/>
+      <c r="J15" s="166"/>
+      <c r="K15" s="166"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="155" t="s">
+      <c r="B16" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="155"/>
-      <c r="D16" s="154" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="166" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 60° gap size ans shape factor 1.2</v>
       </c>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
+      <c r="E16" s="166"/>
+      <c r="F16" s="166"/>
+      <c r="G16" s="166"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="166"/>
+      <c r="J16" s="166"/>
+      <c r="K16" s="166"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="155" t="s">
+      <c r="B17" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="155"/>
-      <c r="D17" s="154">
+      <c r="C17" s="164"/>
+      <c r="D17" s="166">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="154"/>
-      <c r="F17" s="154"/>
-      <c r="G17" s="154"/>
-      <c r="H17" s="154"/>
-      <c r="I17" s="154"/>
-      <c r="J17" s="154"/>
-      <c r="K17" s="154"/>
+      <c r="E17" s="166"/>
+      <c r="F17" s="166"/>
+      <c r="G17" s="166"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="166"/>
+      <c r="J17" s="166"/>
+      <c r="K17" s="166"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="155" t="s">
+      <c r="B18" s="164" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="155"/>
+      <c r="C18" s="164"/>
       <c r="D18" s="165">
         <f>Gap30deg!D18</f>
         <v>45432</v>
@@ -24575,16 +24918,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="156"/>
-      <c r="C28" s="157"/>
-      <c r="D28" s="157"/>
-      <c r="E28" s="157"/>
-      <c r="F28" s="157"/>
-      <c r="G28" s="157"/>
-      <c r="H28" s="157"/>
-      <c r="I28" s="157"/>
-      <c r="J28" s="157"/>
-      <c r="K28" s="158"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
+      <c r="K28" s="157"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -28486,6 +28829,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -28499,28 +28849,21 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
-    <cfRule type="cellIs" dxfId="25" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="3" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K94">
-    <cfRule type="cellIs" dxfId="24" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="2" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K124">
-    <cfRule type="cellIs" dxfId="23" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="1" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
@@ -28546,7 +28889,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J147" sqref="J147"/>
+      <selection pane="bottomLeft" activeCell="J146" sqref="J146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -28591,32 +28934,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="159"/>
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="160" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -28632,12 +28975,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="B5" s="161"/>
+      <c r="C5" s="162"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="163"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -28645,12 +28988,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="B6" s="161"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="163"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -28658,12 +29001,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="B7" s="161"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="162"/>
+      <c r="E7" s="162"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="163"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -28671,12 +29014,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
+      <c r="B8" s="161"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="163"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -28684,12 +29027,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
+      <c r="B9" s="161"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="162"/>
+      <c r="E9" s="162"/>
+      <c r="F9" s="162"/>
+      <c r="G9" s="163"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -28737,106 +29080,106 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="155"/>
-      <c r="D13" s="154" t="str">
+      <c r="C13" s="164"/>
+      <c r="D13" s="166" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="154"/>
-      <c r="F13" s="154"/>
-      <c r="G13" s="154"/>
-      <c r="H13" s="154"/>
-      <c r="I13" s="154"/>
-      <c r="J13" s="154"/>
-      <c r="K13" s="154"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="166"/>
+      <c r="G13" s="166"/>
+      <c r="H13" s="166"/>
+      <c r="I13" s="166"/>
+      <c r="J13" s="166"/>
+      <c r="K13" s="166"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="155" t="s">
+      <c r="B14" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="155"/>
-      <c r="D14" s="154" t="str">
+      <c r="C14" s="164"/>
+      <c r="D14" s="166" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="154"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="154"/>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="154"/>
-      <c r="K14" s="154"/>
+      <c r="E14" s="166"/>
+      <c r="F14" s="166"/>
+      <c r="G14" s="166"/>
+      <c r="H14" s="166"/>
+      <c r="I14" s="166"/>
+      <c r="J14" s="166"/>
+      <c r="K14" s="166"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="155" t="s">
+      <c r="B15" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="155"/>
-      <c r="D15" s="154" t="str">
+      <c r="C15" s="164"/>
+      <c r="D15" s="166" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="154"/>
-      <c r="F15" s="154"/>
-      <c r="G15" s="154"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
-      <c r="K15" s="154"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="166"/>
+      <c r="G15" s="166"/>
+      <c r="H15" s="166"/>
+      <c r="I15" s="166"/>
+      <c r="J15" s="166"/>
+      <c r="K15" s="166"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="155" t="s">
+      <c r="B16" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="155"/>
-      <c r="D16" s="154" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="166" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 90° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
+      <c r="E16" s="166"/>
+      <c r="F16" s="166"/>
+      <c r="G16" s="166"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="166"/>
+      <c r="J16" s="166"/>
+      <c r="K16" s="166"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="155" t="s">
+      <c r="B17" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="155"/>
-      <c r="D17" s="154">
+      <c r="C17" s="164"/>
+      <c r="D17" s="166">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="154"/>
-      <c r="F17" s="154"/>
-      <c r="G17" s="154"/>
-      <c r="H17" s="154"/>
-      <c r="I17" s="154"/>
-      <c r="J17" s="154"/>
-      <c r="K17" s="154"/>
+      <c r="E17" s="166"/>
+      <c r="F17" s="166"/>
+      <c r="G17" s="166"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="166"/>
+      <c r="J17" s="166"/>
+      <c r="K17" s="166"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="155" t="s">
+      <c r="B18" s="164" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="155"/>
+      <c r="C18" s="164"/>
       <c r="D18" s="165">
         <f>Gap30deg!D18</f>
         <v>45432</v>
@@ -29035,16 +29378,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="156"/>
-      <c r="C28" s="157"/>
-      <c r="D28" s="157"/>
-      <c r="E28" s="157"/>
-      <c r="F28" s="157"/>
-      <c r="G28" s="157"/>
-      <c r="H28" s="157"/>
-      <c r="I28" s="157"/>
-      <c r="J28" s="157"/>
-      <c r="K28" s="158"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
+      <c r="K28" s="157"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -32946,6 +33289,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -32959,28 +33309,21 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
-    <cfRule type="cellIs" dxfId="22" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K94">
-    <cfRule type="cellIs" dxfId="21" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="2" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K124">
-    <cfRule type="cellIs" dxfId="20" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="1" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
@@ -33006,7 +33349,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J147" sqref="J147"/>
+      <selection pane="bottomLeft" activeCell="J146" sqref="J146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -33051,32 +33394,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="159"/>
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="160" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -33092,12 +33435,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="B5" s="161"/>
+      <c r="C5" s="162"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="163"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -33105,12 +33448,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="B6" s="161"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="163"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -33118,12 +33461,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="B7" s="161"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="162"/>
+      <c r="E7" s="162"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="163"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -33131,12 +33474,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
+      <c r="B8" s="161"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="163"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -33144,12 +33487,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
+      <c r="B9" s="161"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="162"/>
+      <c r="E9" s="162"/>
+      <c r="F9" s="162"/>
+      <c r="G9" s="163"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -33197,106 +33540,106 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="155"/>
-      <c r="D13" s="154" t="str">
+      <c r="C13" s="164"/>
+      <c r="D13" s="166" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="154"/>
-      <c r="F13" s="154"/>
-      <c r="G13" s="154"/>
-      <c r="H13" s="154"/>
-      <c r="I13" s="154"/>
-      <c r="J13" s="154"/>
-      <c r="K13" s="154"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="166"/>
+      <c r="G13" s="166"/>
+      <c r="H13" s="166"/>
+      <c r="I13" s="166"/>
+      <c r="J13" s="166"/>
+      <c r="K13" s="166"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="155" t="s">
+      <c r="B14" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="155"/>
-      <c r="D14" s="154" t="str">
+      <c r="C14" s="164"/>
+      <c r="D14" s="166" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="154"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="154"/>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="154"/>
-      <c r="K14" s="154"/>
+      <c r="E14" s="166"/>
+      <c r="F14" s="166"/>
+      <c r="G14" s="166"/>
+      <c r="H14" s="166"/>
+      <c r="I14" s="166"/>
+      <c r="J14" s="166"/>
+      <c r="K14" s="166"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="155" t="s">
+      <c r="B15" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="155"/>
-      <c r="D15" s="154" t="str">
+      <c r="C15" s="164"/>
+      <c r="D15" s="166" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="154"/>
-      <c r="F15" s="154"/>
-      <c r="G15" s="154"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
-      <c r="K15" s="154"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="166"/>
+      <c r="G15" s="166"/>
+      <c r="H15" s="166"/>
+      <c r="I15" s="166"/>
+      <c r="J15" s="166"/>
+      <c r="K15" s="166"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="155" t="s">
+      <c r="B16" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="155"/>
-      <c r="D16" s="154" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="166" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 120° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
+      <c r="E16" s="166"/>
+      <c r="F16" s="166"/>
+      <c r="G16" s="166"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="166"/>
+      <c r="J16" s="166"/>
+      <c r="K16" s="166"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="155" t="s">
+      <c r="B17" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="155"/>
-      <c r="D17" s="154">
+      <c r="C17" s="164"/>
+      <c r="D17" s="166">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="154"/>
-      <c r="F17" s="154"/>
-      <c r="G17" s="154"/>
-      <c r="H17" s="154"/>
-      <c r="I17" s="154"/>
-      <c r="J17" s="154"/>
-      <c r="K17" s="154"/>
+      <c r="E17" s="166"/>
+      <c r="F17" s="166"/>
+      <c r="G17" s="166"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="166"/>
+      <c r="J17" s="166"/>
+      <c r="K17" s="166"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="155" t="s">
+      <c r="B18" s="164" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="155"/>
+      <c r="C18" s="164"/>
       <c r="D18" s="165">
         <f>Gap30deg!D18</f>
         <v>45432</v>
@@ -33495,16 +33838,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="156"/>
-      <c r="C28" s="157"/>
-      <c r="D28" s="157"/>
-      <c r="E28" s="157"/>
-      <c r="F28" s="157"/>
-      <c r="G28" s="157"/>
-      <c r="H28" s="157"/>
-      <c r="I28" s="157"/>
-      <c r="J28" s="157"/>
-      <c r="K28" s="158"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
+      <c r="K28" s="157"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -37406,6 +37749,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -37419,28 +37769,21 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
-    <cfRule type="cellIs" dxfId="19" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="3" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K94">
-    <cfRule type="cellIs" dxfId="18" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="2" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K124">
-    <cfRule type="cellIs" dxfId="17" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="1" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
@@ -37462,8 +37805,8 @@
   <sheetPr codeName="Tabelle12"/>
   <dimension ref="B2:R133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G92" sqref="G92"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -39809,8 +40152,8 @@
         <f t="array" ref="E79">INDEX(N79:Q79,case_number)</f>
         <v>1244.3580111747735</v>
       </c>
-      <c r="F79" s="107" cm="1">
-        <f t="array" aca="1" ref="F79" ca="1">-INDIRECT(sheet_name&amp;"!DZ_gap")</f>
+      <c r="F79" s="107">
+        <f ca="1">F93-F92</f>
         <v>1244.3583528535567</v>
       </c>
       <c r="G79" s="118">
@@ -40484,8 +40827,9 @@
         <f t="array" ref="E93">INDEX(N93:Q93,case_number)</f>
         <v>1794.1541531878652</v>
       </c>
-      <c r="F93" s="107" t="s">
-        <v>85</v>
+      <c r="F93" s="107" cm="1">
+        <f t="array" aca="1" ref="F93" ca="1">-INDIRECT(sheet_name&amp;"!DZ_gap")</f>
+        <v>1244.3583528535567</v>
       </c>
       <c r="G93" s="107"/>
       <c r="I93" s="139"/>
@@ -40826,7 +41170,7 @@
         <v>823.89401242504141</v>
       </c>
       <c r="F100" s="111" cm="1">
-        <f t="array" aca="1" ref="F100" ca="1">ROUND(INDIRECT(sheet_name&amp;"!Z2_tilde"),0)</f>
+        <f t="array" aca="1" ref="F100" ca="1">ROUND(INDIRECT(sheet_name&amp;"!Z_2_td"),0)</f>
         <v>824</v>
       </c>
       <c r="G100" s="118">
@@ -41768,7 +42112,29 @@
         <v>(valid in case T-Flange is calculated)</v>
       </c>
     </row>
-    <row r="121" spans="2:18">
+    <row r="121" spans="2:18" ht="15.6">
+      <c r="C121" s="105" t="s">
+        <v>331</v>
+      </c>
+      <c r="D121" s="103" t="s">
+        <v>127</v>
+      </c>
+      <c r="E121" s="108" cm="1">
+        <f t="array" ref="E121">INDEX(N121:Q121,case_number)</f>
+        <v>-123.19166666666668</v>
+      </c>
+      <c r="F121" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="G121" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="L121" s="105" t="s">
+        <v>331</v>
+      </c>
+      <c r="M121" s="103" t="s">
+        <v>127</v>
+      </c>
       <c r="N121" s="109">
         <v>-123.19166666666668</v>
       </c>
@@ -41782,7 +42148,32 @@
         <v>-123.19166666666668</v>
       </c>
     </row>
-    <row r="122" spans="2:18">
+    <row r="122" spans="2:18" ht="16.2">
+      <c r="C122" s="153" t="s">
+        <v>332</v>
+      </c>
+      <c r="D122" s="103" t="s">
+        <v>120</v>
+      </c>
+      <c r="E122" s="108" cm="1">
+        <f t="array" ref="E122">INDEX(N122:Q122,case_number)</f>
+        <v>0</v>
+      </c>
+      <c r="F122" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="G122" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="H122" s="154" t="s">
+        <v>341</v>
+      </c>
+      <c r="L122" s="153" t="s">
+        <v>332</v>
+      </c>
+      <c r="M122" s="103" t="s">
+        <v>120</v>
+      </c>
       <c r="N122" s="113">
         <v>0</v>
       </c>
@@ -41795,8 +42186,36 @@
       <c r="Q122" s="113">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="2:18">
+      <c r="R122" s="154" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="123" spans="2:18" ht="16.2">
+      <c r="C123" s="153" t="s">
+        <v>333</v>
+      </c>
+      <c r="D123" s="103" t="s">
+        <v>120</v>
+      </c>
+      <c r="E123" s="108" cm="1">
+        <f t="array" ref="E123">INDEX(N123:Q123,case_number)</f>
+        <v>-40.182316327404109</v>
+      </c>
+      <c r="F123" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="G123" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="H123" s="154" t="s">
+        <v>341</v>
+      </c>
+      <c r="L123" s="153" t="s">
+        <v>333</v>
+      </c>
+      <c r="M123" s="103" t="s">
+        <v>120</v>
+      </c>
       <c r="N123" s="109">
         <v>-40.182316327404109</v>
       </c>
@@ -41809,8 +42228,36 @@
       <c r="Q123" s="109">
         <v>-87.818771136704058</v>
       </c>
-    </row>
-    <row r="124" spans="2:18">
+      <c r="R123" s="154" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="124" spans="2:18" ht="16.2">
+      <c r="C124" s="153" t="s">
+        <v>334</v>
+      </c>
+      <c r="D124" s="103" t="s">
+        <v>120</v>
+      </c>
+      <c r="E124" s="108" cm="1">
+        <f t="array" ref="E124">INDEX(N124:Q124,case_number)</f>
+        <v>0</v>
+      </c>
+      <c r="F124" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="G124" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="H124" s="154" t="s">
+        <v>341</v>
+      </c>
+      <c r="L124" s="153" t="s">
+        <v>334</v>
+      </c>
+      <c r="M124" s="103" t="s">
+        <v>120</v>
+      </c>
       <c r="N124" s="113">
         <v>0</v>
       </c>
@@ -41823,8 +42270,36 @@
       <c r="Q124" s="113">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="2:18">
+      <c r="R124" s="154" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="125" spans="2:18" ht="16.2">
+      <c r="C125" s="153" t="s">
+        <v>332</v>
+      </c>
+      <c r="D125" s="103" t="s">
+        <v>120</v>
+      </c>
+      <c r="E125" s="108" cm="1">
+        <f t="array" ref="E125">INDEX(N125:Q125,case_number)</f>
+        <v>1.3386781456392284E-2</v>
+      </c>
+      <c r="F125" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="G125" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="H125" s="154" t="s">
+        <v>342</v>
+      </c>
+      <c r="L125" s="153" t="s">
+        <v>332</v>
+      </c>
+      <c r="M125" s="103" t="s">
+        <v>120</v>
+      </c>
       <c r="N125" s="113">
         <v>1.3386781456392284E-2</v>
       </c>
@@ -41837,8 +42312,36 @@
       <c r="Q125" s="113">
         <v>1.2534578790321781E-2</v>
       </c>
-    </row>
-    <row r="126" spans="2:18">
+      <c r="R125" s="154" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="126" spans="2:18" ht="16.2">
+      <c r="C126" s="153" t="s">
+        <v>333</v>
+      </c>
+      <c r="D126" s="103" t="s">
+        <v>120</v>
+      </c>
+      <c r="E126" s="108" cm="1">
+        <f t="array" ref="E126">INDEX(N126:Q126,case_number)</f>
+        <v>-40.149725060359245</v>
+      </c>
+      <c r="F126" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="G126" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="H126" s="154" t="s">
+        <v>342</v>
+      </c>
+      <c r="L126" s="153" t="s">
+        <v>333</v>
+      </c>
+      <c r="M126" s="103" t="s">
+        <v>120</v>
+      </c>
       <c r="N126" s="109">
         <v>-40.149725060359245</v>
       </c>
@@ -41851,8 +42354,36 @@
       <c r="Q126" s="109">
         <v>-87.747542664001102</v>
       </c>
-    </row>
-    <row r="127" spans="2:18">
+      <c r="R126" s="154" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="127" spans="2:18" ht="16.2">
+      <c r="C127" s="153" t="s">
+        <v>334</v>
+      </c>
+      <c r="D127" s="103" t="s">
+        <v>120</v>
+      </c>
+      <c r="E127" s="108" cm="1">
+        <f t="array" ref="E127">INDEX(N127:Q127,case_number)</f>
+        <v>1.2346849851752828E-2</v>
+      </c>
+      <c r="F127" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="G127" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="H127" s="154" t="s">
+        <v>342</v>
+      </c>
+      <c r="L127" s="153" t="s">
+        <v>334</v>
+      </c>
+      <c r="M127" s="103" t="s">
+        <v>120</v>
+      </c>
       <c r="N127" s="113">
         <v>1.2346849851752828E-2</v>
       </c>
@@ -41865,8 +42396,33 @@
       <c r="Q127" s="113">
         <v>1.0262233004222632E-2</v>
       </c>
-    </row>
-    <row r="128" spans="2:18">
+      <c r="R127" s="154" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="128" spans="2:18" ht="16.2">
+      <c r="C128" s="153" t="s">
+        <v>335</v>
+      </c>
+      <c r="D128" s="103" t="s">
+        <v>120</v>
+      </c>
+      <c r="E128" s="108" cm="1">
+        <f t="array" ref="E128">INDEX(N128:Q128,case_number)</f>
+        <v>-14.685047887174937</v>
+      </c>
+      <c r="F128" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="G128" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="L128" s="153" t="s">
+        <v>335</v>
+      </c>
+      <c r="M128" s="103" t="s">
+        <v>120</v>
+      </c>
       <c r="N128" s="113">
         <v>-14.685047887174937</v>
       </c>
@@ -41880,7 +42436,29 @@
         <v>-32.094288667371821</v>
       </c>
     </row>
-    <row r="129" spans="14:17">
+    <row r="129" spans="3:18" ht="16.2">
+      <c r="C129" s="153" t="s">
+        <v>336</v>
+      </c>
+      <c r="D129" s="103" t="s">
+        <v>120</v>
+      </c>
+      <c r="E129" s="108" cm="1">
+        <f t="array" ref="E129">INDEX(N129:Q129,case_number)</f>
+        <v>2925.8132343674552</v>
+      </c>
+      <c r="F129" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="G129" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="L129" s="153" t="s">
+        <v>336</v>
+      </c>
+      <c r="M129" s="103" t="s">
+        <v>120</v>
+      </c>
       <c r="N129" s="113">
         <v>2925.8132343674552</v>
       </c>
@@ -41894,7 +42472,29 @@
         <v>3088.6803607244869</v>
       </c>
     </row>
-    <row r="130" spans="14:17">
+    <row r="130" spans="3:18" ht="16.2">
+      <c r="C130" s="153" t="s">
+        <v>337</v>
+      </c>
+      <c r="D130" s="103" t="s">
+        <v>120</v>
+      </c>
+      <c r="E130" s="108" cm="1">
+        <f t="array" ref="E130">INDEX(N130:Q130,case_number)</f>
+        <v>229.08386220142413</v>
+      </c>
+      <c r="F130" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="G130" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="L130" s="153" t="s">
+        <v>337</v>
+      </c>
+      <c r="M130" s="103" t="s">
+        <v>120</v>
+      </c>
       <c r="N130" s="113">
         <v>229.08386220142413</v>
       </c>
@@ -41908,7 +42508,26 @@
         <v>156.61950693641407</v>
       </c>
     </row>
-    <row r="131" spans="14:17">
+    <row r="131" spans="3:18" ht="15.6">
+      <c r="C131" s="112" t="s">
+        <v>338</v>
+      </c>
+      <c r="E131" s="108" cm="1">
+        <f t="array" ref="E131">INDEX(N131:Q131,case_number)</f>
+        <v>4.1905840717736343E-4</v>
+      </c>
+      <c r="F131" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="G131" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="H131" t="s">
+        <v>343</v>
+      </c>
+      <c r="L131" s="112" t="s">
+        <v>338</v>
+      </c>
       <c r="N131" s="149">
         <v>4.1905840717736343E-4</v>
       </c>
@@ -41921,8 +42540,30 @@
       <c r="Q131" s="149">
         <v>7.5909397505679655E-4</v>
       </c>
-    </row>
-    <row r="132" spans="14:17">
+      <c r="R131" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="132" spans="3:18" ht="15.6">
+      <c r="C132" s="112" t="s">
+        <v>339</v>
+      </c>
+      <c r="E132" s="108" cm="1">
+        <f t="array" ref="E132">INDEX(N132:Q132,case_number)</f>
+        <v>0.59744121614189982</v>
+      </c>
+      <c r="F132" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="G132" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="H132" t="s">
+        <v>344</v>
+      </c>
+      <c r="L132" s="112" t="s">
+        <v>339</v>
+      </c>
       <c r="N132" s="149">
         <v>0.59744121614189982</v>
       </c>
@@ -41935,8 +42576,30 @@
       <c r="Q132" s="149">
         <v>0.79858284162159954</v>
       </c>
-    </row>
-    <row r="133" spans="14:17">
+      <c r="R132" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="133" spans="3:18" ht="15.6">
+      <c r="C133" s="112" t="s">
+        <v>340</v>
+      </c>
+      <c r="E133" s="108" cm="1">
+        <f t="array" ref="E133">INDEX(N133:Q133,case_number)</f>
+        <v>52.604437654353092</v>
+      </c>
+      <c r="F133" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="G133" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="H133" t="s">
+        <v>345</v>
+      </c>
+      <c r="L133" s="112" t="s">
+        <v>340</v>
+      </c>
       <c r="N133" s="149">
         <v>52.604437654353092</v>
       </c>
@@ -41949,100 +42612,103 @@
       <c r="Q133" s="149">
         <v>54.825458530511014</v>
       </c>
+      <c r="R133" t="s">
+        <v>345</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G29:G31">
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="notBetween">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36:G38">
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="notBetween">
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48:G53">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="notBetween">
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G60:G61">
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="notBetween">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G67:G72">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="notBetween">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G76:G79">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="notBetween">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81:G84">
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="notBetween">
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G86:G89">
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="notBetween">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="notBetween">
+      <formula>-0.001</formula>
+      <formula>0.001</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G92">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G94:G95">
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="notBetween">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G97:G101">
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="notBetween">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G104">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="notBetween">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G106:G108">
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="notBetween">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G112:G113">
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="notBetween">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G117">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="notBetween">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G119">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="notBetween">
-      <formula>-0.001</formula>
-      <formula>0.001</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G92">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
@@ -42088,15 +42754,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004E5A98ECA1EC044BB77E0D7F6ADEF7BC" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="5e88349ac6f5efd4674595e2a92e1fa9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2278e7f3-5df8-4100-b836-5320443b7544" xmlns:ns4="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bde21b231255bb48ab8a6ec7dd561648" ns3:_="" ns4:_="">
     <xsd:import namespace="2278e7f3-5df8-4100-b836-5320443b7544"/>
@@ -42349,6 +43006,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -42358,14 +43024,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A7863D2-B6F1-4C67-B9E9-1F3A9276C4FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42380,6 +43038,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
PolynomialLFlangeSegment: tested gap shape and flange tilt
</commit_message>
<xml_diff>
--- a/tests/validation/BnB_ReferenceFlange-Results-ShapeFactor-1.2.xlsx
+++ b/tests/validation/BnB_ReferenceFlange-Results-ShapeFactor-1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelloB\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\tests\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6550611C-22F8-4217-9BFE-72617FDEF058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CDA859-7652-423F-8548-9E437AC1BDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-9165" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
+    <workbookView xWindow="-28920" yWindow="-9165" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Gap30deg" sheetId="2" r:id="rId1"/>
@@ -5435,6 +5435,24 @@
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -5453,26 +5471,8 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -19982,8 +19982,8 @@
   <dimension ref="A1:DJ180"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J149" sqref="J149"/>
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K86" sqref="K86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -20028,32 +20028,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="162"/>
-      <c r="C3" s="162"/>
-      <c r="D3" s="162"/>
-      <c r="E3" s="162"/>
-      <c r="F3" s="162"/>
-      <c r="G3" s="162"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="162"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="159"/>
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="160" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -20069,12 +20069,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="155"/>
-      <c r="C5" s="156"/>
-      <c r="D5" s="156"/>
-      <c r="E5" s="156"/>
-      <c r="F5" s="156"/>
-      <c r="G5" s="157"/>
+      <c r="B5" s="161"/>
+      <c r="C5" s="162"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="163"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -20082,12 +20082,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="155"/>
-      <c r="C6" s="156"/>
-      <c r="D6" s="156"/>
-      <c r="E6" s="156"/>
-      <c r="F6" s="156"/>
-      <c r="G6" s="157"/>
+      <c r="B6" s="161"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="163"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -20095,12 +20095,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="155"/>
-      <c r="C7" s="156"/>
-      <c r="D7" s="156"/>
-      <c r="E7" s="156"/>
-      <c r="F7" s="156"/>
-      <c r="G7" s="157"/>
+      <c r="B7" s="161"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="162"/>
+      <c r="E7" s="162"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="163"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -20108,12 +20108,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="155"/>
-      <c r="C8" s="156"/>
-      <c r="D8" s="156"/>
-      <c r="E8" s="156"/>
-      <c r="F8" s="156"/>
-      <c r="G8" s="157"/>
+      <c r="B8" s="161"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="163"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -20121,12 +20121,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="155"/>
-      <c r="C9" s="156"/>
-      <c r="D9" s="156"/>
-      <c r="E9" s="156"/>
-      <c r="F9" s="156"/>
-      <c r="G9" s="157"/>
+      <c r="B9" s="161"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="162"/>
+      <c r="E9" s="162"/>
+      <c r="F9" s="162"/>
+      <c r="G9" s="163"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -20174,112 +20174,112 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="158" t="s">
+      <c r="B13" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="158"/>
-      <c r="D13" s="160" t="s">
+      <c r="C13" s="164"/>
+      <c r="D13" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="160"/>
-      <c r="F13" s="160"/>
-      <c r="G13" s="160"/>
-      <c r="H13" s="160"/>
-      <c r="I13" s="160"/>
-      <c r="J13" s="160"/>
-      <c r="K13" s="160"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="166"/>
+      <c r="G13" s="166"/>
+      <c r="H13" s="166"/>
+      <c r="I13" s="166"/>
+      <c r="J13" s="166"/>
+      <c r="K13" s="166"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="158" t="s">
+      <c r="B14" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="158"/>
-      <c r="D14" s="160" t="s">
+      <c r="C14" s="164"/>
+      <c r="D14" s="166" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="160"/>
-      <c r="F14" s="160"/>
-      <c r="G14" s="160"/>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="160"/>
-      <c r="K14" s="160"/>
+      <c r="E14" s="166"/>
+      <c r="F14" s="166"/>
+      <c r="G14" s="166"/>
+      <c r="H14" s="166"/>
+      <c r="I14" s="166"/>
+      <c r="J14" s="166"/>
+      <c r="K14" s="166"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="158" t="s">
+      <c r="B15" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="158"/>
-      <c r="D15" s="160" t="s">
+      <c r="C15" s="164"/>
+      <c r="D15" s="166" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="160"/>
-      <c r="F15" s="160"/>
-      <c r="G15" s="160"/>
-      <c r="H15" s="160"/>
-      <c r="I15" s="160"/>
-      <c r="J15" s="160"/>
-      <c r="K15" s="160"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="166"/>
+      <c r="G15" s="166"/>
+      <c r="H15" s="166"/>
+      <c r="I15" s="166"/>
+      <c r="J15" s="166"/>
+      <c r="K15" s="166"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="158" t="s">
+      <c r="B16" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="158"/>
-      <c r="D16" s="160" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="166" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 30° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="160"/>
-      <c r="F16" s="160"/>
-      <c r="G16" s="160"/>
-      <c r="H16" s="160"/>
-      <c r="I16" s="160"/>
-      <c r="J16" s="160"/>
-      <c r="K16" s="160"/>
+      <c r="E16" s="166"/>
+      <c r="F16" s="166"/>
+      <c r="G16" s="166"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="166"/>
+      <c r="J16" s="166"/>
+      <c r="K16" s="166"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="158" t="s">
+      <c r="B17" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="158"/>
-      <c r="D17" s="164">
+      <c r="C17" s="164"/>
+      <c r="D17" s="167">
         <v>0.1</v>
       </c>
-      <c r="E17" s="160"/>
-      <c r="F17" s="160"/>
-      <c r="G17" s="160"/>
-      <c r="H17" s="160"/>
-      <c r="I17" s="160"/>
-      <c r="J17" s="160"/>
-      <c r="K17" s="160"/>
+      <c r="E17" s="166"/>
+      <c r="F17" s="166"/>
+      <c r="G17" s="166"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="166"/>
+      <c r="J17" s="166"/>
+      <c r="K17" s="166"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="158" t="s">
+      <c r="B18" s="164" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="158"/>
-      <c r="D18" s="159">
+      <c r="C18" s="164"/>
+      <c r="D18" s="165">
         <v>45432</v>
       </c>
-      <c r="E18" s="159"/>
-      <c r="F18" s="159"/>
-      <c r="G18" s="159"/>
-      <c r="H18" s="159"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
-      <c r="K18" s="159"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="165"/>
+      <c r="G18" s="165"/>
+      <c r="H18" s="165"/>
+      <c r="I18" s="165"/>
+      <c r="J18" s="165"/>
+      <c r="K18" s="165"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -20467,16 +20467,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="165"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
-      <c r="H28" s="166"/>
-      <c r="I28" s="166"/>
-      <c r="J28" s="166"/>
-      <c r="K28" s="167"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
+      <c r="K28" s="157"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -24439,6 +24439,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B28:K28"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="B4:G4"/>
@@ -24455,10 +24459,6 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="27" priority="5" stopIfTrue="1" operator="between">
@@ -24498,8 +24498,8 @@
   <dimension ref="A1:DJ180"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J149" sqref="J149"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -24544,32 +24544,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="162"/>
-      <c r="C3" s="162"/>
-      <c r="D3" s="162"/>
-      <c r="E3" s="162"/>
-      <c r="F3" s="162"/>
-      <c r="G3" s="162"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="162"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="159"/>
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="160" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -24585,12 +24585,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="155"/>
-      <c r="C5" s="156"/>
-      <c r="D5" s="156"/>
-      <c r="E5" s="156"/>
-      <c r="F5" s="156"/>
-      <c r="G5" s="157"/>
+      <c r="B5" s="161"/>
+      <c r="C5" s="162"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="163"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -24598,12 +24598,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="155"/>
-      <c r="C6" s="156"/>
-      <c r="D6" s="156"/>
-      <c r="E6" s="156"/>
-      <c r="F6" s="156"/>
-      <c r="G6" s="157"/>
+      <c r="B6" s="161"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="163"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -24611,12 +24611,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="155"/>
-      <c r="C7" s="156"/>
-      <c r="D7" s="156"/>
-      <c r="E7" s="156"/>
-      <c r="F7" s="156"/>
-      <c r="G7" s="157"/>
+      <c r="B7" s="161"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="162"/>
+      <c r="E7" s="162"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="163"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -24624,12 +24624,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="155"/>
-      <c r="C8" s="156"/>
-      <c r="D8" s="156"/>
-      <c r="E8" s="156"/>
-      <c r="F8" s="156"/>
-      <c r="G8" s="157"/>
+      <c r="B8" s="161"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="163"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -24637,12 +24637,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="155"/>
-      <c r="C9" s="156"/>
-      <c r="D9" s="156"/>
-      <c r="E9" s="156"/>
-      <c r="F9" s="156"/>
-      <c r="G9" s="157"/>
+      <c r="B9" s="161"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="162"/>
+      <c r="E9" s="162"/>
+      <c r="F9" s="162"/>
+      <c r="G9" s="163"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -24690,117 +24690,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="158" t="s">
+      <c r="B13" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="158"/>
-      <c r="D13" s="160" t="str">
+      <c r="C13" s="164"/>
+      <c r="D13" s="166" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="160"/>
-      <c r="F13" s="160"/>
-      <c r="G13" s="160"/>
-      <c r="H13" s="160"/>
-      <c r="I13" s="160"/>
-      <c r="J13" s="160"/>
-      <c r="K13" s="160"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="166"/>
+      <c r="G13" s="166"/>
+      <c r="H13" s="166"/>
+      <c r="I13" s="166"/>
+      <c r="J13" s="166"/>
+      <c r="K13" s="166"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="158" t="s">
+      <c r="B14" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="158"/>
-      <c r="D14" s="160" t="str">
+      <c r="C14" s="164"/>
+      <c r="D14" s="166" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="160"/>
-      <c r="F14" s="160"/>
-      <c r="G14" s="160"/>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="160"/>
-      <c r="K14" s="160"/>
+      <c r="E14" s="166"/>
+      <c r="F14" s="166"/>
+      <c r="G14" s="166"/>
+      <c r="H14" s="166"/>
+      <c r="I14" s="166"/>
+      <c r="J14" s="166"/>
+      <c r="K14" s="166"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="158" t="s">
+      <c r="B15" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="158"/>
-      <c r="D15" s="160" t="str">
+      <c r="C15" s="164"/>
+      <c r="D15" s="166" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="160"/>
-      <c r="F15" s="160"/>
-      <c r="G15" s="160"/>
-      <c r="H15" s="160"/>
-      <c r="I15" s="160"/>
-      <c r="J15" s="160"/>
-      <c r="K15" s="160"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="166"/>
+      <c r="G15" s="166"/>
+      <c r="H15" s="166"/>
+      <c r="I15" s="166"/>
+      <c r="J15" s="166"/>
+      <c r="K15" s="166"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="158" t="s">
+      <c r="B16" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="158"/>
-      <c r="D16" s="160" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="166" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 60° gap size ans shape factor 1.2</v>
       </c>
-      <c r="E16" s="160"/>
-      <c r="F16" s="160"/>
-      <c r="G16" s="160"/>
-      <c r="H16" s="160"/>
-      <c r="I16" s="160"/>
-      <c r="J16" s="160"/>
-      <c r="K16" s="160"/>
+      <c r="E16" s="166"/>
+      <c r="F16" s="166"/>
+      <c r="G16" s="166"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="166"/>
+      <c r="J16" s="166"/>
+      <c r="K16" s="166"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="158" t="s">
+      <c r="B17" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="158"/>
-      <c r="D17" s="160">
+      <c r="C17" s="164"/>
+      <c r="D17" s="166">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="160"/>
-      <c r="F17" s="160"/>
-      <c r="G17" s="160"/>
-      <c r="H17" s="160"/>
-      <c r="I17" s="160"/>
-      <c r="J17" s="160"/>
-      <c r="K17" s="160"/>
+      <c r="E17" s="166"/>
+      <c r="F17" s="166"/>
+      <c r="G17" s="166"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="166"/>
+      <c r="J17" s="166"/>
+      <c r="K17" s="166"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="158" t="s">
+      <c r="B18" s="164" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="158"/>
-      <c r="D18" s="159">
+      <c r="C18" s="164"/>
+      <c r="D18" s="165">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="159"/>
-      <c r="F18" s="159"/>
-      <c r="G18" s="159"/>
-      <c r="H18" s="159"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
-      <c r="K18" s="159"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="165"/>
+      <c r="G18" s="165"/>
+      <c r="H18" s="165"/>
+      <c r="I18" s="165"/>
+      <c r="J18" s="165"/>
+      <c r="K18" s="165"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -24988,16 +24988,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="165"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
-      <c r="H28" s="166"/>
-      <c r="I28" s="166"/>
-      <c r="J28" s="166"/>
-      <c r="K28" s="167"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
+      <c r="K28" s="157"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -28923,6 +28923,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -28936,13 +28943,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="24" priority="3" stopIfTrue="1" operator="between">
@@ -28982,8 +28982,8 @@
   <dimension ref="A1:DJ180"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J149" sqref="J149"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K86" sqref="K86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -29028,32 +29028,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="162"/>
-      <c r="C3" s="162"/>
-      <c r="D3" s="162"/>
-      <c r="E3" s="162"/>
-      <c r="F3" s="162"/>
-      <c r="G3" s="162"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="162"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="159"/>
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="160" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -29069,12 +29069,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="155"/>
-      <c r="C5" s="156"/>
-      <c r="D5" s="156"/>
-      <c r="E5" s="156"/>
-      <c r="F5" s="156"/>
-      <c r="G5" s="157"/>
+      <c r="B5" s="161"/>
+      <c r="C5" s="162"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="163"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -29082,12 +29082,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="155"/>
-      <c r="C6" s="156"/>
-      <c r="D6" s="156"/>
-      <c r="E6" s="156"/>
-      <c r="F6" s="156"/>
-      <c r="G6" s="157"/>
+      <c r="B6" s="161"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="163"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -29095,12 +29095,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="155"/>
-      <c r="C7" s="156"/>
-      <c r="D7" s="156"/>
-      <c r="E7" s="156"/>
-      <c r="F7" s="156"/>
-      <c r="G7" s="157"/>
+      <c r="B7" s="161"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="162"/>
+      <c r="E7" s="162"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="163"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -29108,12 +29108,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="155"/>
-      <c r="C8" s="156"/>
-      <c r="D8" s="156"/>
-      <c r="E8" s="156"/>
-      <c r="F8" s="156"/>
-      <c r="G8" s="157"/>
+      <c r="B8" s="161"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="163"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -29121,12 +29121,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="155"/>
-      <c r="C9" s="156"/>
-      <c r="D9" s="156"/>
-      <c r="E9" s="156"/>
-      <c r="F9" s="156"/>
-      <c r="G9" s="157"/>
+      <c r="B9" s="161"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="162"/>
+      <c r="E9" s="162"/>
+      <c r="F9" s="162"/>
+      <c r="G9" s="163"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -29174,117 +29174,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="158" t="s">
+      <c r="B13" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="158"/>
-      <c r="D13" s="160" t="str">
+      <c r="C13" s="164"/>
+      <c r="D13" s="166" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="160"/>
-      <c r="F13" s="160"/>
-      <c r="G13" s="160"/>
-      <c r="H13" s="160"/>
-      <c r="I13" s="160"/>
-      <c r="J13" s="160"/>
-      <c r="K13" s="160"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="166"/>
+      <c r="G13" s="166"/>
+      <c r="H13" s="166"/>
+      <c r="I13" s="166"/>
+      <c r="J13" s="166"/>
+      <c r="K13" s="166"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="158" t="s">
+      <c r="B14" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="158"/>
-      <c r="D14" s="160" t="str">
+      <c r="C14" s="164"/>
+      <c r="D14" s="166" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="160"/>
-      <c r="F14" s="160"/>
-      <c r="G14" s="160"/>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="160"/>
-      <c r="K14" s="160"/>
+      <c r="E14" s="166"/>
+      <c r="F14" s="166"/>
+      <c r="G14" s="166"/>
+      <c r="H14" s="166"/>
+      <c r="I14" s="166"/>
+      <c r="J14" s="166"/>
+      <c r="K14" s="166"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="158" t="s">
+      <c r="B15" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="158"/>
-      <c r="D15" s="160" t="str">
+      <c r="C15" s="164"/>
+      <c r="D15" s="166" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="160"/>
-      <c r="F15" s="160"/>
-      <c r="G15" s="160"/>
-      <c r="H15" s="160"/>
-      <c r="I15" s="160"/>
-      <c r="J15" s="160"/>
-      <c r="K15" s="160"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="166"/>
+      <c r="G15" s="166"/>
+      <c r="H15" s="166"/>
+      <c r="I15" s="166"/>
+      <c r="J15" s="166"/>
+      <c r="K15" s="166"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="158" t="s">
+      <c r="B16" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="158"/>
-      <c r="D16" s="160" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="166" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 90° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="160"/>
-      <c r="F16" s="160"/>
-      <c r="G16" s="160"/>
-      <c r="H16" s="160"/>
-      <c r="I16" s="160"/>
-      <c r="J16" s="160"/>
-      <c r="K16" s="160"/>
+      <c r="E16" s="166"/>
+      <c r="F16" s="166"/>
+      <c r="G16" s="166"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="166"/>
+      <c r="J16" s="166"/>
+      <c r="K16" s="166"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="158" t="s">
+      <c r="B17" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="158"/>
-      <c r="D17" s="160">
+      <c r="C17" s="164"/>
+      <c r="D17" s="166">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="160"/>
-      <c r="F17" s="160"/>
-      <c r="G17" s="160"/>
-      <c r="H17" s="160"/>
-      <c r="I17" s="160"/>
-      <c r="J17" s="160"/>
-      <c r="K17" s="160"/>
+      <c r="E17" s="166"/>
+      <c r="F17" s="166"/>
+      <c r="G17" s="166"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="166"/>
+      <c r="J17" s="166"/>
+      <c r="K17" s="166"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="158" t="s">
+      <c r="B18" s="164" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="158"/>
-      <c r="D18" s="159">
+      <c r="C18" s="164"/>
+      <c r="D18" s="165">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="159"/>
-      <c r="F18" s="159"/>
-      <c r="G18" s="159"/>
-      <c r="H18" s="159"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
-      <c r="K18" s="159"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="165"/>
+      <c r="G18" s="165"/>
+      <c r="H18" s="165"/>
+      <c r="I18" s="165"/>
+      <c r="J18" s="165"/>
+      <c r="K18" s="165"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -29472,16 +29472,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="165"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
-      <c r="H28" s="166"/>
-      <c r="I28" s="166"/>
-      <c r="J28" s="166"/>
-      <c r="K28" s="167"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
+      <c r="K28" s="157"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -33407,6 +33407,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -33420,13 +33427,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="between">
@@ -33465,9 +33465,9 @@
   </sheetPr>
   <dimension ref="A1:DJ180"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J149" sqref="J149"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O117" sqref="O117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -33512,32 +33512,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="162"/>
-      <c r="C3" s="162"/>
-      <c r="D3" s="162"/>
-      <c r="E3" s="162"/>
-      <c r="F3" s="162"/>
-      <c r="G3" s="162"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="162"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="159"/>
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="160" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -33553,12 +33553,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="155"/>
-      <c r="C5" s="156"/>
-      <c r="D5" s="156"/>
-      <c r="E5" s="156"/>
-      <c r="F5" s="156"/>
-      <c r="G5" s="157"/>
+      <c r="B5" s="161"/>
+      <c r="C5" s="162"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="163"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -33566,12 +33566,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="155"/>
-      <c r="C6" s="156"/>
-      <c r="D6" s="156"/>
-      <c r="E6" s="156"/>
-      <c r="F6" s="156"/>
-      <c r="G6" s="157"/>
+      <c r="B6" s="161"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="163"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -33579,12 +33579,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="155"/>
-      <c r="C7" s="156"/>
-      <c r="D7" s="156"/>
-      <c r="E7" s="156"/>
-      <c r="F7" s="156"/>
-      <c r="G7" s="157"/>
+      <c r="B7" s="161"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="162"/>
+      <c r="E7" s="162"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="163"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -33592,12 +33592,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="155"/>
-      <c r="C8" s="156"/>
-      <c r="D8" s="156"/>
-      <c r="E8" s="156"/>
-      <c r="F8" s="156"/>
-      <c r="G8" s="157"/>
+      <c r="B8" s="161"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="163"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -33605,12 +33605,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="155"/>
-      <c r="C9" s="156"/>
-      <c r="D9" s="156"/>
-      <c r="E9" s="156"/>
-      <c r="F9" s="156"/>
-      <c r="G9" s="157"/>
+      <c r="B9" s="161"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="162"/>
+      <c r="E9" s="162"/>
+      <c r="F9" s="162"/>
+      <c r="G9" s="163"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -33658,117 +33658,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="158" t="s">
+      <c r="B13" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="158"/>
-      <c r="D13" s="160" t="str">
+      <c r="C13" s="164"/>
+      <c r="D13" s="166" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="160"/>
-      <c r="F13" s="160"/>
-      <c r="G13" s="160"/>
-      <c r="H13" s="160"/>
-      <c r="I13" s="160"/>
-      <c r="J13" s="160"/>
-      <c r="K13" s="160"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="166"/>
+      <c r="G13" s="166"/>
+      <c r="H13" s="166"/>
+      <c r="I13" s="166"/>
+      <c r="J13" s="166"/>
+      <c r="K13" s="166"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="158" t="s">
+      <c r="B14" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="158"/>
-      <c r="D14" s="160" t="str">
+      <c r="C14" s="164"/>
+      <c r="D14" s="166" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="160"/>
-      <c r="F14" s="160"/>
-      <c r="G14" s="160"/>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="160"/>
-      <c r="K14" s="160"/>
+      <c r="E14" s="166"/>
+      <c r="F14" s="166"/>
+      <c r="G14" s="166"/>
+      <c r="H14" s="166"/>
+      <c r="I14" s="166"/>
+      <c r="J14" s="166"/>
+      <c r="K14" s="166"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="158" t="s">
+      <c r="B15" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="158"/>
-      <c r="D15" s="160" t="str">
+      <c r="C15" s="164"/>
+      <c r="D15" s="166" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="160"/>
-      <c r="F15" s="160"/>
-      <c r="G15" s="160"/>
-      <c r="H15" s="160"/>
-      <c r="I15" s="160"/>
-      <c r="J15" s="160"/>
-      <c r="K15" s="160"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="166"/>
+      <c r="G15" s="166"/>
+      <c r="H15" s="166"/>
+      <c r="I15" s="166"/>
+      <c r="J15" s="166"/>
+      <c r="K15" s="166"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="158" t="s">
+      <c r="B16" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="158"/>
-      <c r="D16" s="160" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="166" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 120° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="160"/>
-      <c r="F16" s="160"/>
-      <c r="G16" s="160"/>
-      <c r="H16" s="160"/>
-      <c r="I16" s="160"/>
-      <c r="J16" s="160"/>
-      <c r="K16" s="160"/>
+      <c r="E16" s="166"/>
+      <c r="F16" s="166"/>
+      <c r="G16" s="166"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="166"/>
+      <c r="J16" s="166"/>
+      <c r="K16" s="166"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="158" t="s">
+      <c r="B17" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="158"/>
-      <c r="D17" s="160">
+      <c r="C17" s="164"/>
+      <c r="D17" s="166">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="160"/>
-      <c r="F17" s="160"/>
-      <c r="G17" s="160"/>
-      <c r="H17" s="160"/>
-      <c r="I17" s="160"/>
-      <c r="J17" s="160"/>
-      <c r="K17" s="160"/>
+      <c r="E17" s="166"/>
+      <c r="F17" s="166"/>
+      <c r="G17" s="166"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="166"/>
+      <c r="J17" s="166"/>
+      <c r="K17" s="166"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="158" t="s">
+      <c r="B18" s="164" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="158"/>
-      <c r="D18" s="159">
+      <c r="C18" s="164"/>
+      <c r="D18" s="165">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="159"/>
-      <c r="F18" s="159"/>
-      <c r="G18" s="159"/>
-      <c r="H18" s="159"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
-      <c r="K18" s="159"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="165"/>
+      <c r="G18" s="165"/>
+      <c r="H18" s="165"/>
+      <c r="I18" s="165"/>
+      <c r="J18" s="165"/>
+      <c r="K18" s="165"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -33956,16 +33956,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="165"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
-      <c r="H28" s="166"/>
-      <c r="I28" s="166"/>
-      <c r="J28" s="166"/>
-      <c r="K28" s="167"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
+      <c r="K28" s="157"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -37891,6 +37891,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -37904,13 +37911,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="18" priority="3" stopIfTrue="1" operator="between">
@@ -37947,7 +37947,7 @@
   <sheetPr codeName="Tabelle12"/>
   <dimension ref="B2:R133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
@@ -43149,20 +43149,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -43185,6 +43185,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -43199,12 +43207,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
PolynomialLFlangeSegment: shell_force_at_closed_gap now returns Z4, not delta-Z-total anymore
</commit_message>
<xml_diff>
--- a/tests/validation/BnB_ReferenceFlange-Results-ShapeFactor-1.2.xlsx
+++ b/tests/validation/BnB_ReferenceFlange-Results-ShapeFactor-1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelloB\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\tests\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CDA859-7652-423F-8548-9E437AC1BDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA686CF-34E0-4B28-BB14-4726E68542A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-9165" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
   </bookViews>
@@ -19983,7 +19983,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K86" sqref="K86"/>
+      <selection pane="bottomLeft" activeCell="J116" sqref="J116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -28923,13 +28923,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -28943,6 +28936,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="24" priority="3" stopIfTrue="1" operator="between">
@@ -33407,13 +33407,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -33427,6 +33420,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="between">
@@ -37891,13 +37891,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -37911,6 +37904,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="18" priority="3" stopIfTrue="1" operator="between">
@@ -37947,8 +37947,8 @@
   <sheetPr codeName="Tabelle12"/>
   <dimension ref="B2:R133"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F94" sqref="F94"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -37980,19 +37980,19 @@
     </row>
     <row r="21" spans="2:18" ht="18">
       <c r="G21" s="135">
-        <v>30</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="2:18">
       <c r="G22" s="136">
         <f>MATCH(gap_angle,N48:Q48,0)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:18">
       <c r="G23" s="136" t="str">
         <f>"Gap"&amp;gap_angle&amp;"deg"</f>
-        <v>Gap30deg</v>
+        <v>Gap120deg</v>
       </c>
     </row>
     <row r="25" spans="2:18">
@@ -39019,11 +39019,11 @@
       </c>
       <c r="E48" s="110" cm="1">
         <f t="array" ref="E48">INDEX(N48:Q48,case_number)</f>
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="F48" s="110" cm="1">
         <f t="array" aca="1" ref="F48" ca="1">INDIRECT(sheet_name&amp;"!gap.angle")</f>
-        <v>29.999999999999996</v>
+        <v>119.99999999999999</v>
       </c>
       <c r="G48" s="118">
         <f t="shared" ref="G48:G53" ca="1" si="1">(F48-E48)/E48</f>
@@ -39065,11 +39065,11 @@
       </c>
       <c r="E49" s="109" cm="1">
         <f t="array" ref="E49">INDEX(N49:Q49,case_number)</f>
-        <v>1.9634954084936207</v>
+        <v>7.8539816339744828</v>
       </c>
       <c r="F49" s="109" cm="1">
         <f t="array" aca="1" ref="F49" ca="1">INDIRECT(sheet_name&amp;"!gap.L")/1000</f>
-        <v>1.9634954084936205</v>
+        <v>7.8539816339744819</v>
       </c>
       <c r="G49" s="118">
         <f t="shared" ca="1" si="1"/>
@@ -39209,15 +39209,15 @@
       </c>
       <c r="E52" s="109" cm="1">
         <f t="array" ref="E52">INDEX(N52:Q52,case_number)</f>
-        <v>0.28773533056547307</v>
+        <v>2.1533230192475301</v>
       </c>
       <c r="F52" s="109" cm="1">
         <f t="array" aca="1" ref="F52" ca="1">INDIRECT(sheet_name&amp;"!gap.k_mean")</f>
-        <v>0.28773533056547312</v>
+        <v>2.1533230192475297</v>
       </c>
       <c r="G52" s="118">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9292434864416651E-16</v>
+        <v>-2.0623436701347657E-16</v>
       </c>
       <c r="I52" s="144"/>
       <c r="J52" s="142"/>
@@ -39261,15 +39261,15 @@
       </c>
       <c r="E53" s="109" cm="1">
         <f t="array" ref="E53">INDEX(N53:Q53,case_number)</f>
-        <v>1.2162355202035975</v>
+        <v>0.44426272750754409</v>
       </c>
       <c r="F53" s="109" cm="1">
         <f t="array" aca="1" ref="F53" ca="1">INDIRECT(sheet_name&amp;"!gap.COV")</f>
-        <v>1.2162355202035973</v>
+        <v>0.44426272750754392</v>
       </c>
       <c r="G53" s="118">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.825671107581705E-16</v>
+        <v>-3.7485353459219818E-16</v>
       </c>
       <c r="I53" s="144"/>
       <c r="J53" s="142"/>
@@ -39449,7 +39449,7 @@
       <c r="D57" s="103"/>
       <c r="E57" s="109" cm="1">
         <f t="array" ref="E57">INDEX(N57:Q57,case_number)</f>
-        <v>0.95286282352314688</v>
+        <v>0.42441366570439232</v>
       </c>
       <c r="F57" s="109" t="s">
         <v>85</v>
@@ -39493,7 +39493,7 @@
       <c r="D58" s="103"/>
       <c r="E58" s="109" cm="1">
         <f t="array" ref="E58">INDEX(N58:Q58,case_number)</f>
-        <v>-1.6996879926957522</v>
+        <v>0.67694875947348121</v>
       </c>
       <c r="F58" s="109" t="s">
         <v>85</v>
@@ -39537,7 +39537,7 @@
       <c r="D59" s="103"/>
       <c r="E59" s="109" cm="1">
         <f t="array" ref="E59">INDEX(N59:Q59,case_number)</f>
-        <v>-0.13232393428252798</v>
+        <v>1.3750667981906362</v>
       </c>
       <c r="F59" s="113" t="s">
         <v>85</v>
@@ -39583,15 +39583,15 @@
       </c>
       <c r="E60" s="109" cm="1">
         <f t="array" ref="E60">INDEX(N60:Q60,case_number)</f>
-        <v>0.87601845454409977</v>
+        <v>3.9552630780086151</v>
       </c>
       <c r="F60" s="109" cm="1">
         <f t="array" aca="1" ref="F60" ca="1">INDIRECT(sheet_name&amp;"!gap.h")</f>
-        <v>0.87601845454410032</v>
+        <v>3.9552630780086138</v>
       </c>
       <c r="G60" s="118">
         <f t="shared" ref="G60:G61" ca="1" si="2">(F60-E60)/E60</f>
-        <v>6.3367559145939581E-16</v>
+        <v>-3.3683413802678182E-16</v>
       </c>
       <c r="I60" s="144"/>
       <c r="J60" s="142"/>
@@ -39632,15 +39632,15 @@
       </c>
       <c r="E61" s="109" cm="1">
         <f t="array" ref="E61">INDEX(N61:Q61,case_number)</f>
-        <v>0.87601845454409977</v>
+        <v>3.9552630780086151</v>
       </c>
       <c r="F61" s="109" cm="1">
         <f t="array" aca="1" ref="F61" ca="1">INDIRECT(sheet_name&amp;"!gap.h")</f>
-        <v>0.87601845454410032</v>
+        <v>3.9552630780086138</v>
       </c>
       <c r="G61" s="118">
         <f t="shared" ca="1" si="2"/>
-        <v>6.3367559145939581E-16</v>
+        <v>-3.3683413802678182E-16</v>
       </c>
       <c r="H61" t="s">
         <v>164</v>
@@ -39925,15 +39925,15 @@
       </c>
       <c r="E69" s="108" cm="1">
         <f t="array" ref="E69">INDEX(N69:Q69,case_number)</f>
-        <v>2000.9202638759255</v>
+        <v>1541.2016094157079</v>
       </c>
       <c r="F69" s="108" cm="1">
         <f t="array" aca="1" ref="F69" ca="1">INDIRECT(sheet_name&amp;"!Point2.Z")</f>
-        <v>2000.9619972862092</v>
+        <v>1541.2066792348119</v>
       </c>
       <c r="G69" s="118">
         <f t="shared" ca="1" si="4"/>
-        <v>2.0857108120304573E-5</v>
+        <v>3.2895236242709198E-6</v>
       </c>
       <c r="K69" s="106"/>
       <c r="L69" s="103" t="s">
@@ -40005,15 +40005,15 @@
       </c>
       <c r="E71" s="107" cm="1">
         <f t="array" ref="E71">INDEX(N71:Q71,case_number)</f>
-        <v>251.14925721102841</v>
+        <v>114.91573803665135</v>
       </c>
       <c r="F71" s="107" cm="1">
         <f t="array" aca="1" ref="F71" ca="1">INDIRECT(sheet_name&amp;"!Point3.Z")</f>
-        <v>251.15459961508168</v>
+        <v>114.91611609263964</v>
       </c>
       <c r="G71" s="118">
         <f t="shared" ca="1" si="4"/>
-        <v>2.1271829001577241E-5</v>
+        <v>3.2898538942688651E-6</v>
       </c>
       <c r="K71" s="106"/>
       <c r="L71" s="103" t="s">
@@ -40045,15 +40045,15 @@
       </c>
       <c r="E72" s="107" cm="1">
         <f t="array" ref="E72">INDEX(N72:Q72,case_number)</f>
-        <v>2939.9421878185444</v>
+        <v>2916.677985871765</v>
       </c>
       <c r="F72" s="107" cm="1">
         <f t="array" aca="1" ref="F72" ca="1">INDIRECT(sheet_name&amp;"!Point3.Fs")</f>
-        <v>2939.9408906954832</v>
+        <v>2916.6766448801113</v>
       </c>
       <c r="G72" s="118">
         <f t="shared" ca="1" si="4"/>
-        <v>-4.4120699605041146E-7</v>
+        <v>-4.5976678268955551E-7</v>
       </c>
       <c r="K72" s="106"/>
       <c r="L72" s="103" t="s">
@@ -40083,7 +40083,7 @@
       <c r="D73" s="103"/>
       <c r="E73" s="107" cm="1">
         <f t="array" ref="E73">INDEX(N73:Q73,case_number)</f>
-        <v>1391753646.6838758</v>
+        <v>565514679.49266434</v>
       </c>
       <c r="F73" s="110" t="s">
         <v>85</v>
@@ -40115,7 +40115,7 @@
       <c r="D74" s="103"/>
       <c r="E74" s="107" cm="1">
         <f t="array" ref="E74">INDEX(N74:Q74,case_number)</f>
-        <v>187240.87089252812</v>
+        <v>137817.1148098961</v>
       </c>
       <c r="F74" s="111" t="s">
         <v>85</v>
@@ -40147,7 +40147,7 @@
       <c r="D75" s="103"/>
       <c r="E75" s="107" cm="1">
         <f t="array" ref="E75">INDEX(N75:Q75,case_number)</f>
-        <v>213725556.87489808</v>
+        <v>97725643.802408978</v>
       </c>
       <c r="F75" s="111" t="s">
         <v>85</v>
@@ -40179,15 +40179,15 @@
       <c r="D76" s="103"/>
       <c r="E76" s="146" cm="1">
         <f t="array" ref="E76">INDEX(N76:Q76,case_number)</f>
-        <v>1.3453592978805262E-4</v>
+        <v>2.4370209971124864E-4</v>
       </c>
       <c r="F76" s="146" cm="1">
         <f t="array" aca="1" ref="F76" ca="1">INDIRECT(sheet_name&amp;"!Fs_coeff.tens.2")*1000</f>
-        <v>1.3453194356000459E-4</v>
+        <v>2.4370432807676286E-4</v>
       </c>
       <c r="G76" s="118">
         <f t="shared" ref="G76:G78" ca="1" si="5">(F76-E76)/E76</f>
-        <v>-2.962946816001108E-5</v>
+        <v>9.1438092526099532E-6</v>
       </c>
       <c r="K76" s="106"/>
       <c r="L76" s="105" t="s">
@@ -40215,15 +40215,15 @@
       <c r="D77" s="103"/>
       <c r="E77" s="146" cm="1">
         <f t="array" ref="E77">INDEX(N77:Q77,case_number)</f>
-        <v>0.15356565250189275</v>
+        <v>0.17280832372040422</v>
       </c>
       <c r="F77" s="146" cm="1">
         <f t="array" aca="1" ref="F77" ca="1">INDIRECT(sheet_name&amp;"!Fs_coeff.tens.1")</f>
-        <v>0.15355954292157073</v>
+        <v>0.17280234972532127</v>
       </c>
       <c r="G77" s="118">
         <f t="shared" ca="1" si="5"/>
-        <v>-3.9784810095743922E-5</v>
+        <v>-3.4570065575189399E-5</v>
       </c>
       <c r="K77" s="106"/>
       <c r="L77" s="105" t="s">
@@ -40251,15 +40251,15 @@
       <c r="D78" s="103"/>
       <c r="E78" s="108" cm="1">
         <f t="array" ref="E78">INDEX(N78:Q78,case_number)</f>
-        <v>2892.88830676009</v>
+        <v>2893.6013508215733</v>
       </c>
       <c r="F78" s="107" cm="1">
         <f t="array" aca="1" ref="F78" ca="1">INDIRECT(sheet_name&amp;"!Fs_coeff.tens.0")/1000</f>
-        <v>2892.8876140937446</v>
+        <v>2893.6005804047468</v>
       </c>
       <c r="G78" s="118">
         <f t="shared" ca="1" si="5"/>
-        <v>-2.3943763879138282E-7</v>
+        <v>-2.6624843339515334E-7</v>
       </c>
       <c r="K78" s="106"/>
       <c r="L78" s="112" t="s">
@@ -40292,15 +40292,15 @@
       </c>
       <c r="E79" s="107" cm="1">
         <f t="array" ref="E79">INDEX(N79:Q79,case_number)</f>
-        <v>1244.3580111747735</v>
+        <v>681.32565393551567</v>
       </c>
       <c r="F79" s="107" cm="1">
         <f t="array" aca="1" ref="F79" ca="1">-INDIRECT(sheet_name&amp;"!DZ_gap")</f>
-        <v>1244.3583528535567</v>
+        <v>681.3256543935745</v>
       </c>
       <c r="G79" s="118">
         <f ca="1">(F79-E79)/E79</f>
-        <v>2.7458237906393814E-7</v>
+        <v>6.7230526026688042E-10</v>
       </c>
       <c r="I79" s="139"/>
       <c r="K79" s="106">
@@ -40519,15 +40519,15 @@
       </c>
       <c r="E84" s="111" cm="1">
         <f t="array" ref="E84">INDEX(N84:Q84,case_number)</f>
-        <v>14636.622779298261</v>
+        <v>1774.9582977160969</v>
       </c>
       <c r="F84" s="111" cm="1">
         <f t="array" aca="1" ref="F84" ca="1">INDIRECT(sheet_name&amp;"!gap.stiffness")</f>
-        <v>14636.626798256961</v>
+        <v>1774.9582989094115</v>
       </c>
       <c r="G84" s="118">
         <f ca="1">(F84-E84)/E84</f>
-        <v>2.7458237876438642E-7</v>
+        <v>6.7230569630928792E-10</v>
       </c>
       <c r="I84" s="138"/>
       <c r="K84" s="106">
@@ -40570,7 +40570,7 @@
       </c>
       <c r="E85" s="111" cm="1">
         <f t="array" ref="E85">INDEX(N85:Q85,case_number)</f>
-        <v>4797.9387029107638</v>
+        <v>594.89447044033909</v>
       </c>
       <c r="F85" s="111" t="s">
         <v>85</v>
@@ -40617,15 +40617,15 @@
       </c>
       <c r="E86" s="111" cm="1">
         <f t="array" ref="E86">INDEX(N86:Q86,case_number)</f>
-        <v>5169.2082946490964</v>
+        <v>800.4072256196913</v>
       </c>
       <c r="F86" s="111" cm="1">
         <f t="array" aca="1" ref="F86" ca="1">INDIRECT(sheet_name&amp;"!gap.k_shell")</f>
-        <v>5169.2082946490964</v>
+        <v>800.40722561969153</v>
       </c>
       <c r="G86" s="118">
         <f ca="1">(F86-E86)/E86</f>
-        <v>0</v>
+        <v>2.840724923081433E-16</v>
       </c>
       <c r="H86" t="s">
         <v>152</v>
@@ -40665,15 +40665,15 @@
       </c>
       <c r="E87" s="111" cm="1">
         <f t="array" ref="E87">INDEX(N87:Q87,case_number)</f>
-        <v>5169.2082946490964</v>
+        <v>800.4072256196913</v>
       </c>
       <c r="F87" s="111" cm="1">
         <f t="array" aca="1" ref="F87" ca="1">INDIRECT(sheet_name&amp;"!gap.k_shell")</f>
-        <v>5169.2082946490964</v>
+        <v>800.40722561969153</v>
       </c>
       <c r="G87" s="118">
         <f ca="1">(F87-E87)/E87</f>
-        <v>0</v>
+        <v>2.840724923081433E-16</v>
       </c>
       <c r="H87" t="s">
         <v>150</v>
@@ -40716,11 +40716,11 @@
       </c>
       <c r="E88" s="109" cm="1">
         <f t="array" ref="E88">INDEX(N88:Q88,case_number)</f>
-        <v>1.8</v>
+        <v>2.9062003167089676</v>
       </c>
       <c r="F88" s="109" cm="1">
         <f t="array" aca="1" ref="F88" ca="1">INDIRECT(sheet_name&amp;"!gap.k_fac")</f>
-        <v>1.8</v>
+        <v>2.9062003167089676</v>
       </c>
       <c r="G88" s="118">
         <f ca="1">(F88-E88)/E88</f>
@@ -40767,15 +40767,15 @@
       </c>
       <c r="E89" s="107" cm="1">
         <f t="array" ref="E89">INDEX(N89:Q89,case_number)</f>
-        <v>1483.8020595773849</v>
+        <v>6.3920006148981718</v>
       </c>
       <c r="F89" s="107" cm="1">
         <f t="array" aca="1" ref="F89" ca="1">INDIRECT(sheet_name&amp;"!gap.k_fl")</f>
-        <v>1483.8038863767938</v>
+        <v>6.3920011573135929</v>
       </c>
       <c r="G89" s="118">
         <f ca="1">(F89-E89)/E89</f>
-        <v>1.2311611223035349E-6</v>
+        <v>8.4858474474946531E-8</v>
       </c>
       <c r="I89" s="138"/>
       <c r="K89" s="106">
@@ -40818,7 +40818,7 @@
       </c>
       <c r="E90" s="110" cm="1">
         <f t="array" ref="E90">INDEX(N90:Q90,case_number)</f>
-        <v>549.79614201309175</v>
+        <v>579.62119250410046</v>
       </c>
       <c r="F90" s="110" t="s">
         <v>85</v>
@@ -40868,7 +40868,7 @@
       </c>
       <c r="E91" s="110" cm="1">
         <f t="array" ref="E91">INDEX(N91:Q91,case_number)</f>
-        <v>431.02794916761809</v>
+        <v>298.39439776040422</v>
       </c>
       <c r="F91" s="110" t="s">
         <v>85</v>
@@ -40967,11 +40967,11 @@
       </c>
       <c r="E93" s="107" cm="1">
         <f t="array" ref="E93">INDEX(N93:Q93,case_number)</f>
-        <v>1794.1541531878652</v>
+        <v>1260.9468464396161</v>
       </c>
       <c r="F93" s="107" cm="1">
         <f t="array" aca="1" ref="F93" ca="1">-INDIRECT(sheet_name&amp;"!DZ_gap_tot")</f>
-        <v>1244.3583528535567</v>
+        <v>681.3256543935745</v>
       </c>
       <c r="G93" s="107"/>
       <c r="I93" s="139"/>
@@ -41166,15 +41166,15 @@
       </c>
       <c r="E97" s="109" cm="1">
         <f t="array" ref="E97">INDEX(N97:Q97,case_number)</f>
-        <v>2.4286136732398829</v>
+        <v>1.1112353497098411</v>
       </c>
       <c r="F97" s="109" cm="1">
         <f t="array" aca="1" ref="F97" ca="1">INDIRECT(sheet_name&amp;"!stiffness_correction_factor")</f>
-        <v>2.4286653342946511</v>
+        <v>1.1112390055117838</v>
       </c>
       <c r="G97" s="118">
         <f ca="1">(F97-E97)/E97</f>
-        <v>2.1271829001672139E-5</v>
+        <v>3.2898538942991016E-6</v>
       </c>
       <c r="I97" s="139"/>
       <c r="K97" s="106">
@@ -41258,15 +41258,15 @@
       </c>
       <c r="E99" s="107" cm="1">
         <f t="array" ref="E99">INDEX(N99:Q99,case_number)</f>
-        <v>10245.332978022379</v>
+        <v>15956.782644600848</v>
       </c>
       <c r="F99" s="107" cm="1">
         <f t="array" aca="1" ref="F99" ca="1">INDIRECT(sheet_name&amp;"!k_seg")</f>
-        <v>10244.96531616569</v>
+        <v>15956.258245417217</v>
       </c>
       <c r="G99" s="118">
         <f ca="1">(F99-E99)/E99</f>
-        <v>-3.5885788922463456E-5</v>
+        <v>-3.2863716659570941E-5</v>
       </c>
       <c r="I99" s="138"/>
       <c r="K99" s="106">
@@ -41309,15 +41309,15 @@
       </c>
       <c r="E100" s="111" cm="1">
         <f t="array" ref="E100">INDEX(N100:Q100,case_number)</f>
-        <v>823.89401242504141</v>
+        <v>1386.9263696642993</v>
       </c>
       <c r="F100" s="111" cm="1">
         <f t="array" aca="1" ref="F100" ca="1">ROUND(INDIRECT(sheet_name&amp;"!Z_2_td"),0)</f>
-        <v>824</v>
+        <v>1387</v>
       </c>
       <c r="G100" s="118">
         <f ca="1">(F100-E100)/E100</f>
-        <v>1.2864224446373524E-4</v>
+        <v>5.3088856994296868E-5</v>
       </c>
       <c r="I100" s="138"/>
       <c r="K100" s="106">
@@ -41360,15 +41360,15 @@
       </c>
       <c r="E101" s="109" cm="1">
         <f t="array" ref="E101">INDEX(N101:Q101,case_number)</f>
-        <v>0.41430870717841117</v>
+        <v>0.44780286498460981</v>
       </c>
       <c r="F101" s="109" cm="1">
         <f t="array" aca="1" ref="F101" ca="1">INDIRECT(sheet_name&amp;"!u")</f>
-        <v>0.41432340368180404</v>
+        <v>0.44781758178683745</v>
       </c>
       <c r="G101" s="118">
         <f ca="1">(F101-E101)/E101</f>
-        <v>3.5472349816039453E-5</v>
+        <v>3.2864466439153234E-5</v>
       </c>
       <c r="H101" t="s">
         <v>303</v>
@@ -41414,7 +41414,7 @@
       </c>
       <c r="E102" s="110" cm="1">
         <f t="array" ref="E102">INDEX(N102:Q102,case_number)</f>
-        <v>0.41430870717841117</v>
+        <v>0.44780286498460981</v>
       </c>
       <c r="F102" s="104"/>
       <c r="G102" s="104"/>
@@ -41577,15 +41577,15 @@
       </c>
       <c r="E106" s="107" cm="1">
         <f t="array" ref="E106">INDEX(N106:Q106,case_number)</f>
-        <v>-1367.6496778414403</v>
+        <v>-804.6173206021823</v>
       </c>
       <c r="F106" s="107" cm="1">
         <f t="array" aca="1" ref="F106" ca="1">INDIRECT(sheet_name&amp;"!point4.Z")</f>
-        <v>-1367.6500195202234</v>
+        <v>-804.61732106024112</v>
       </c>
       <c r="G106" s="118">
         <f ca="1">(F106-E106)/E106</f>
-        <v>2.4982916945142781E-7</v>
+        <v>5.6928779603303134E-10</v>
       </c>
       <c r="I106" s="103"/>
       <c r="K106" s="106">
@@ -41628,15 +41628,15 @@
       </c>
       <c r="E107" s="113" cm="1">
         <f t="array" ref="E107">INDEX(N107:Q107,case_number)</f>
-        <v>0.12040478807649153</v>
+        <v>0.11273981784143602</v>
       </c>
       <c r="F107" s="113" cm="1">
         <f t="array" aca="1" ref="F107" ca="1">INDIRECT(sheet_name&amp;"!true_force_initial_slope")</f>
-        <v>0.12038620783873294</v>
+        <v>0.11270892416039283</v>
       </c>
       <c r="G107" s="118">
         <f ca="1">(F107-E107)/E107</f>
-        <v>-1.5431477481436177E-4</v>
+        <v>-2.740263523101379E-4</v>
       </c>
       <c r="I107" s="105"/>
       <c r="K107" s="106">
@@ -41679,15 +41679,15 @@
       </c>
       <c r="E108" s="108" cm="1">
         <f t="array" ref="E108">INDEX(N108:Q108,case_number)</f>
-        <v>2801.0866686866084</v>
+        <v>2837.5937349423066</v>
       </c>
       <c r="F108" s="108" cm="1">
         <f t="array" aca="1" ref="F108" ca="1">INDIRECT(sheet_name&amp;"!point4.Fs")</f>
-        <v>2801.0982083537542</v>
+        <v>2837.6042592452122</v>
       </c>
       <c r="G108" s="118">
         <f ca="1">(F108-E108)/E108</f>
-        <v>4.1197108518018312E-6</v>
+        <v>3.7088829088019403E-6</v>
       </c>
       <c r="I108" s="103"/>
       <c r="K108" s="106">
@@ -42073,15 +42073,15 @@
       </c>
       <c r="E117" s="113" cm="1">
         <f t="array" ref="E117">INDEX(N117:Q117,case_number)</f>
-        <v>0.49415030308522712</v>
+        <v>0.61147882833072409</v>
       </c>
       <c r="F117" s="113" cm="1">
         <f t="array" aca="1" ref="F117" ca="1">INDIRECT(sheet_name&amp;"!true_moment_initial_slope")</f>
-        <v>0.49406616497246486</v>
+        <v>0.61134783038820784</v>
       </c>
       <c r="G117" s="118">
         <f ca="1">(F117-E117)/E117</f>
-        <v>-1.7026826096622647E-4</v>
+        <v>-2.1423136247229451E-4</v>
       </c>
       <c r="H117" t="s">
         <v>303</v>
@@ -42123,7 +42123,7 @@
       </c>
       <c r="E118" s="113" cm="1">
         <f t="array" ref="E118">INDEX(N118:Q118,case_number)</f>
-        <v>0.1234684985175353</v>
+        <v>0.10262233004223215</v>
       </c>
       <c r="F118" s="109" t="s">
         <v>85</v>
@@ -42170,15 +42170,15 @@
       </c>
       <c r="E119" s="108" cm="1">
         <f t="array" ref="E119">INDEX(N119:Q119,case_number)</f>
-        <v>-322.13499207144736</v>
+        <v>-240.40239495744856</v>
       </c>
       <c r="F119" s="108" cm="1">
         <f t="array" aca="1" ref="F119" ca="1">INDIRECT(sheet_name&amp;"!point4.Ms")</f>
-        <v>-322.08126090496728</v>
+        <v>-240.35514075009525</v>
       </c>
       <c r="G119" s="118">
         <f ca="1">(F119-E119)/E119</f>
-        <v>-1.6679705031286883E-4</v>
+        <v>-1.9656296419876817E-4</v>
       </c>
       <c r="H119" t="s">
         <v>303</v>
@@ -42220,7 +42220,7 @@
       </c>
       <c r="E120" s="108" cm="1">
         <f t="array" ref="E120">INDEX(N120:Q120,case_number)</f>
-        <v>-76.819507629007845</v>
+        <v>-34.959613062205065</v>
       </c>
       <c r="F120" s="109" t="s">
         <v>85</v>
@@ -42341,7 +42341,7 @@
       </c>
       <c r="E123" s="108" cm="1">
         <f t="array" ref="E123">INDEX(N123:Q123,case_number)</f>
-        <v>-40.182316327404109</v>
+        <v>-87.818771136704058</v>
       </c>
       <c r="F123" s="109" t="s">
         <v>85</v>
@@ -42425,7 +42425,7 @@
       </c>
       <c r="E125" s="108" cm="1">
         <f t="array" ref="E125">INDEX(N125:Q125,case_number)</f>
-        <v>1.3386781456392284E-2</v>
+        <v>1.2534578790321781E-2</v>
       </c>
       <c r="F125" s="109" t="s">
         <v>85</v>
@@ -42467,7 +42467,7 @@
       </c>
       <c r="E126" s="108" cm="1">
         <f t="array" ref="E126">INDEX(N126:Q126,case_number)</f>
-        <v>-40.149725060359245</v>
+        <v>-87.747542664001102</v>
       </c>
       <c r="F126" s="109" t="s">
         <v>85</v>
@@ -42509,7 +42509,7 @@
       </c>
       <c r="E127" s="108" cm="1">
         <f t="array" ref="E127">INDEX(N127:Q127,case_number)</f>
-        <v>1.2346849851752828E-2</v>
+        <v>1.0262233004222632E-2</v>
       </c>
       <c r="F127" s="109" t="s">
         <v>85</v>
@@ -42551,7 +42551,7 @@
       </c>
       <c r="E128" s="108" cm="1">
         <f t="array" ref="E128">INDEX(N128:Q128,case_number)</f>
-        <v>-14.685047887174937</v>
+        <v>-32.094288667371821</v>
       </c>
       <c r="F128" s="109" t="s">
         <v>85</v>
@@ -42587,7 +42587,7 @@
       </c>
       <c r="E129" s="108" cm="1">
         <f t="array" ref="E129">INDEX(N129:Q129,case_number)</f>
-        <v>2925.8132343674552</v>
+        <v>3088.6803607244869</v>
       </c>
       <c r="F129" s="109" t="s">
         <v>85</v>
@@ -42623,7 +42623,7 @@
       </c>
       <c r="E130" s="108" cm="1">
         <f t="array" ref="E130">INDEX(N130:Q130,case_number)</f>
-        <v>229.08386220142413</v>
+        <v>156.61950693641407</v>
       </c>
       <c r="F130" s="109" t="s">
         <v>85</v>
@@ -42656,7 +42656,7 @@
       </c>
       <c r="E131" s="108" cm="1">
         <f t="array" ref="E131">INDEX(N131:Q131,case_number)</f>
-        <v>4.1905840717736343E-4</v>
+        <v>7.5909397505679655E-4</v>
       </c>
       <c r="F131" s="109" t="s">
         <v>85</v>
@@ -42692,7 +42692,7 @@
       </c>
       <c r="E132" s="108" cm="1">
         <f t="array" ref="E132">INDEX(N132:Q132,case_number)</f>
-        <v>0.59744121614189982</v>
+        <v>0.79858284162159954</v>
       </c>
       <c r="F132" s="109" t="s">
         <v>85</v>
@@ -42728,7 +42728,7 @@
       </c>
       <c r="E133" s="108" cm="1">
         <f t="array" ref="E133">INDEX(N133:Q133,case_number)</f>
-        <v>52.604437654353092</v>
+        <v>54.825458530511014</v>
       </c>
       <c r="F133" s="109" t="s">
         <v>85</v>
@@ -42855,7 +42855,7 @@
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G21" xr:uid="{A97D2F7B-FDA4-407E-92F3-17F2D0816A54}">
       <formula1>$N$48:$Q$48</formula1>
     </dataValidation>
@@ -43149,20 +43149,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -43185,14 +43185,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -43207,4 +43199,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>